<commit_message>
Last Update 15-09-2018 14:50:42.23
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Lab Attendance" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="63">
   <si>
     <t>S.NO</t>
   </si>
@@ -381,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -423,6 +423,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -779,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -793,61 +796,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="D3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -902,8 +905,8 @@
       <c r="AF4" s="12"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="27"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
@@ -956,8 +959,8 @@
       <c r="AF5" s="12"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="27"/>
-      <c r="B6" s="30"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="10" t="s">
         <v>50</v>
       </c>
@@ -3656,10 +3659,10 @@
       <c r="AF55" s="12"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="26"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D7:D55,"A")</f>
@@ -3779,10 +3782,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="20"/>
+      <c r="B57" s="21"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(49-D56)</f>
@@ -3920,13 +3923,2330 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AF57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
+    <col min="4" max="32" width="4.140625" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="18.75">
+      <c r="A1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="1:32" ht="19.5">
+      <c r="A2" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:32" ht="18.75">
+      <c r="A3" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:32">
+      <c r="A4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19">
+        <v>9</v>
+      </c>
+      <c r="I4" s="19">
+        <v>9</v>
+      </c>
+      <c r="J4" s="19">
+        <v>9</v>
+      </c>
+      <c r="K4" s="19">
+        <v>9</v>
+      </c>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+    </row>
+    <row r="5" spans="1:32">
+      <c r="A5" s="28"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19">
+        <v>15</v>
+      </c>
+      <c r="I5" s="19">
+        <v>15</v>
+      </c>
+      <c r="J5" s="19">
+        <v>15</v>
+      </c>
+      <c r="K5" s="19">
+        <v>15</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+    </row>
+    <row r="6" spans="1:32" ht="15" customHeight="1">
+      <c r="A6" s="28"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19">
+        <v>1</v>
+      </c>
+      <c r="I6" s="19">
+        <v>2</v>
+      </c>
+      <c r="J6" s="19">
+        <v>3</v>
+      </c>
+      <c r="K6" s="19">
+        <v>4</v>
+      </c>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="19"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="19"/>
+    </row>
+    <row r="7" spans="1:32" ht="15" customHeight="1">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="19"/>
+      <c r="AF7" s="19"/>
+    </row>
+    <row r="8" spans="1:32" ht="15" customHeight="1">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
+      <c r="AF8" s="19"/>
+    </row>
+    <row r="9" spans="1:32" ht="15" customHeight="1">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+      <c r="X9" s="19"/>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
+      <c r="AA9" s="19"/>
+      <c r="AB9" s="19"/>
+      <c r="AC9" s="19"/>
+      <c r="AD9" s="19"/>
+      <c r="AE9" s="19"/>
+      <c r="AF9" s="19"/>
+    </row>
+    <row r="10" spans="1:32" ht="15" customHeight="1">
+      <c r="A10" s="3">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="19"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="19"/>
+      <c r="AF10" s="19"/>
+    </row>
+    <row r="11" spans="1:32" ht="15" customHeight="1">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19"/>
+    </row>
+    <row r="12" spans="1:32" ht="15" customHeight="1">
+      <c r="A12" s="3">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19"/>
+    </row>
+    <row r="13" spans="1:32" ht="15" customHeight="1">
+      <c r="A13" s="3">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19"/>
+    </row>
+    <row r="14" spans="1:32" ht="15" customHeight="1">
+      <c r="A14" s="3">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+    </row>
+    <row r="15" spans="1:32" ht="15" customHeight="1">
+      <c r="A15" s="3">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
+    </row>
+    <row r="16" spans="1:32" ht="15" customHeight="1">
+      <c r="A16" s="3">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="19"/>
+      <c r="AE16" s="19"/>
+      <c r="AF16" s="19"/>
+    </row>
+    <row r="17" spans="1:32" ht="15" customHeight="1">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
+      <c r="AE17" s="19"/>
+      <c r="AF17" s="19"/>
+    </row>
+    <row r="18" spans="1:32" ht="15" customHeight="1">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19"/>
+    </row>
+    <row r="19" spans="1:32" ht="15" customHeight="1">
+      <c r="A19" s="3">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="19"/>
+    </row>
+    <row r="20" spans="1:32" ht="15" customHeight="1">
+      <c r="A20" s="3">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="19"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="19"/>
+      <c r="AE20" s="19"/>
+      <c r="AF20" s="19"/>
+    </row>
+    <row r="21" spans="1:32" ht="15" customHeight="1">
+      <c r="A21" s="3">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="19"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
+      <c r="AA21" s="19"/>
+      <c r="AB21" s="19"/>
+      <c r="AC21" s="19"/>
+      <c r="AD21" s="19"/>
+      <c r="AE21" s="19"/>
+      <c r="AF21" s="19"/>
+    </row>
+    <row r="22" spans="1:32" ht="15" customHeight="1">
+      <c r="A22" s="3">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
+      <c r="X22" s="19"/>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="19"/>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="19"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="19"/>
+      <c r="AE22" s="19"/>
+      <c r="AF22" s="19"/>
+    </row>
+    <row r="23" spans="1:32" ht="15" customHeight="1">
+      <c r="A23" s="3">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="19"/>
+      <c r="Z23" s="19"/>
+      <c r="AA23" s="19"/>
+      <c r="AB23" s="19"/>
+      <c r="AC23" s="19"/>
+      <c r="AD23" s="19"/>
+      <c r="AE23" s="19"/>
+      <c r="AF23" s="19"/>
+    </row>
+    <row r="24" spans="1:32" ht="15" customHeight="1">
+      <c r="A24" s="3">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="19"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
+    </row>
+    <row r="25" spans="1:32" ht="15" customHeight="1">
+      <c r="A25" s="3">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="19"/>
+      <c r="AD25" s="19"/>
+      <c r="AE25" s="19"/>
+      <c r="AF25" s="19"/>
+    </row>
+    <row r="26" spans="1:32" ht="15" customHeight="1">
+      <c r="A26" s="3">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="19"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="19"/>
+      <c r="Z26" s="19"/>
+      <c r="AA26" s="19"/>
+      <c r="AB26" s="19"/>
+      <c r="AC26" s="19"/>
+      <c r="AD26" s="19"/>
+      <c r="AE26" s="19"/>
+      <c r="AF26" s="19"/>
+    </row>
+    <row r="27" spans="1:32" ht="15" customHeight="1">
+      <c r="A27" s="3">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="19"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
+      <c r="AA27" s="19"/>
+      <c r="AB27" s="19"/>
+      <c r="AC27" s="19"/>
+      <c r="AD27" s="19"/>
+      <c r="AE27" s="19"/>
+      <c r="AF27" s="19"/>
+    </row>
+    <row r="28" spans="1:32" ht="15" customHeight="1">
+      <c r="A28" s="3">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="19"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="19"/>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
+      <c r="AA28" s="19"/>
+      <c r="AB28" s="19"/>
+      <c r="AC28" s="19"/>
+      <c r="AD28" s="19"/>
+      <c r="AE28" s="19"/>
+      <c r="AF28" s="19"/>
+    </row>
+    <row r="29" spans="1:32" ht="15" customHeight="1">
+      <c r="A29" s="3">
+        <v>23</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
+      <c r="AA29" s="19"/>
+      <c r="AB29" s="19"/>
+      <c r="AC29" s="19"/>
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="19"/>
+      <c r="AF29" s="19"/>
+    </row>
+    <row r="30" spans="1:32" ht="15" customHeight="1">
+      <c r="A30" s="3">
+        <v>24</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+      <c r="Y30" s="19"/>
+      <c r="Z30" s="19"/>
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="19"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="19"/>
+      <c r="AE30" s="19"/>
+      <c r="AF30" s="19"/>
+    </row>
+    <row r="31" spans="1:32" ht="15" customHeight="1">
+      <c r="A31" s="3">
+        <v>25</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="19"/>
+      <c r="Y31" s="19"/>
+      <c r="Z31" s="19"/>
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="19"/>
+      <c r="AC31" s="19"/>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="19"/>
+      <c r="AF31" s="19"/>
+    </row>
+    <row r="32" spans="1:32" ht="15" customHeight="1">
+      <c r="A32" s="3">
+        <v>26</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+      <c r="AA32" s="19"/>
+      <c r="AB32" s="19"/>
+      <c r="AC32" s="19"/>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="19"/>
+      <c r="AF32" s="19"/>
+    </row>
+    <row r="33" spans="1:32" ht="15" customHeight="1">
+      <c r="A33" s="3">
+        <v>27</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="19"/>
+      <c r="Z33" s="19"/>
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="19"/>
+      <c r="AC33" s="19"/>
+      <c r="AD33" s="19"/>
+      <c r="AE33" s="19"/>
+      <c r="AF33" s="19"/>
+    </row>
+    <row r="34" spans="1:32" ht="15" customHeight="1">
+      <c r="A34" s="3">
+        <v>28</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="19"/>
+      <c r="Z34" s="19"/>
+      <c r="AA34" s="19"/>
+      <c r="AB34" s="19"/>
+      <c r="AC34" s="19"/>
+      <c r="AD34" s="19"/>
+      <c r="AE34" s="19"/>
+      <c r="AF34" s="19"/>
+    </row>
+    <row r="35" spans="1:32" ht="15" customHeight="1">
+      <c r="A35" s="3">
+        <v>29</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="19"/>
+      <c r="Y35" s="19"/>
+      <c r="Z35" s="19"/>
+      <c r="AA35" s="19"/>
+      <c r="AB35" s="19"/>
+      <c r="AC35" s="19"/>
+      <c r="AD35" s="19"/>
+      <c r="AE35" s="19"/>
+      <c r="AF35" s="19"/>
+    </row>
+    <row r="36" spans="1:32" ht="15" customHeight="1">
+      <c r="A36" s="3">
+        <v>30</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
+      <c r="Y36" s="19"/>
+      <c r="Z36" s="19"/>
+      <c r="AA36" s="19"/>
+      <c r="AB36" s="19"/>
+      <c r="AC36" s="19"/>
+      <c r="AD36" s="19"/>
+      <c r="AE36" s="19"/>
+      <c r="AF36" s="19"/>
+    </row>
+    <row r="37" spans="1:32" ht="15" customHeight="1">
+      <c r="A37" s="3">
+        <v>31</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
+      <c r="Y37" s="19"/>
+      <c r="Z37" s="19"/>
+      <c r="AA37" s="19"/>
+      <c r="AB37" s="19"/>
+      <c r="AC37" s="19"/>
+      <c r="AD37" s="19"/>
+      <c r="AE37" s="19"/>
+      <c r="AF37" s="19"/>
+    </row>
+    <row r="38" spans="1:32" ht="15" customHeight="1">
+      <c r="A38" s="3">
+        <v>32</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19"/>
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="19"/>
+      <c r="AC38" s="19"/>
+      <c r="AD38" s="19"/>
+      <c r="AE38" s="19"/>
+      <c r="AF38" s="19"/>
+    </row>
+    <row r="39" spans="1:32" ht="15" customHeight="1">
+      <c r="A39" s="3">
+        <v>33</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+      <c r="Y39" s="19"/>
+      <c r="Z39" s="19"/>
+      <c r="AA39" s="19"/>
+      <c r="AB39" s="19"/>
+      <c r="AC39" s="19"/>
+      <c r="AD39" s="19"/>
+      <c r="AE39" s="19"/>
+      <c r="AF39" s="19"/>
+    </row>
+    <row r="40" spans="1:32" ht="15" customHeight="1">
+      <c r="A40" s="3">
+        <v>34</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
+      <c r="Y40" s="19"/>
+      <c r="Z40" s="19"/>
+      <c r="AA40" s="19"/>
+      <c r="AB40" s="19"/>
+      <c r="AC40" s="19"/>
+      <c r="AD40" s="19"/>
+      <c r="AE40" s="19"/>
+      <c r="AF40" s="19"/>
+    </row>
+    <row r="41" spans="1:32" ht="15" customHeight="1">
+      <c r="A41" s="3">
+        <v>35</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
+      <c r="U41" s="19"/>
+      <c r="V41" s="19"/>
+      <c r="W41" s="19"/>
+      <c r="X41" s="19"/>
+      <c r="Y41" s="19"/>
+      <c r="Z41" s="19"/>
+      <c r="AA41" s="19"/>
+      <c r="AB41" s="19"/>
+      <c r="AC41" s="19"/>
+      <c r="AD41" s="19"/>
+      <c r="AE41" s="19"/>
+      <c r="AF41" s="19"/>
+    </row>
+    <row r="42" spans="1:32" ht="15" customHeight="1">
+      <c r="A42" s="3">
+        <v>36</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
+      <c r="U42" s="19"/>
+      <c r="V42" s="19"/>
+      <c r="W42" s="19"/>
+      <c r="X42" s="19"/>
+      <c r="Y42" s="19"/>
+      <c r="Z42" s="19"/>
+      <c r="AA42" s="19"/>
+      <c r="AB42" s="19"/>
+      <c r="AC42" s="19"/>
+      <c r="AD42" s="19"/>
+      <c r="AE42" s="19"/>
+      <c r="AF42" s="19"/>
+    </row>
+    <row r="43" spans="1:32" ht="15" customHeight="1">
+      <c r="A43" s="3">
+        <v>37</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="4"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
+      <c r="U43" s="19"/>
+      <c r="V43" s="19"/>
+      <c r="W43" s="19"/>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="19"/>
+      <c r="AA43" s="19"/>
+      <c r="AB43" s="19"/>
+      <c r="AC43" s="19"/>
+      <c r="AD43" s="19"/>
+      <c r="AE43" s="19"/>
+      <c r="AF43" s="19"/>
+    </row>
+    <row r="44" spans="1:32" ht="15" customHeight="1">
+      <c r="A44" s="3">
+        <v>38</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
+      <c r="U44" s="19"/>
+      <c r="V44" s="19"/>
+      <c r="W44" s="19"/>
+      <c r="X44" s="19"/>
+      <c r="Y44" s="19"/>
+      <c r="Z44" s="19"/>
+      <c r="AA44" s="19"/>
+      <c r="AB44" s="19"/>
+      <c r="AC44" s="19"/>
+      <c r="AD44" s="19"/>
+      <c r="AE44" s="19"/>
+      <c r="AF44" s="19"/>
+    </row>
+    <row r="45" spans="1:32" ht="15" customHeight="1">
+      <c r="A45" s="3">
+        <v>39</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
+      <c r="U45" s="19"/>
+      <c r="V45" s="19"/>
+      <c r="W45" s="19"/>
+      <c r="X45" s="19"/>
+      <c r="Y45" s="19"/>
+      <c r="Z45" s="19"/>
+      <c r="AA45" s="19"/>
+      <c r="AB45" s="19"/>
+      <c r="AC45" s="19"/>
+      <c r="AD45" s="19"/>
+      <c r="AE45" s="19"/>
+      <c r="AF45" s="19"/>
+    </row>
+    <row r="46" spans="1:32" ht="15" customHeight="1">
+      <c r="A46" s="3">
+        <v>40</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="8"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="19"/>
+      <c r="U46" s="19"/>
+      <c r="V46" s="19"/>
+      <c r="W46" s="19"/>
+      <c r="X46" s="19"/>
+      <c r="Y46" s="19"/>
+      <c r="Z46" s="19"/>
+      <c r="AA46" s="19"/>
+      <c r="AB46" s="19"/>
+      <c r="AC46" s="19"/>
+      <c r="AD46" s="19"/>
+      <c r="AE46" s="19"/>
+      <c r="AF46" s="19"/>
+    </row>
+    <row r="47" spans="1:32" ht="15" customHeight="1">
+      <c r="A47" s="3">
+        <v>41</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="19"/>
+      <c r="U47" s="19"/>
+      <c r="V47" s="19"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="19"/>
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="19"/>
+      <c r="AA47" s="19"/>
+      <c r="AB47" s="19"/>
+      <c r="AC47" s="19"/>
+      <c r="AD47" s="19"/>
+      <c r="AE47" s="19"/>
+      <c r="AF47" s="19"/>
+    </row>
+    <row r="48" spans="1:32" ht="15" customHeight="1">
+      <c r="A48" s="3">
+        <v>42</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="19"/>
+      <c r="S48" s="19"/>
+      <c r="T48" s="19"/>
+      <c r="U48" s="19"/>
+      <c r="V48" s="19"/>
+      <c r="W48" s="19"/>
+      <c r="X48" s="19"/>
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="19"/>
+      <c r="AA48" s="19"/>
+      <c r="AB48" s="19"/>
+      <c r="AC48" s="19"/>
+      <c r="AD48" s="19"/>
+      <c r="AE48" s="19"/>
+      <c r="AF48" s="19"/>
+    </row>
+    <row r="49" spans="1:32" ht="15" customHeight="1">
+      <c r="A49" s="3">
+        <v>43</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+      <c r="O49" s="19"/>
+      <c r="P49" s="19"/>
+      <c r="Q49" s="19"/>
+      <c r="R49" s="19"/>
+      <c r="S49" s="19"/>
+      <c r="T49" s="19"/>
+      <c r="U49" s="19"/>
+      <c r="V49" s="19"/>
+      <c r="W49" s="19"/>
+      <c r="X49" s="19"/>
+      <c r="Y49" s="19"/>
+      <c r="Z49" s="19"/>
+      <c r="AA49" s="19"/>
+      <c r="AB49" s="19"/>
+      <c r="AC49" s="19"/>
+      <c r="AD49" s="19"/>
+      <c r="AE49" s="19"/>
+      <c r="AF49" s="19"/>
+    </row>
+    <row r="50" spans="1:32" ht="15" customHeight="1">
+      <c r="A50" s="3">
+        <v>44</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
+      <c r="W50" s="19"/>
+      <c r="X50" s="19"/>
+      <c r="Y50" s="19"/>
+      <c r="Z50" s="19"/>
+      <c r="AA50" s="19"/>
+      <c r="AB50" s="19"/>
+      <c r="AC50" s="19"/>
+      <c r="AD50" s="19"/>
+      <c r="AE50" s="19"/>
+      <c r="AF50" s="19"/>
+    </row>
+    <row r="51" spans="1:32" ht="15" customHeight="1">
+      <c r="A51" s="3">
+        <v>45</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+      <c r="O51" s="19"/>
+      <c r="P51" s="19"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="19"/>
+      <c r="S51" s="19"/>
+      <c r="T51" s="19"/>
+      <c r="U51" s="19"/>
+      <c r="V51" s="19"/>
+      <c r="W51" s="19"/>
+      <c r="X51" s="19"/>
+      <c r="Y51" s="19"/>
+      <c r="Z51" s="19"/>
+      <c r="AA51" s="19"/>
+      <c r="AB51" s="19"/>
+      <c r="AC51" s="19"/>
+      <c r="AD51" s="19"/>
+      <c r="AE51" s="19"/>
+      <c r="AF51" s="19"/>
+    </row>
+    <row r="52" spans="1:32" ht="15" customHeight="1">
+      <c r="A52" s="3">
+        <v>46</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+      <c r="O52" s="19"/>
+      <c r="P52" s="19"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="19"/>
+      <c r="S52" s="19"/>
+      <c r="T52" s="19"/>
+      <c r="U52" s="19"/>
+      <c r="V52" s="19"/>
+      <c r="W52" s="19"/>
+      <c r="X52" s="19"/>
+      <c r="Y52" s="19"/>
+      <c r="Z52" s="19"/>
+      <c r="AA52" s="19"/>
+      <c r="AB52" s="19"/>
+      <c r="AC52" s="19"/>
+      <c r="AD52" s="19"/>
+      <c r="AE52" s="19"/>
+      <c r="AF52" s="19"/>
+    </row>
+    <row r="53" spans="1:32" ht="15" customHeight="1">
+      <c r="A53" s="3">
+        <v>47</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
+      <c r="N53" s="19"/>
+      <c r="O53" s="19"/>
+      <c r="P53" s="19"/>
+      <c r="Q53" s="19"/>
+      <c r="R53" s="19"/>
+      <c r="S53" s="19"/>
+      <c r="T53" s="19"/>
+      <c r="U53" s="19"/>
+      <c r="V53" s="19"/>
+      <c r="W53" s="19"/>
+      <c r="X53" s="19"/>
+      <c r="Y53" s="19"/>
+      <c r="Z53" s="19"/>
+      <c r="AA53" s="19"/>
+      <c r="AB53" s="19"/>
+      <c r="AC53" s="19"/>
+      <c r="AD53" s="19"/>
+      <c r="AE53" s="19"/>
+      <c r="AF53" s="19"/>
+    </row>
+    <row r="54" spans="1:32" ht="15" customHeight="1">
+      <c r="A54" s="3">
+        <v>48</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
+      <c r="O54" s="19"/>
+      <c r="P54" s="19"/>
+      <c r="Q54" s="19"/>
+      <c r="R54" s="19"/>
+      <c r="S54" s="19"/>
+      <c r="T54" s="19"/>
+      <c r="U54" s="19"/>
+      <c r="V54" s="19"/>
+      <c r="W54" s="19"/>
+      <c r="X54" s="19"/>
+      <c r="Y54" s="19"/>
+      <c r="Z54" s="19"/>
+      <c r="AA54" s="19"/>
+      <c r="AB54" s="19"/>
+      <c r="AC54" s="19"/>
+      <c r="AD54" s="19"/>
+      <c r="AE54" s="19"/>
+      <c r="AF54" s="19"/>
+    </row>
+    <row r="55" spans="1:32" ht="15" customHeight="1">
+      <c r="A55" s="3">
+        <v>49</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
+      <c r="O55" s="19"/>
+      <c r="P55" s="19"/>
+      <c r="Q55" s="19"/>
+      <c r="R55" s="19"/>
+      <c r="S55" s="19"/>
+      <c r="T55" s="19"/>
+      <c r="U55" s="19"/>
+      <c r="V55" s="19"/>
+      <c r="W55" s="19"/>
+      <c r="X55" s="19"/>
+      <c r="Y55" s="19"/>
+      <c r="Z55" s="19"/>
+      <c r="AA55" s="19"/>
+      <c r="AB55" s="19"/>
+      <c r="AC55" s="19"/>
+      <c r="AD55" s="19"/>
+      <c r="AE55" s="19"/>
+      <c r="AF55" s="19"/>
+    </row>
+    <row r="56" spans="1:32">
+      <c r="A56" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="27"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="19">
+        <f>COUNTIF(D7:D55,"A")</f>
+        <v>0</v>
+      </c>
+      <c r="E56" s="19">
+        <f t="shared" ref="E56:AF56" si="0">COUNTIF(E7:E55,"A")</f>
+        <v>0</v>
+      </c>
+      <c r="F56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF56" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32">
+      <c r="A57" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="21"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="19">
+        <f>(49-D56)</f>
+        <v>49</v>
+      </c>
+      <c r="E57" s="19">
+        <f t="shared" ref="E57:AF57" si="1">(49-E56)</f>
+        <v>49</v>
+      </c>
+      <c r="F57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="G57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="H57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="K57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="L57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="M57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="N57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="O57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="P57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="Q57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="R57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="S57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="T57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="U57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="V57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="W57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="X57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="Y57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="Z57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="AA57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="AB57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="AC57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="AD57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="AE57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="AF57" s="19">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3940,4 +6260,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last Update 17-09-2018 14:02:18.62
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="63">
   <si>
     <t>S.NO</t>
   </si>
@@ -381,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -423,6 +423,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="N56" sqref="N56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -796,61 +802,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -883,8 +889,12 @@
       <c r="L4" s="12">
         <v>9</v>
       </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
+      <c r="M4" s="12">
+        <v>9</v>
+      </c>
+      <c r="N4" s="12">
+        <v>9</v>
+      </c>
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
@@ -905,8 +915,8 @@
       <c r="AF4" s="12"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="28"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
@@ -937,8 +947,12 @@
       <c r="L5" s="12">
         <v>14</v>
       </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="M5" s="12">
+        <v>15</v>
+      </c>
+      <c r="N5" s="12">
+        <v>17</v>
+      </c>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
@@ -959,8 +973,8 @@
       <c r="AF5" s="12"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="10" t="s">
         <v>50</v>
       </c>
@@ -991,8 +1005,12 @@
       <c r="L6" s="12">
         <v>4</v>
       </c>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
+      <c r="M6" s="12">
+        <v>7</v>
+      </c>
+      <c r="N6" s="12">
+        <v>5</v>
+      </c>
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
@@ -1045,8 +1063,12 @@
         <v>55</v>
       </c>
       <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
+      <c r="M7" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
@@ -1099,8 +1121,12 @@
         <v>55</v>
       </c>
       <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
+      <c r="M8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
@@ -1153,8 +1179,12 @@
         <v>57</v>
       </c>
       <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
+      <c r="M9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
@@ -1207,8 +1237,12 @@
         <v>55</v>
       </c>
       <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="M10" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
@@ -1261,8 +1295,12 @@
         <v>55</v>
       </c>
       <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="M11" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
@@ -1315,8 +1353,12 @@
         <v>55</v>
       </c>
       <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="M12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
@@ -1369,8 +1411,12 @@
         <v>55</v>
       </c>
       <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="M13" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
@@ -1423,8 +1469,12 @@
         <v>55</v>
       </c>
       <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="M14" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
@@ -1477,8 +1527,12 @@
         <v>55</v>
       </c>
       <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
+      <c r="M15" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
@@ -1531,8 +1585,12 @@
         <v>55</v>
       </c>
       <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="M16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
@@ -1585,8 +1643,12 @@
         <v>55</v>
       </c>
       <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="M17" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
@@ -1639,8 +1701,12 @@
         <v>55</v>
       </c>
       <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
+      <c r="M18" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
@@ -1693,8 +1759,12 @@
         <v>55</v>
       </c>
       <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="M19" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
@@ -1747,8 +1817,12 @@
         <v>55</v>
       </c>
       <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
+      <c r="M20" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
@@ -1801,8 +1875,12 @@
         <v>55</v>
       </c>
       <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
+      <c r="M21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N21" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="12"/>
@@ -1855,8 +1933,12 @@
         <v>55</v>
       </c>
       <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
+      <c r="M22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N22" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
@@ -1909,8 +1991,12 @@
         <v>55</v>
       </c>
       <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
+      <c r="M23" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
@@ -1963,8 +2049,12 @@
         <v>55</v>
       </c>
       <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
+      <c r="M24" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
@@ -2017,8 +2107,12 @@
         <v>55</v>
       </c>
       <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
+      <c r="M25" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N25" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
@@ -2071,8 +2165,12 @@
         <v>55</v>
       </c>
       <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
+      <c r="M26" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
@@ -2125,8 +2223,12 @@
         <v>55</v>
       </c>
       <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
+      <c r="M27" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
@@ -2179,8 +2281,12 @@
         <v>55</v>
       </c>
       <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
+      <c r="M28" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N28" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
@@ -2233,8 +2339,12 @@
         <v>55</v>
       </c>
       <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
+      <c r="M29" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N29" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
@@ -2287,8 +2397,12 @@
         <v>57</v>
       </c>
       <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
+      <c r="M30" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
       <c r="Q30" s="12"/>
@@ -2341,8 +2455,12 @@
         <v>55</v>
       </c>
       <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
+      <c r="M31" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N31" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
@@ -2395,8 +2513,12 @@
         <v>55</v>
       </c>
       <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
+      <c r="M32" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N32" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
@@ -2449,8 +2571,12 @@
         <v>55</v>
       </c>
       <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
+      <c r="M33" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N33" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O33" s="12"/>
       <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
@@ -2503,8 +2629,12 @@
         <v>55</v>
       </c>
       <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
+      <c r="M34" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N34" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O34" s="12"/>
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
@@ -2557,8 +2687,12 @@
         <v>55</v>
       </c>
       <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
+      <c r="M35" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N35" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O35" s="12"/>
       <c r="P35" s="12"/>
       <c r="Q35" s="12"/>
@@ -2611,8 +2745,12 @@
         <v>55</v>
       </c>
       <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
+      <c r="M36" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N36" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O36" s="12"/>
       <c r="P36" s="12"/>
       <c r="Q36" s="12"/>
@@ -2665,8 +2803,12 @@
         <v>55</v>
       </c>
       <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
+      <c r="M37" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N37" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
       <c r="Q37" s="12"/>
@@ -2719,8 +2861,12 @@
         <v>55</v>
       </c>
       <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
+      <c r="M38" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N38" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
@@ -2773,8 +2919,12 @@
         <v>55</v>
       </c>
       <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
+      <c r="M39" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N39" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="12"/>
@@ -2827,8 +2977,12 @@
         <v>55</v>
       </c>
       <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
+      <c r="M40" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N40" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O40" s="12"/>
       <c r="P40" s="12"/>
       <c r="Q40" s="12"/>
@@ -2881,8 +3035,12 @@
         <v>55</v>
       </c>
       <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
+      <c r="M41" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N41" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O41" s="12"/>
       <c r="P41" s="12"/>
       <c r="Q41" s="12"/>
@@ -2935,8 +3093,12 @@
         <v>55</v>
       </c>
       <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
+      <c r="M42" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N42" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O42" s="12"/>
       <c r="P42" s="12"/>
       <c r="Q42" s="12"/>
@@ -2989,8 +3151,12 @@
         <v>55</v>
       </c>
       <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
+      <c r="M43" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N43" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O43" s="12"/>
       <c r="P43" s="12"/>
       <c r="Q43" s="12"/>
@@ -3043,8 +3209,12 @@
         <v>55</v>
       </c>
       <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
+      <c r="M44" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N44" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="12"/>
@@ -3097,8 +3267,12 @@
         <v>55</v>
       </c>
       <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
+      <c r="M45" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="N45" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O45" s="12"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="12"/>
@@ -3151,8 +3325,12 @@
         <v>55</v>
       </c>
       <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
+      <c r="M46" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N46" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O46" s="12"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="12"/>
@@ -3205,8 +3383,12 @@
         <v>55</v>
       </c>
       <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
+      <c r="M47" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N47" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O47" s="12"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="12"/>
@@ -3259,8 +3441,12 @@
         <v>55</v>
       </c>
       <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
+      <c r="M48" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N48" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O48" s="12"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="12"/>
@@ -3313,8 +3499,12 @@
         <v>55</v>
       </c>
       <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
+      <c r="M49" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N49" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O49" s="12"/>
       <c r="P49" s="12"/>
       <c r="Q49" s="12"/>
@@ -3367,8 +3557,12 @@
         <v>55</v>
       </c>
       <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
+      <c r="M50" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N50" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O50" s="12"/>
       <c r="P50" s="12"/>
       <c r="Q50" s="12"/>
@@ -3421,8 +3615,12 @@
         <v>55</v>
       </c>
       <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
+      <c r="M51" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N51" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O51" s="12"/>
       <c r="P51" s="12"/>
       <c r="Q51" s="12"/>
@@ -3475,8 +3673,12 @@
         <v>55</v>
       </c>
       <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
+      <c r="M52" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N52" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O52" s="12"/>
       <c r="P52" s="12"/>
       <c r="Q52" s="12"/>
@@ -3529,8 +3731,12 @@
         <v>55</v>
       </c>
       <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
+      <c r="M53" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N53" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O53" s="12"/>
       <c r="P53" s="12"/>
       <c r="Q53" s="12"/>
@@ -3583,8 +3789,12 @@
         <v>55</v>
       </c>
       <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
+      <c r="M54" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N54" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O54" s="12"/>
       <c r="P54" s="12"/>
       <c r="Q54" s="12"/>
@@ -3637,8 +3847,12 @@
         <v>55</v>
       </c>
       <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
+      <c r="M55" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N55" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="O55" s="12"/>
       <c r="P55" s="12"/>
       <c r="Q55" s="12"/>
@@ -3659,10 +3873,10 @@
       <c r="AF55" s="12"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="27"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D7:D55,"A")</f>
@@ -3702,11 +3916,11 @@
       </c>
       <c r="M56" s="12">
         <f t="shared" ref="M56" si="7">COUNTIF(M7:M55,"A")</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N56" s="12">
         <f t="shared" ref="N56" si="8">COUNTIF(N7:N55,"A")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O56" s="12">
         <f t="shared" ref="O56" si="9">COUNTIF(O7:O55,"A")</f>
@@ -3782,10 +3996,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="21"/>
+      <c r="B57" s="23"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(49-D56)</f>
@@ -3825,11 +4039,11 @@
       </c>
       <c r="M57" s="12">
         <f t="shared" ref="M57" si="34">(49-M56)</f>
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="N57" s="12">
         <f t="shared" ref="N57" si="35">(49-N56)</f>
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O57" s="12">
         <f t="shared" ref="O57" si="36">(49-O56)</f>
@@ -3925,8 +4139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3939,61 +4153,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="19" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -4038,8 +4252,8 @@
       <c r="AF4" s="19"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="28"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
@@ -4082,8 +4296,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="10" t="s">
         <v>50</v>
       </c>
@@ -5988,10 +6202,10 @@
       <c r="AF55" s="19"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="27"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>COUNTIF(D7:D55,"A")</f>
@@ -6111,10 +6325,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="21"/>
+      <c r="B57" s="23"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>(49-D56)</f>

</xml_diff>

<commit_message>
Last Update 18-09-2018 13:56:15.14
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="63">
   <si>
     <t>S.NO</t>
   </si>
@@ -381,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -423,6 +423,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -789,7 +792,7 @@
   <dimension ref="A1:AF57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="N56" sqref="N56"/>
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -802,61 +805,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -895,7 +898,9 @@
       <c r="N4" s="12">
         <v>9</v>
       </c>
-      <c r="O4" s="12"/>
+      <c r="O4" s="12">
+        <v>9</v>
+      </c>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
@@ -915,8 +920,8 @@
       <c r="AF4" s="12"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="30"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
@@ -953,7 +958,9 @@
       <c r="N5" s="12">
         <v>17</v>
       </c>
-      <c r="O5" s="12"/>
+      <c r="O5" s="12">
+        <v>18</v>
+      </c>
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
@@ -973,8 +980,8 @@
       <c r="AF5" s="12"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10" t="s">
         <v>50</v>
       </c>
@@ -1011,7 +1018,9 @@
       <c r="N6" s="12">
         <v>5</v>
       </c>
-      <c r="O6" s="12"/>
+      <c r="O6" s="12">
+        <v>5</v>
+      </c>
       <c r="P6" s="12"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
@@ -1069,7 +1078,9 @@
       <c r="N7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O7" s="12"/>
+      <c r="O7" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
@@ -1127,7 +1138,9 @@
       <c r="N8" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O8" s="12"/>
+      <c r="O8" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
@@ -1185,7 +1198,9 @@
       <c r="N9" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O9" s="12"/>
+      <c r="O9" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P9" s="12"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
@@ -1243,7 +1258,9 @@
       <c r="N10" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O10" s="12"/>
+      <c r="O10" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
@@ -1301,7 +1318,9 @@
       <c r="N11" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O11" s="12"/>
+      <c r="O11" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
       <c r="R11" s="12"/>
@@ -1359,7 +1378,9 @@
       <c r="N12" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O12" s="12"/>
+      <c r="O12" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
@@ -1417,7 +1438,9 @@
       <c r="N13" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O13" s="12"/>
+      <c r="O13" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
@@ -1475,7 +1498,9 @@
       <c r="N14" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O14" s="12"/>
+      <c r="O14" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
@@ -1533,7 +1558,9 @@
       <c r="N15" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="O15" s="12"/>
+      <c r="O15" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
@@ -1591,7 +1618,9 @@
       <c r="N16" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O16" s="12"/>
+      <c r="O16" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
@@ -1649,7 +1678,9 @@
       <c r="N17" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="12"/>
+      <c r="O17" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
       <c r="R17" s="12"/>
@@ -1707,7 +1738,9 @@
       <c r="N18" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="12"/>
+      <c r="O18" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
       <c r="R18" s="12"/>
@@ -1765,7 +1798,9 @@
       <c r="N19" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O19" s="12"/>
+      <c r="O19" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
       <c r="R19" s="12"/>
@@ -1823,7 +1858,9 @@
       <c r="N20" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O20" s="12"/>
+      <c r="O20" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
       <c r="R20" s="12"/>
@@ -1881,7 +1918,9 @@
       <c r="N21" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O21" s="12"/>
+      <c r="O21" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P21" s="12"/>
       <c r="Q21" s="12"/>
       <c r="R21" s="12"/>
@@ -1939,7 +1978,9 @@
       <c r="N22" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O22" s="12"/>
+      <c r="O22" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
       <c r="R22" s="12"/>
@@ -1997,7 +2038,9 @@
       <c r="N23" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="O23" s="12"/>
+      <c r="O23" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
       <c r="R23" s="12"/>
@@ -2055,7 +2098,9 @@
       <c r="N24" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O24" s="12"/>
+      <c r="O24" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
       <c r="R24" s="12"/>
@@ -2113,7 +2158,9 @@
       <c r="N25" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O25" s="12"/>
+      <c r="O25" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
       <c r="R25" s="12"/>
@@ -2171,7 +2218,9 @@
       <c r="N26" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O26" s="12"/>
+      <c r="O26" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
       <c r="R26" s="12"/>
@@ -2229,7 +2278,9 @@
       <c r="N27" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O27" s="12"/>
+      <c r="O27" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
@@ -2287,7 +2338,9 @@
       <c r="N28" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O28" s="12"/>
+      <c r="O28" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P28" s="12"/>
       <c r="Q28" s="12"/>
       <c r="R28" s="12"/>
@@ -2345,7 +2398,9 @@
       <c r="N29" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O29" s="12"/>
+      <c r="O29" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P29" s="12"/>
       <c r="Q29" s="12"/>
       <c r="R29" s="12"/>
@@ -2403,7 +2458,9 @@
       <c r="N30" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="O30" s="12"/>
+      <c r="O30" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="P30" s="12"/>
       <c r="Q30" s="12"/>
       <c r="R30" s="12"/>
@@ -2461,7 +2518,9 @@
       <c r="N31" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O31" s="12"/>
+      <c r="O31" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
       <c r="R31" s="12"/>
@@ -2519,7 +2578,9 @@
       <c r="N32" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O32" s="12"/>
+      <c r="O32" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
       <c r="R32" s="12"/>
@@ -2577,7 +2638,9 @@
       <c r="N33" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O33" s="12"/>
+      <c r="O33" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
@@ -2635,7 +2698,9 @@
       <c r="N34" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O34" s="12"/>
+      <c r="O34" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
       <c r="R34" s="12"/>
@@ -2693,7 +2758,9 @@
       <c r="N35" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O35" s="12"/>
+      <c r="O35" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P35" s="12"/>
       <c r="Q35" s="12"/>
       <c r="R35" s="12"/>
@@ -2751,7 +2818,9 @@
       <c r="N36" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O36" s="12"/>
+      <c r="O36" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P36" s="12"/>
       <c r="Q36" s="12"/>
       <c r="R36" s="12"/>
@@ -2809,7 +2878,9 @@
       <c r="N37" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O37" s="12"/>
+      <c r="O37" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P37" s="12"/>
       <c r="Q37" s="12"/>
       <c r="R37" s="12"/>
@@ -2867,7 +2938,9 @@
       <c r="N38" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O38" s="12"/>
+      <c r="O38" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
       <c r="R38" s="12"/>
@@ -2925,7 +2998,9 @@
       <c r="N39" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O39" s="12"/>
+      <c r="O39" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P39" s="12"/>
       <c r="Q39" s="12"/>
       <c r="R39" s="12"/>
@@ -2983,7 +3058,9 @@
       <c r="N40" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O40" s="12"/>
+      <c r="O40" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P40" s="12"/>
       <c r="Q40" s="12"/>
       <c r="R40" s="12"/>
@@ -3041,7 +3118,9 @@
       <c r="N41" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O41" s="12"/>
+      <c r="O41" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P41" s="12"/>
       <c r="Q41" s="12"/>
       <c r="R41" s="12"/>
@@ -3099,7 +3178,9 @@
       <c r="N42" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O42" s="12"/>
+      <c r="O42" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P42" s="12"/>
       <c r="Q42" s="12"/>
       <c r="R42" s="12"/>
@@ -3157,7 +3238,9 @@
       <c r="N43" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O43" s="12"/>
+      <c r="O43" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P43" s="12"/>
       <c r="Q43" s="12"/>
       <c r="R43" s="12"/>
@@ -3215,7 +3298,9 @@
       <c r="N44" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O44" s="12"/>
+      <c r="O44" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P44" s="12"/>
       <c r="Q44" s="12"/>
       <c r="R44" s="12"/>
@@ -3273,7 +3358,9 @@
       <c r="N45" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O45" s="12"/>
+      <c r="O45" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P45" s="12"/>
       <c r="Q45" s="12"/>
       <c r="R45" s="12"/>
@@ -3331,7 +3418,9 @@
       <c r="N46" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O46" s="12"/>
+      <c r="O46" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P46" s="12"/>
       <c r="Q46" s="12"/>
       <c r="R46" s="12"/>
@@ -3389,7 +3478,9 @@
       <c r="N47" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O47" s="12"/>
+      <c r="O47" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P47" s="12"/>
       <c r="Q47" s="12"/>
       <c r="R47" s="12"/>
@@ -3447,7 +3538,9 @@
       <c r="N48" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O48" s="12"/>
+      <c r="O48" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P48" s="12"/>
       <c r="Q48" s="12"/>
       <c r="R48" s="12"/>
@@ -3505,7 +3598,9 @@
       <c r="N49" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O49" s="12"/>
+      <c r="O49" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P49" s="12"/>
       <c r="Q49" s="12"/>
       <c r="R49" s="12"/>
@@ -3563,7 +3658,9 @@
       <c r="N50" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O50" s="12"/>
+      <c r="O50" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P50" s="12"/>
       <c r="Q50" s="12"/>
       <c r="R50" s="12"/>
@@ -3621,7 +3718,9 @@
       <c r="N51" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O51" s="12"/>
+      <c r="O51" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P51" s="12"/>
       <c r="Q51" s="12"/>
       <c r="R51" s="12"/>
@@ -3679,7 +3778,9 @@
       <c r="N52" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O52" s="12"/>
+      <c r="O52" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P52" s="12"/>
       <c r="Q52" s="12"/>
       <c r="R52" s="12"/>
@@ -3737,7 +3838,9 @@
       <c r="N53" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O53" s="12"/>
+      <c r="O53" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P53" s="12"/>
       <c r="Q53" s="12"/>
       <c r="R53" s="12"/>
@@ -3795,7 +3898,9 @@
       <c r="N54" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O54" s="12"/>
+      <c r="O54" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P54" s="12"/>
       <c r="Q54" s="12"/>
       <c r="R54" s="12"/>
@@ -3853,7 +3958,9 @@
       <c r="N55" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="O55" s="12"/>
+      <c r="O55" s="22" t="s">
+        <v>55</v>
+      </c>
       <c r="P55" s="12"/>
       <c r="Q55" s="12"/>
       <c r="R55" s="12"/>
@@ -3873,10 +3980,10 @@
       <c r="AF55" s="12"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D7:D55,"A")</f>
@@ -3924,7 +4031,7 @@
       </c>
       <c r="O56" s="12">
         <f t="shared" ref="O56" si="9">COUNTIF(O7:O55,"A")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P56" s="12">
         <f t="shared" ref="P56" si="10">COUNTIF(P7:P55,"A")</f>
@@ -3996,10 +4103,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="23"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(49-D56)</f>
@@ -4047,7 +4154,7 @@
       </c>
       <c r="O57" s="12">
         <f t="shared" ref="O57" si="36">(49-O56)</f>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P57" s="12">
         <f t="shared" ref="P57" si="37">(49-P56)</f>
@@ -4153,61 +4260,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="19" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="32" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -4252,8 +4359,8 @@
       <c r="AF4" s="19"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="30"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
@@ -4296,8 +4403,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10" t="s">
         <v>50</v>
       </c>
@@ -6202,10 +6309,10 @@
       <c r="AF55" s="19"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>COUNTIF(D7:D55,"A")</f>
@@ -6325,10 +6432,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="23"/>
+      <c r="B57" s="24"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>(49-D56)</f>

</xml_diff>

<commit_message>
Last Update 18-09-2018 15:49:40.85
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="63">
   <si>
     <t>S.NO</t>
   </si>
@@ -381,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -423,6 +423,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -805,61 +808,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -901,7 +904,9 @@
       <c r="O4" s="12">
         <v>9</v>
       </c>
-      <c r="P4" s="12"/>
+      <c r="P4" s="23">
+        <v>9</v>
+      </c>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
@@ -920,8 +925,8 @@
       <c r="AF4" s="12"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="31"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
@@ -961,7 +966,9 @@
       <c r="O5" s="12">
         <v>18</v>
       </c>
-      <c r="P5" s="12"/>
+      <c r="P5" s="23">
+        <v>18</v>
+      </c>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
@@ -980,8 +987,8 @@
       <c r="AF5" s="12"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="31"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="10" t="s">
         <v>50</v>
       </c>
@@ -1021,7 +1028,9 @@
       <c r="O6" s="12">
         <v>5</v>
       </c>
-      <c r="P6" s="12"/>
+      <c r="P6" s="23">
+        <v>7</v>
+      </c>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
       <c r="S6" s="12"/>
@@ -1081,7 +1090,9 @@
       <c r="O7" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P7" s="12"/>
+      <c r="P7" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
@@ -1141,7 +1152,9 @@
       <c r="O8" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P8" s="12"/>
+      <c r="P8" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
@@ -1201,7 +1214,9 @@
       <c r="O9" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P9" s="12"/>
+      <c r="P9" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
@@ -1261,7 +1276,9 @@
       <c r="O10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P10" s="12"/>
+      <c r="P10" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
       <c r="S10" s="12"/>
@@ -1321,7 +1338,9 @@
       <c r="O11" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P11" s="12"/>
+      <c r="P11" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q11" s="12"/>
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
@@ -1381,7 +1400,9 @@
       <c r="O12" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P12" s="12"/>
+      <c r="P12" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q12" s="12"/>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
@@ -1441,7 +1462,9 @@
       <c r="O13" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P13" s="12"/>
+      <c r="P13" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
@@ -1501,7 +1524,9 @@
       <c r="O14" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P14" s="12"/>
+      <c r="P14" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
@@ -1561,7 +1586,9 @@
       <c r="O15" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P15" s="12"/>
+      <c r="P15" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
@@ -1621,7 +1648,9 @@
       <c r="O16" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P16" s="12"/>
+      <c r="P16" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
@@ -1681,7 +1710,9 @@
       <c r="O17" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P17" s="12"/>
+      <c r="P17" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q17" s="12"/>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
@@ -1741,7 +1772,9 @@
       <c r="O18" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P18" s="12"/>
+      <c r="P18" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q18" s="12"/>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
@@ -1801,7 +1834,9 @@
       <c r="O19" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P19" s="12"/>
+      <c r="P19" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q19" s="12"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
@@ -1861,7 +1896,9 @@
       <c r="O20" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P20" s="12"/>
+      <c r="P20" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q20" s="12"/>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
@@ -1921,7 +1958,9 @@
       <c r="O21" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P21" s="12"/>
+      <c r="P21" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q21" s="12"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
@@ -1981,7 +2020,9 @@
       <c r="O22" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P22" s="12"/>
+      <c r="P22" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q22" s="12"/>
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
@@ -2041,7 +2082,9 @@
       <c r="O23" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P23" s="12"/>
+      <c r="P23" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q23" s="12"/>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
@@ -2101,7 +2144,9 @@
       <c r="O24" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P24" s="12"/>
+      <c r="P24" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q24" s="12"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
@@ -2161,7 +2206,9 @@
       <c r="O25" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P25" s="12"/>
+      <c r="P25" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q25" s="12"/>
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
@@ -2221,7 +2268,9 @@
       <c r="O26" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P26" s="12"/>
+      <c r="P26" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q26" s="12"/>
       <c r="R26" s="12"/>
       <c r="S26" s="12"/>
@@ -2281,7 +2330,9 @@
       <c r="O27" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P27" s="12"/>
+      <c r="P27" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
       <c r="S27" s="12"/>
@@ -2341,7 +2392,9 @@
       <c r="O28" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P28" s="12"/>
+      <c r="P28" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q28" s="12"/>
       <c r="R28" s="12"/>
       <c r="S28" s="12"/>
@@ -2401,7 +2454,9 @@
       <c r="O29" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P29" s="12"/>
+      <c r="P29" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q29" s="12"/>
       <c r="R29" s="12"/>
       <c r="S29" s="12"/>
@@ -2461,7 +2516,9 @@
       <c r="O30" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="P30" s="12"/>
+      <c r="P30" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="Q30" s="12"/>
       <c r="R30" s="12"/>
       <c r="S30" s="12"/>
@@ -2521,7 +2578,9 @@
       <c r="O31" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P31" s="12"/>
+      <c r="P31" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q31" s="12"/>
       <c r="R31" s="12"/>
       <c r="S31" s="12"/>
@@ -2581,7 +2640,9 @@
       <c r="O32" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P32" s="12"/>
+      <c r="P32" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q32" s="12"/>
       <c r="R32" s="12"/>
       <c r="S32" s="12"/>
@@ -2641,7 +2702,9 @@
       <c r="O33" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P33" s="12"/>
+      <c r="P33" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
       <c r="S33" s="12"/>
@@ -2701,7 +2764,9 @@
       <c r="O34" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="P34" s="12"/>
+      <c r="P34" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="Q34" s="12"/>
       <c r="R34" s="12"/>
       <c r="S34" s="12"/>
@@ -2761,7 +2826,9 @@
       <c r="O35" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P35" s="12"/>
+      <c r="P35" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q35" s="12"/>
       <c r="R35" s="12"/>
       <c r="S35" s="12"/>
@@ -2821,7 +2888,9 @@
       <c r="O36" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P36" s="12"/>
+      <c r="P36" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q36" s="12"/>
       <c r="R36" s="12"/>
       <c r="S36" s="12"/>
@@ -2881,7 +2950,9 @@
       <c r="O37" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P37" s="12"/>
+      <c r="P37" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q37" s="12"/>
       <c r="R37" s="12"/>
       <c r="S37" s="12"/>
@@ -2941,7 +3012,9 @@
       <c r="O38" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P38" s="12"/>
+      <c r="P38" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q38" s="12"/>
       <c r="R38" s="12"/>
       <c r="S38" s="12"/>
@@ -3001,7 +3074,9 @@
       <c r="O39" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P39" s="12"/>
+      <c r="P39" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q39" s="12"/>
       <c r="R39" s="12"/>
       <c r="S39" s="12"/>
@@ -3061,7 +3136,9 @@
       <c r="O40" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P40" s="12"/>
+      <c r="P40" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q40" s="12"/>
       <c r="R40" s="12"/>
       <c r="S40" s="12"/>
@@ -3121,7 +3198,9 @@
       <c r="O41" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P41" s="12"/>
+      <c r="P41" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q41" s="12"/>
       <c r="R41" s="12"/>
       <c r="S41" s="12"/>
@@ -3181,7 +3260,9 @@
       <c r="O42" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P42" s="12"/>
+      <c r="P42" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q42" s="12"/>
       <c r="R42" s="12"/>
       <c r="S42" s="12"/>
@@ -3241,7 +3322,9 @@
       <c r="O43" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P43" s="12"/>
+      <c r="P43" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q43" s="12"/>
       <c r="R43" s="12"/>
       <c r="S43" s="12"/>
@@ -3301,7 +3384,9 @@
       <c r="O44" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P44" s="12"/>
+      <c r="P44" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q44" s="12"/>
       <c r="R44" s="12"/>
       <c r="S44" s="12"/>
@@ -3361,7 +3446,9 @@
       <c r="O45" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P45" s="12"/>
+      <c r="P45" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q45" s="12"/>
       <c r="R45" s="12"/>
       <c r="S45" s="12"/>
@@ -3421,7 +3508,9 @@
       <c r="O46" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P46" s="12"/>
+      <c r="P46" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q46" s="12"/>
       <c r="R46" s="12"/>
       <c r="S46" s="12"/>
@@ -3481,7 +3570,9 @@
       <c r="O47" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P47" s="12"/>
+      <c r="P47" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q47" s="12"/>
       <c r="R47" s="12"/>
       <c r="S47" s="12"/>
@@ -3541,7 +3632,9 @@
       <c r="O48" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P48" s="12"/>
+      <c r="P48" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q48" s="12"/>
       <c r="R48" s="12"/>
       <c r="S48" s="12"/>
@@ -3601,7 +3694,9 @@
       <c r="O49" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P49" s="12"/>
+      <c r="P49" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q49" s="12"/>
       <c r="R49" s="12"/>
       <c r="S49" s="12"/>
@@ -3661,7 +3756,9 @@
       <c r="O50" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P50" s="12"/>
+      <c r="P50" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q50" s="12"/>
       <c r="R50" s="12"/>
       <c r="S50" s="12"/>
@@ -3721,7 +3818,9 @@
       <c r="O51" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P51" s="12"/>
+      <c r="P51" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q51" s="12"/>
       <c r="R51" s="12"/>
       <c r="S51" s="12"/>
@@ -3781,7 +3880,9 @@
       <c r="O52" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P52" s="12"/>
+      <c r="P52" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q52" s="12"/>
       <c r="R52" s="12"/>
       <c r="S52" s="12"/>
@@ -3841,7 +3942,9 @@
       <c r="O53" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P53" s="12"/>
+      <c r="P53" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q53" s="12"/>
       <c r="R53" s="12"/>
       <c r="S53" s="12"/>
@@ -3901,7 +4004,9 @@
       <c r="O54" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P54" s="12"/>
+      <c r="P54" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q54" s="12"/>
       <c r="R54" s="12"/>
       <c r="S54" s="12"/>
@@ -3961,7 +4066,9 @@
       <c r="O55" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="P55" s="12"/>
+      <c r="P55" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="Q55" s="12"/>
       <c r="R55" s="12"/>
       <c r="S55" s="12"/>
@@ -3980,10 +4087,10 @@
       <c r="AF55" s="12"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="30"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>COUNTIF(D7:D55,"A")</f>
@@ -4035,7 +4142,7 @@
       </c>
       <c r="P56" s="12">
         <f t="shared" ref="P56" si="10">COUNTIF(P7:P55,"A")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q56" s="12">
         <f t="shared" ref="Q56" si="11">COUNTIF(Q7:Q55,"A")</f>
@@ -4103,10 +4210,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="24"/>
+      <c r="B57" s="25"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(49-D56)</f>
@@ -4158,7 +4265,7 @@
       </c>
       <c r="P57" s="12">
         <f t="shared" ref="P57" si="37">(49-P56)</f>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q57" s="12">
         <f t="shared" ref="Q57" si="38">(49-Q56)</f>
@@ -4260,61 +4367,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="19" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="11" t="s">
         <v>57</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>56</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -4359,8 +4466,8 @@
       <c r="AF4" s="19"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="31"/>
-      <c r="B5" s="33"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="9" t="s">
         <v>49</v>
       </c>
@@ -4403,8 +4510,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="31"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="10" t="s">
         <v>50</v>
       </c>
@@ -6309,10 +6416,10 @@
       <c r="AF55" s="19"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="30"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>COUNTIF(D7:D55,"A")</f>
@@ -6432,10 +6539,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="24"/>
+      <c r="B57" s="25"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>(49-D56)</f>

</xml_diff>

<commit_message>
Last Update 24-09-2018 14:21:25.02
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="16605" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="62">
   <si>
     <t>S.NO</t>
   </si>
@@ -376,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -418,6 +418,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -792,75 +798,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG50" sqref="AG50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
     <col min="4" max="32" width="4.140625" style="2" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
+    <col min="33" max="33" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -908,7 +915,9 @@
       <c r="Q4" s="12">
         <v>9</v>
       </c>
-      <c r="R4" s="12"/>
+      <c r="R4" s="12">
+        <v>9</v>
+      </c>
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
       <c r="U4" s="12"/>
@@ -925,8 +934,8 @@
       <c r="AF4" s="12"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="33"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -972,7 +981,9 @@
       <c r="Q5" s="12">
         <v>19</v>
       </c>
-      <c r="R5" s="12"/>
+      <c r="R5" s="12">
+        <v>24</v>
+      </c>
       <c r="S5" s="12"/>
       <c r="T5" s="12"/>
       <c r="U5" s="12"/>
@@ -989,8 +1000,8 @@
       <c r="AF5" s="12"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="33"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -1036,7 +1047,9 @@
       <c r="Q6" s="12">
         <v>4</v>
       </c>
-      <c r="R6" s="12"/>
+      <c r="R6" s="12">
+        <v>4</v>
+      </c>
       <c r="S6" s="12"/>
       <c r="T6" s="12"/>
       <c r="U6" s="12"/>
@@ -1102,7 +1115,9 @@
       <c r="Q7" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R7" s="12"/>
+      <c r="R7" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
@@ -1168,7 +1183,9 @@
       <c r="Q8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="R8" s="12"/>
+      <c r="R8" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
@@ -1234,7 +1251,9 @@
       <c r="Q9" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R9" s="12"/>
+      <c r="R9" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
@@ -1300,7 +1319,9 @@
       <c r="Q10" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R10" s="12"/>
+      <c r="R10" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
@@ -1366,7 +1387,9 @@
       <c r="Q11" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R11" s="12"/>
+      <c r="R11" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S11" s="12"/>
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
@@ -1432,7 +1455,9 @@
       <c r="Q12" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R12" s="12"/>
+      <c r="R12" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S12" s="12"/>
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
@@ -1498,7 +1523,9 @@
       <c r="Q13" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R13" s="12"/>
+      <c r="R13" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S13" s="12"/>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
@@ -1564,7 +1591,9 @@
       <c r="Q14" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R14" s="12"/>
+      <c r="R14" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S14" s="12"/>
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
@@ -1630,7 +1659,9 @@
       <c r="Q15" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R15" s="12"/>
+      <c r="R15" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S15" s="12"/>
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
@@ -1696,7 +1727,9 @@
       <c r="Q16" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R16" s="12"/>
+      <c r="R16" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S16" s="12"/>
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
@@ -1762,7 +1795,9 @@
       <c r="Q17" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R17" s="12"/>
+      <c r="R17" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
@@ -1828,7 +1863,9 @@
       <c r="Q18" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R18" s="12"/>
+      <c r="R18" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
@@ -1894,7 +1931,9 @@
       <c r="Q19" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R19" s="12"/>
+      <c r="R19" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S19" s="12"/>
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
@@ -1960,7 +1999,9 @@
       <c r="Q20" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R20" s="12"/>
+      <c r="R20" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S20" s="12"/>
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
@@ -2026,7 +2067,9 @@
       <c r="Q21" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R21" s="12"/>
+      <c r="R21" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S21" s="12"/>
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
@@ -2092,7 +2135,9 @@
       <c r="Q22" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R22" s="12"/>
+      <c r="R22" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S22" s="12"/>
       <c r="T22" s="12"/>
       <c r="U22" s="12"/>
@@ -2158,7 +2203,9 @@
       <c r="Q23" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="R23" s="12"/>
+      <c r="R23" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S23" s="12"/>
       <c r="T23" s="12"/>
       <c r="U23" s="12"/>
@@ -2224,7 +2271,9 @@
       <c r="Q24" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R24" s="12"/>
+      <c r="R24" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S24" s="12"/>
       <c r="T24" s="12"/>
       <c r="U24" s="12"/>
@@ -2290,7 +2339,9 @@
       <c r="Q25" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R25" s="12"/>
+      <c r="R25" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S25" s="12"/>
       <c r="T25" s="12"/>
       <c r="U25" s="12"/>
@@ -2356,7 +2407,9 @@
       <c r="Q26" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R26" s="12"/>
+      <c r="R26" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S26" s="12"/>
       <c r="T26" s="12"/>
       <c r="U26" s="12"/>
@@ -2422,7 +2475,9 @@
       <c r="Q27" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R27" s="12"/>
+      <c r="R27" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S27" s="12"/>
       <c r="T27" s="12"/>
       <c r="U27" s="12"/>
@@ -2488,7 +2543,9 @@
       <c r="Q28" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R28" s="12"/>
+      <c r="R28" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S28" s="12"/>
       <c r="T28" s="12"/>
       <c r="U28" s="12"/>
@@ -2554,7 +2611,9 @@
       <c r="Q29" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R29" s="12"/>
+      <c r="R29" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S29" s="12"/>
       <c r="T29" s="12"/>
       <c r="U29" s="12"/>
@@ -2620,7 +2679,9 @@
       <c r="Q30" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R30" s="12"/>
+      <c r="R30" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="S30" s="12"/>
       <c r="T30" s="12"/>
       <c r="U30" s="12"/>
@@ -2686,7 +2747,9 @@
       <c r="Q31" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R31" s="12"/>
+      <c r="R31" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S31" s="12"/>
       <c r="T31" s="12"/>
       <c r="U31" s="12"/>
@@ -2752,7 +2815,9 @@
       <c r="Q32" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R32" s="12"/>
+      <c r="R32" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S32" s="12"/>
       <c r="T32" s="12"/>
       <c r="U32" s="12"/>
@@ -2818,7 +2883,9 @@
       <c r="Q33" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R33" s="12"/>
+      <c r="R33" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S33" s="12"/>
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
@@ -2884,7 +2951,9 @@
       <c r="Q34" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R34" s="12"/>
+      <c r="R34" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S34" s="12"/>
       <c r="T34" s="12"/>
       <c r="U34" s="12"/>
@@ -2950,7 +3019,9 @@
       <c r="Q35" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R35" s="12"/>
+      <c r="R35" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S35" s="12"/>
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
@@ -3016,7 +3087,9 @@
       <c r="Q36" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R36" s="12"/>
+      <c r="R36" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S36" s="12"/>
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
@@ -3082,7 +3155,9 @@
       <c r="Q37" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R37" s="12"/>
+      <c r="R37" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S37" s="12"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
@@ -3148,7 +3223,9 @@
       <c r="Q38" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R38" s="12"/>
+      <c r="R38" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S38" s="12"/>
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
@@ -3214,7 +3291,9 @@
       <c r="Q39" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R39" s="12"/>
+      <c r="R39" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S39" s="12"/>
       <c r="T39" s="12"/>
       <c r="U39" s="12"/>
@@ -3280,7 +3359,9 @@
       <c r="Q40" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R40" s="12"/>
+      <c r="R40" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S40" s="12"/>
       <c r="T40" s="12"/>
       <c r="U40" s="12"/>
@@ -3346,7 +3427,9 @@
       <c r="Q41" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R41" s="12"/>
+      <c r="R41" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S41" s="12"/>
       <c r="T41" s="12"/>
       <c r="U41" s="12"/>
@@ -3412,7 +3495,9 @@
       <c r="Q42" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R42" s="12"/>
+      <c r="R42" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S42" s="12"/>
       <c r="T42" s="12"/>
       <c r="U42" s="12"/>
@@ -3478,7 +3563,9 @@
       <c r="Q43" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R43" s="12"/>
+      <c r="R43" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S43" s="12"/>
       <c r="T43" s="12"/>
       <c r="U43" s="12"/>
@@ -3544,7 +3631,9 @@
       <c r="Q44" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R44" s="12"/>
+      <c r="R44" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="S44" s="12"/>
       <c r="T44" s="12"/>
       <c r="U44" s="12"/>
@@ -3610,7 +3699,9 @@
       <c r="Q45" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R45" s="12"/>
+      <c r="R45" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S45" s="12"/>
       <c r="T45" s="12"/>
       <c r="U45" s="12"/>
@@ -3676,7 +3767,9 @@
       <c r="Q46" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R46" s="12"/>
+      <c r="R46" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S46" s="12"/>
       <c r="T46" s="12"/>
       <c r="U46" s="12"/>
@@ -3742,7 +3835,9 @@
       <c r="Q47" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R47" s="12"/>
+      <c r="R47" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S47" s="12"/>
       <c r="T47" s="12"/>
       <c r="U47" s="12"/>
@@ -3808,7 +3903,9 @@
       <c r="Q48" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R48" s="12"/>
+      <c r="R48" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S48" s="12"/>
       <c r="T48" s="12"/>
       <c r="U48" s="12"/>
@@ -3874,7 +3971,9 @@
       <c r="Q49" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R49" s="12"/>
+      <c r="R49" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S49" s="12"/>
       <c r="T49" s="12"/>
       <c r="U49" s="12"/>
@@ -3940,7 +4039,9 @@
       <c r="Q50" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R50" s="12"/>
+      <c r="R50" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S50" s="12"/>
       <c r="T50" s="12"/>
       <c r="U50" s="12"/>
@@ -4006,7 +4107,9 @@
       <c r="Q51" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R51" s="12"/>
+      <c r="R51" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S51" s="12"/>
       <c r="T51" s="12"/>
       <c r="U51" s="12"/>
@@ -4072,7 +4175,9 @@
       <c r="Q52" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R52" s="12"/>
+      <c r="R52" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="S52" s="12"/>
       <c r="T52" s="12"/>
       <c r="U52" s="12"/>
@@ -4138,7 +4243,9 @@
       <c r="Q53" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R53" s="12"/>
+      <c r="R53" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S53" s="12"/>
       <c r="T53" s="12"/>
       <c r="U53" s="12"/>
@@ -4204,7 +4311,9 @@
       <c r="Q54" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R54" s="12"/>
+      <c r="R54" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="S54" s="12"/>
       <c r="T54" s="12"/>
       <c r="U54" s="12"/>
@@ -4221,10 +4330,10 @@
       <c r="AF54" s="12"/>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="32"/>
+      <c r="B55" s="34"/>
       <c r="C55" s="13"/>
       <c r="D55" s="12">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -4284,7 +4393,7 @@
       </c>
       <c r="R55" s="12">
         <f t="shared" ref="R55" si="12">COUNTIF(R7:R54,"A")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S55" s="12">
         <f t="shared" ref="S55" si="13">COUNTIF(S7:S54,"A")</f>
@@ -4344,10 +4453,10 @@
       </c>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="26"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>(48-D55)</f>
@@ -4407,7 +4516,7 @@
       </c>
       <c r="R56" s="24">
         <f t="shared" si="27"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="S56" s="24">
         <f t="shared" si="27"/>
@@ -4487,11 +4596,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="AH11" sqref="AH11"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
@@ -4501,61 +4610,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -4608,8 +4717,8 @@
       <c r="AF4" s="19"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="33"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -4660,8 +4769,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="33"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -4731,10 +4840,18 @@
       <c r="G7" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="H7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
@@ -4777,10 +4894,18 @@
       <c r="G8" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
+      <c r="H8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L8" s="19"/>
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
@@ -4823,10 +4948,18 @@
       <c r="G9" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
+      <c r="H9" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
@@ -4869,10 +5002,18 @@
       <c r="G10" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
+      <c r="H10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
@@ -4915,10 +5056,18 @@
       <c r="G11" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
+      <c r="H11" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
@@ -4961,10 +5110,18 @@
       <c r="G12" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
+      <c r="H12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
@@ -5007,10 +5164,18 @@
       <c r="G13" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
+      <c r="H13" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
@@ -5053,10 +5218,18 @@
       <c r="G14" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
+      <c r="H14" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
@@ -5099,10 +5272,18 @@
       <c r="G15" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+      <c r="H15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
@@ -5145,10 +5326,18 @@
       <c r="G16" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
+      <c r="H16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
@@ -5191,10 +5380,18 @@
       <c r="G17" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
+      <c r="H17" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
@@ -5237,10 +5434,18 @@
       <c r="G18" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+      <c r="H18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
@@ -5283,10 +5488,18 @@
       <c r="G19" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="H19" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
@@ -5329,10 +5542,18 @@
       <c r="G20" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
+      <c r="H20" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
@@ -5375,10 +5596,18 @@
       <c r="G21" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
+      <c r="H21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
@@ -5421,10 +5650,18 @@
       <c r="G22" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
+      <c r="H22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
@@ -5467,10 +5704,18 @@
       <c r="G23" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
+      <c r="H23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L23" s="19"/>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
@@ -5513,10 +5758,18 @@
       <c r="G24" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
+      <c r="H24" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L24" s="19"/>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
@@ -5559,10 +5812,18 @@
       <c r="G25" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
+      <c r="H25" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L25" s="19"/>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
@@ -5605,10 +5866,18 @@
       <c r="G26" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
+      <c r="H26" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L26" s="19"/>
       <c r="M26" s="19"/>
       <c r="N26" s="19"/>
@@ -5651,10 +5920,18 @@
       <c r="G27" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
+      <c r="H27" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
@@ -5697,10 +5974,18 @@
       <c r="G28" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
+      <c r="H28" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L28" s="19"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -5743,10 +6028,18 @@
       <c r="G29" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
+      <c r="H29" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L29" s="19"/>
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
@@ -5789,10 +6082,18 @@
       <c r="G30" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
+      <c r="H30" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J30" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
       <c r="N30" s="19"/>
@@ -5835,10 +6136,18 @@
       <c r="G31" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="H31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
       <c r="N31" s="19"/>
@@ -5881,10 +6190,18 @@
       <c r="G32" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
+      <c r="H32" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
@@ -5927,10 +6244,18 @@
       <c r="G33" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
+      <c r="H33" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
@@ -5973,10 +6298,18 @@
       <c r="G34" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
+      <c r="H34" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J34" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K34" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
@@ -6019,10 +6352,18 @@
       <c r="G35" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
+      <c r="H35" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K35" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L35" s="19"/>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
@@ -6065,10 +6406,18 @@
       <c r="G36" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
+      <c r="H36" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K36" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L36" s="19"/>
       <c r="M36" s="19"/>
       <c r="N36" s="19"/>
@@ -6111,10 +6460,18 @@
       <c r="G37" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
+      <c r="H37" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L37" s="19"/>
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
@@ -6157,10 +6514,18 @@
       <c r="G38" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
+      <c r="H38" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L38" s="19"/>
       <c r="M38" s="19"/>
       <c r="N38" s="19"/>
@@ -6203,10 +6568,18 @@
       <c r="G39" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
+      <c r="H39" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L39" s="19"/>
       <c r="M39" s="19"/>
       <c r="N39" s="19"/>
@@ -6249,10 +6622,18 @@
       <c r="G40" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
+      <c r="H40" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J40" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L40" s="19"/>
       <c r="M40" s="19"/>
       <c r="N40" s="19"/>
@@ -6295,10 +6676,18 @@
       <c r="G41" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
+      <c r="H41" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J41" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K41" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L41" s="19"/>
       <c r="M41" s="19"/>
       <c r="N41" s="19"/>
@@ -6341,10 +6730,18 @@
       <c r="G42" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
+      <c r="H42" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I42" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J42" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K42" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L42" s="19"/>
       <c r="M42" s="19"/>
       <c r="N42" s="19"/>
@@ -6387,10 +6784,18 @@
       <c r="G43" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
+      <c r="H43" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K43" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="L43" s="19"/>
       <c r="M43" s="19"/>
       <c r="N43" s="19"/>
@@ -6433,10 +6838,18 @@
       <c r="G44" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
+      <c r="H44" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I44" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J44" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K44" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L44" s="19"/>
       <c r="M44" s="19"/>
       <c r="N44" s="19"/>
@@ -6479,10 +6892,18 @@
       <c r="G45" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
+      <c r="H45" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I45" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K45" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L45" s="19"/>
       <c r="M45" s="19"/>
       <c r="N45" s="19"/>
@@ -6525,10 +6946,18 @@
       <c r="G46" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
+      <c r="H46" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I46" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J46" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K46" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L46" s="19"/>
       <c r="M46" s="19"/>
       <c r="N46" s="19"/>
@@ -6571,10 +7000,18 @@
       <c r="G47" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
+      <c r="H47" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I47" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J47" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K47" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L47" s="19"/>
       <c r="M47" s="19"/>
       <c r="N47" s="19"/>
@@ -6617,10 +7054,18 @@
       <c r="G48" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
+      <c r="H48" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I48" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J48" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K48" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L48" s="19"/>
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
@@ -6663,10 +7108,18 @@
       <c r="G49" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="19"/>
-      <c r="K49" s="19"/>
+      <c r="H49" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I49" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J49" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K49" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L49" s="19"/>
       <c r="M49" s="19"/>
       <c r="N49" s="19"/>
@@ -6709,10 +7162,18 @@
       <c r="G50" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
+      <c r="H50" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I50" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J50" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K50" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L50" s="19"/>
       <c r="M50" s="19"/>
       <c r="N50" s="19"/>
@@ -6755,10 +7216,18 @@
       <c r="G51" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
+      <c r="H51" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I51" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J51" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K51" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L51" s="19"/>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -6801,10 +7270,18 @@
       <c r="G52" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
+      <c r="H52" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I52" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J52" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K52" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L52" s="19"/>
       <c r="M52" s="19"/>
       <c r="N52" s="19"/>
@@ -6847,10 +7324,18 @@
       <c r="G53" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
+      <c r="H53" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I53" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J53" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K53" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L53" s="19"/>
       <c r="M53" s="19"/>
       <c r="N53" s="19"/>
@@ -6893,10 +7378,18 @@
       <c r="G54" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
+      <c r="H54" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I54" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J54" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="K54" s="25" t="s">
+        <v>54</v>
+      </c>
       <c r="L54" s="19"/>
       <c r="M54" s="19"/>
       <c r="N54" s="19"/>
@@ -6920,10 +7413,10 @@
       <c r="AF54" s="19"/>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="31" t="s">
+      <c r="A55" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="32"/>
+      <c r="B55" s="34"/>
       <c r="C55" s="13"/>
       <c r="D55" s="19">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -6943,19 +7436,19 @@
       </c>
       <c r="H55" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I55" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J55" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K55" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L55" s="19">
         <f t="shared" si="0"/>
@@ -7043,10 +7536,10 @@
       </c>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="26"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>(48-D55)</f>
@@ -7066,19 +7559,19 @@
       </c>
       <c r="H56" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="I56" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J56" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="K56" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="L56" s="24">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Last Update 26-09-2018  8:51:42.13
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -10,12 +10,206 @@
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
     <sheet name="Lab Attendance" sheetId="4" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$Q$1:$Q$56</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Rajasekaran S</author>
+  </authors>
+  <commentList>
+    <comment ref="D6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Introduction to Problem Solving</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Factorial using Recurssion and Solving Tower of Honai Problem</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tower of Honai Problem and Introduction to Programming Languages</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Unit Test 1
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Unit Test 1
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Rajasekaran S</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rajasekaran S:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Finding GCD of Given numbers
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Finding Sqrt</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="62">
   <si>
     <t>S.NO</t>
   </si>
@@ -207,7 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +447,32 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -376,7 +596,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -418,6 +638,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -796,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF56"/>
+  <dimension ref="A1:AE56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -807,67 +1030,67 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
-    <col min="4" max="32" width="4.140625" style="2" customWidth="1"/>
-    <col min="33" max="33" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="31" width="4.140625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:31" ht="18.75">
+      <c r="A1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
+    </row>
+    <row r="2" spans="1:31" ht="19.5">
+      <c r="A2" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-    </row>
-    <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="40" t="s">
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+    </row>
+    <row r="3" spans="1:31" ht="18.75">
+      <c r="A3" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-    </row>
-    <row r="4" spans="1:32">
-      <c r="A4" s="35" t="s">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -918,8 +1141,12 @@
       <c r="R4" s="12">
         <v>9</v>
       </c>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
+      <c r="S4" s="12">
+        <v>9</v>
+      </c>
+      <c r="T4" s="27">
+        <v>9</v>
+      </c>
       <c r="U4" s="12"/>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
@@ -931,11 +1158,10 @@
       <c r="AC4" s="12"/>
       <c r="AD4" s="12"/>
       <c r="AE4" s="12"/>
-      <c r="AF4" s="12"/>
-    </row>
-    <row r="5" spans="1:32">
-      <c r="A5" s="35"/>
-      <c r="B5" s="37"/>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="A5" s="36"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -984,8 +1210,12 @@
       <c r="R5" s="12">
         <v>24</v>
       </c>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
+      <c r="S5" s="12">
+        <v>25</v>
+      </c>
+      <c r="T5" s="27">
+        <v>25</v>
+      </c>
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
@@ -997,11 +1227,10 @@
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
       <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-    </row>
-    <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="38"/>
+    </row>
+    <row r="6" spans="1:31" ht="15" customHeight="1">
+      <c r="A6" s="36"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -1050,8 +1279,12 @@
       <c r="R6" s="12">
         <v>4</v>
       </c>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
+      <c r="S6" s="12">
+        <v>1</v>
+      </c>
+      <c r="T6" s="27">
+        <v>2</v>
+      </c>
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
@@ -1063,9 +1296,8 @@
       <c r="AC6" s="12"/>
       <c r="AD6" s="12"/>
       <c r="AE6" s="12"/>
-      <c r="AF6" s="12"/>
-    </row>
-    <row r="7" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="7" spans="1:31" ht="15" customHeight="1">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1118,8 +1350,12 @@
       <c r="R7" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
+      <c r="S7" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T7" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
@@ -1131,9 +1367,8 @@
       <c r="AC7" s="12"/>
       <c r="AD7" s="12"/>
       <c r="AE7" s="12"/>
-      <c r="AF7" s="12"/>
-    </row>
-    <row r="8" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:31" ht="15" customHeight="1">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -1186,8 +1421,12 @@
       <c r="R8" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
+      <c r="S8" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T8" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -1199,9 +1438,8 @@
       <c r="AC8" s="12"/>
       <c r="AD8" s="12"/>
       <c r="AE8" s="12"/>
-      <c r="AF8" s="12"/>
-    </row>
-    <row r="9" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="9" spans="1:31" ht="15" customHeight="1">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -1254,8 +1492,12 @@
       <c r="R9" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
+      <c r="S9" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T9" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
@@ -1267,9 +1509,8 @@
       <c r="AC9" s="12"/>
       <c r="AD9" s="12"/>
       <c r="AE9" s="12"/>
-      <c r="AF9" s="12"/>
-    </row>
-    <row r="10" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="10" spans="1:31" ht="15" customHeight="1">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -1322,8 +1563,12 @@
       <c r="R10" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
+      <c r="S10" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T10" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U10" s="12"/>
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
@@ -1335,9 +1580,8 @@
       <c r="AC10" s="12"/>
       <c r="AD10" s="12"/>
       <c r="AE10" s="12"/>
-      <c r="AF10" s="12"/>
-    </row>
-    <row r="11" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="11" spans="1:31" ht="15" customHeight="1">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -1390,8 +1634,12 @@
       <c r="R11" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
+      <c r="S11" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T11" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
@@ -1403,9 +1651,8 @@
       <c r="AC11" s="12"/>
       <c r="AD11" s="12"/>
       <c r="AE11" s="12"/>
-      <c r="AF11" s="12"/>
-    </row>
-    <row r="12" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="12" spans="1:31" ht="15" customHeight="1">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -1458,8 +1705,12 @@
       <c r="R12" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S12" s="12"/>
-      <c r="T12" s="12"/>
+      <c r="S12" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T12" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
@@ -1471,9 +1722,8 @@
       <c r="AC12" s="12"/>
       <c r="AD12" s="12"/>
       <c r="AE12" s="12"/>
-      <c r="AF12" s="12"/>
-    </row>
-    <row r="13" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="13" spans="1:31" ht="15" customHeight="1">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -1526,8 +1776,12 @@
       <c r="R13" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S13" s="12"/>
-      <c r="T13" s="12"/>
+      <c r="S13" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T13" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
@@ -1539,9 +1793,8 @@
       <c r="AC13" s="12"/>
       <c r="AD13" s="12"/>
       <c r="AE13" s="12"/>
-      <c r="AF13" s="12"/>
-    </row>
-    <row r="14" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="14" spans="1:31" ht="15" customHeight="1">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -1594,8 +1847,12 @@
       <c r="R14" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
+      <c r="S14" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T14" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U14" s="12"/>
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
@@ -1607,9 +1864,8 @@
       <c r="AC14" s="12"/>
       <c r="AD14" s="12"/>
       <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
-    </row>
-    <row r="15" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:31" ht="15" customHeight="1">
       <c r="A15" s="3">
         <v>9</v>
       </c>
@@ -1662,8 +1918,12 @@
       <c r="R15" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S15" s="12"/>
-      <c r="T15" s="12"/>
+      <c r="S15" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T15" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U15" s="12"/>
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
@@ -1675,9 +1935,8 @@
       <c r="AC15" s="12"/>
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
-      <c r="AF15" s="12"/>
-    </row>
-    <row r="16" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="16" spans="1:31" ht="15" customHeight="1">
       <c r="A16" s="3">
         <v>10</v>
       </c>
@@ -1730,8 +1989,12 @@
       <c r="R16" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
+      <c r="S16" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T16" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U16" s="12"/>
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
@@ -1743,9 +2006,8 @@
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
-      <c r="AF16" s="12"/>
-    </row>
-    <row r="17" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="17" spans="1:31" ht="15" customHeight="1">
       <c r="A17" s="3">
         <v>11</v>
       </c>
@@ -1798,8 +2060,12 @@
       <c r="R17" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
+      <c r="S17" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T17" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U17" s="12"/>
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
@@ -1811,9 +2077,8 @@
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
       <c r="AE17" s="12"/>
-      <c r="AF17" s="12"/>
-    </row>
-    <row r="18" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="18" spans="1:31" ht="15" customHeight="1">
       <c r="A18" s="3">
         <v>12</v>
       </c>
@@ -1866,8 +2131,12 @@
       <c r="R18" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
+      <c r="S18" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T18" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U18" s="12"/>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
@@ -1879,9 +2148,8 @@
       <c r="AC18" s="12"/>
       <c r="AD18" s="12"/>
       <c r="AE18" s="12"/>
-      <c r="AF18" s="12"/>
-    </row>
-    <row r="19" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="19" spans="1:31" ht="15" customHeight="1">
       <c r="A19" s="3">
         <v>13</v>
       </c>
@@ -1934,8 +2202,12 @@
       <c r="R19" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12"/>
+      <c r="S19" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T19" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U19" s="12"/>
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
@@ -1947,9 +2219,8 @@
       <c r="AC19" s="12"/>
       <c r="AD19" s="12"/>
       <c r="AE19" s="12"/>
-      <c r="AF19" s="12"/>
-    </row>
-    <row r="20" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="20" spans="1:31" ht="15" customHeight="1">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -2002,8 +2273,12 @@
       <c r="R20" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S20" s="12"/>
-      <c r="T20" s="12"/>
+      <c r="S20" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T20" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U20" s="12"/>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
@@ -2015,9 +2290,8 @@
       <c r="AC20" s="12"/>
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
-      <c r="AF20" s="12"/>
-    </row>
-    <row r="21" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="21" spans="1:31" ht="15" customHeight="1">
       <c r="A21" s="3">
         <v>15</v>
       </c>
@@ -2070,8 +2344,12 @@
       <c r="R21" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
+      <c r="S21" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T21" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U21" s="12"/>
       <c r="V21" s="12"/>
       <c r="W21" s="12"/>
@@ -2083,9 +2361,8 @@
       <c r="AC21" s="12"/>
       <c r="AD21" s="12"/>
       <c r="AE21" s="12"/>
-      <c r="AF21" s="12"/>
-    </row>
-    <row r="22" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="22" spans="1:31" ht="15" customHeight="1">
       <c r="A22" s="3">
         <v>16</v>
       </c>
@@ -2138,8 +2415,12 @@
       <c r="R22" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
+      <c r="S22" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T22" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U22" s="12"/>
       <c r="V22" s="12"/>
       <c r="W22" s="12"/>
@@ -2151,9 +2432,8 @@
       <c r="AC22" s="12"/>
       <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
-      <c r="AF22" s="12"/>
-    </row>
-    <row r="23" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="23" spans="1:31" ht="15" customHeight="1">
       <c r="A23" s="3">
         <v>17</v>
       </c>
@@ -2206,8 +2486,12 @@
       <c r="R23" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
+      <c r="S23" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T23" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U23" s="12"/>
       <c r="V23" s="12"/>
       <c r="W23" s="12"/>
@@ -2219,9 +2503,8 @@
       <c r="AC23" s="12"/>
       <c r="AD23" s="12"/>
       <c r="AE23" s="12"/>
-      <c r="AF23" s="12"/>
-    </row>
-    <row r="24" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="24" spans="1:31" ht="15" customHeight="1">
       <c r="A24" s="3">
         <v>18</v>
       </c>
@@ -2274,8 +2557,12 @@
       <c r="R24" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S24" s="12"/>
-      <c r="T24" s="12"/>
+      <c r="S24" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T24" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U24" s="12"/>
       <c r="V24" s="12"/>
       <c r="W24" s="12"/>
@@ -2287,9 +2574,8 @@
       <c r="AC24" s="12"/>
       <c r="AD24" s="12"/>
       <c r="AE24" s="12"/>
-      <c r="AF24" s="12"/>
-    </row>
-    <row r="25" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="25" spans="1:31" ht="15" customHeight="1">
       <c r="A25" s="3">
         <v>19</v>
       </c>
@@ -2342,8 +2628,12 @@
       <c r="R25" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S25" s="12"/>
-      <c r="T25" s="12"/>
+      <c r="S25" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T25" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U25" s="12"/>
       <c r="V25" s="12"/>
       <c r="W25" s="12"/>
@@ -2355,9 +2645,8 @@
       <c r="AC25" s="12"/>
       <c r="AD25" s="12"/>
       <c r="AE25" s="12"/>
-      <c r="AF25" s="12"/>
-    </row>
-    <row r="26" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="26" spans="1:31" ht="15" customHeight="1">
       <c r="A26" s="3">
         <v>20</v>
       </c>
@@ -2410,8 +2699,12 @@
       <c r="R26" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S26" s="12"/>
-      <c r="T26" s="12"/>
+      <c r="S26" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T26" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U26" s="12"/>
       <c r="V26" s="12"/>
       <c r="W26" s="12"/>
@@ -2423,9 +2716,8 @@
       <c r="AC26" s="12"/>
       <c r="AD26" s="12"/>
       <c r="AE26" s="12"/>
-      <c r="AF26" s="12"/>
-    </row>
-    <row r="27" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="27" spans="1:31" ht="15" customHeight="1">
       <c r="A27" s="3">
         <v>21</v>
       </c>
@@ -2478,8 +2770,12 @@
       <c r="R27" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
+      <c r="S27" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T27" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U27" s="12"/>
       <c r="V27" s="12"/>
       <c r="W27" s="12"/>
@@ -2491,9 +2787,8 @@
       <c r="AC27" s="12"/>
       <c r="AD27" s="12"/>
       <c r="AE27" s="12"/>
-      <c r="AF27" s="12"/>
-    </row>
-    <row r="28" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="28" spans="1:31" ht="15" customHeight="1">
       <c r="A28" s="3">
         <v>22</v>
       </c>
@@ -2546,8 +2841,12 @@
       <c r="R28" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S28" s="12"/>
-      <c r="T28" s="12"/>
+      <c r="S28" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T28" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U28" s="12"/>
       <c r="V28" s="12"/>
       <c r="W28" s="12"/>
@@ -2559,9 +2858,8 @@
       <c r="AC28" s="12"/>
       <c r="AD28" s="12"/>
       <c r="AE28" s="12"/>
-      <c r="AF28" s="12"/>
-    </row>
-    <row r="29" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="29" spans="1:31" ht="15" customHeight="1">
       <c r="A29" s="3">
         <v>23</v>
       </c>
@@ -2614,8 +2912,12 @@
       <c r="R29" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S29" s="12"/>
-      <c r="T29" s="12"/>
+      <c r="S29" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T29" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U29" s="12"/>
       <c r="V29" s="12"/>
       <c r="W29" s="12"/>
@@ -2627,9 +2929,8 @@
       <c r="AC29" s="12"/>
       <c r="AD29" s="12"/>
       <c r="AE29" s="12"/>
-      <c r="AF29" s="12"/>
-    </row>
-    <row r="30" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="30" spans="1:31" ht="15" customHeight="1">
       <c r="A30" s="3">
         <v>24</v>
       </c>
@@ -2682,8 +2983,12 @@
       <c r="R30" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="S30" s="12"/>
-      <c r="T30" s="12"/>
+      <c r="S30" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T30" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U30" s="12"/>
       <c r="V30" s="12"/>
       <c r="W30" s="12"/>
@@ -2695,9 +3000,8 @@
       <c r="AC30" s="12"/>
       <c r="AD30" s="12"/>
       <c r="AE30" s="12"/>
-      <c r="AF30" s="12"/>
-    </row>
-    <row r="31" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="31" spans="1:31" ht="15" customHeight="1">
       <c r="A31" s="3">
         <v>25</v>
       </c>
@@ -2750,8 +3054,12 @@
       <c r="R31" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S31" s="12"/>
-      <c r="T31" s="12"/>
+      <c r="S31" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T31" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U31" s="12"/>
       <c r="V31" s="12"/>
       <c r="W31" s="12"/>
@@ -2763,9 +3071,8 @@
       <c r="AC31" s="12"/>
       <c r="AD31" s="12"/>
       <c r="AE31" s="12"/>
-      <c r="AF31" s="12"/>
-    </row>
-    <row r="32" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="32" spans="1:31" ht="15" customHeight="1">
       <c r="A32" s="3">
         <v>26</v>
       </c>
@@ -2818,8 +3125,12 @@
       <c r="R32" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S32" s="12"/>
-      <c r="T32" s="12"/>
+      <c r="S32" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T32" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U32" s="12"/>
       <c r="V32" s="12"/>
       <c r="W32" s="12"/>
@@ -2831,9 +3142,8 @@
       <c r="AC32" s="12"/>
       <c r="AD32" s="12"/>
       <c r="AE32" s="12"/>
-      <c r="AF32" s="12"/>
-    </row>
-    <row r="33" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="33" spans="1:31" ht="15" customHeight="1">
       <c r="A33" s="3">
         <v>27</v>
       </c>
@@ -2886,8 +3196,12 @@
       <c r="R33" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S33" s="12"/>
-      <c r="T33" s="12"/>
+      <c r="S33" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T33" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U33" s="12"/>
       <c r="V33" s="12"/>
       <c r="W33" s="12"/>
@@ -2899,9 +3213,8 @@
       <c r="AC33" s="12"/>
       <c r="AD33" s="12"/>
       <c r="AE33" s="12"/>
-      <c r="AF33" s="12"/>
-    </row>
-    <row r="34" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="34" spans="1:31" ht="15" customHeight="1">
       <c r="A34" s="3">
         <v>28</v>
       </c>
@@ -2954,8 +3267,12 @@
       <c r="R34" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S34" s="12"/>
-      <c r="T34" s="12"/>
+      <c r="S34" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T34" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U34" s="12"/>
       <c r="V34" s="12"/>
       <c r="W34" s="12"/>
@@ -2967,9 +3284,8 @@
       <c r="AC34" s="12"/>
       <c r="AD34" s="12"/>
       <c r="AE34" s="12"/>
-      <c r="AF34" s="12"/>
-    </row>
-    <row r="35" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="35" spans="1:31" ht="15" customHeight="1">
       <c r="A35" s="3">
         <v>29</v>
       </c>
@@ -3022,8 +3338,12 @@
       <c r="R35" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S35" s="12"/>
-      <c r="T35" s="12"/>
+      <c r="S35" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T35" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U35" s="12"/>
       <c r="V35" s="12"/>
       <c r="W35" s="12"/>
@@ -3035,9 +3355,8 @@
       <c r="AC35" s="12"/>
       <c r="AD35" s="12"/>
       <c r="AE35" s="12"/>
-      <c r="AF35" s="12"/>
-    </row>
-    <row r="36" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="36" spans="1:31" ht="15" customHeight="1">
       <c r="A36" s="3">
         <v>30</v>
       </c>
@@ -3090,8 +3409,12 @@
       <c r="R36" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S36" s="12"/>
-      <c r="T36" s="12"/>
+      <c r="S36" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T36" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U36" s="12"/>
       <c r="V36" s="12"/>
       <c r="W36" s="12"/>
@@ -3103,9 +3426,8 @@
       <c r="AC36" s="12"/>
       <c r="AD36" s="12"/>
       <c r="AE36" s="12"/>
-      <c r="AF36" s="12"/>
-    </row>
-    <row r="37" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="37" spans="1:31" ht="15" customHeight="1">
       <c r="A37" s="3">
         <v>31</v>
       </c>
@@ -3158,8 +3480,12 @@
       <c r="R37" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S37" s="12"/>
-      <c r="T37" s="12"/>
+      <c r="S37" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T37" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U37" s="12"/>
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
@@ -3171,9 +3497,8 @@
       <c r="AC37" s="12"/>
       <c r="AD37" s="12"/>
       <c r="AE37" s="12"/>
-      <c r="AF37" s="12"/>
-    </row>
-    <row r="38" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="38" spans="1:31" ht="15" customHeight="1">
       <c r="A38" s="3">
         <v>32</v>
       </c>
@@ -3226,8 +3551,12 @@
       <c r="R38" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S38" s="12"/>
-      <c r="T38" s="12"/>
+      <c r="S38" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T38" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U38" s="12"/>
       <c r="V38" s="12"/>
       <c r="W38" s="12"/>
@@ -3239,9 +3568,8 @@
       <c r="AC38" s="12"/>
       <c r="AD38" s="12"/>
       <c r="AE38" s="12"/>
-      <c r="AF38" s="12"/>
-    </row>
-    <row r="39" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="39" spans="1:31" ht="15" customHeight="1">
       <c r="A39" s="3">
         <v>33</v>
       </c>
@@ -3294,8 +3622,12 @@
       <c r="R39" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S39" s="12"/>
-      <c r="T39" s="12"/>
+      <c r="S39" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T39" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U39" s="12"/>
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
@@ -3307,9 +3639,8 @@
       <c r="AC39" s="12"/>
       <c r="AD39" s="12"/>
       <c r="AE39" s="12"/>
-      <c r="AF39" s="12"/>
-    </row>
-    <row r="40" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="40" spans="1:31" ht="15" customHeight="1">
       <c r="A40" s="3">
         <v>34</v>
       </c>
@@ -3362,8 +3693,12 @@
       <c r="R40" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S40" s="12"/>
-      <c r="T40" s="12"/>
+      <c r="S40" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T40" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U40" s="12"/>
       <c r="V40" s="12"/>
       <c r="W40" s="12"/>
@@ -3375,9 +3710,8 @@
       <c r="AC40" s="12"/>
       <c r="AD40" s="12"/>
       <c r="AE40" s="12"/>
-      <c r="AF40" s="12"/>
-    </row>
-    <row r="41" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="41" spans="1:31" ht="15" customHeight="1">
       <c r="A41" s="3">
         <v>35</v>
       </c>
@@ -3430,8 +3764,12 @@
       <c r="R41" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S41" s="12"/>
-      <c r="T41" s="12"/>
+      <c r="S41" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T41" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U41" s="12"/>
       <c r="V41" s="12"/>
       <c r="W41" s="12"/>
@@ -3443,9 +3781,8 @@
       <c r="AC41" s="12"/>
       <c r="AD41" s="12"/>
       <c r="AE41" s="12"/>
-      <c r="AF41" s="12"/>
-    </row>
-    <row r="42" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="42" spans="1:31" ht="15" customHeight="1">
       <c r="A42" s="3">
         <v>36</v>
       </c>
@@ -3498,8 +3835,12 @@
       <c r="R42" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S42" s="12"/>
-      <c r="T42" s="12"/>
+      <c r="S42" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T42" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U42" s="12"/>
       <c r="V42" s="12"/>
       <c r="W42" s="12"/>
@@ -3511,9 +3852,8 @@
       <c r="AC42" s="12"/>
       <c r="AD42" s="12"/>
       <c r="AE42" s="12"/>
-      <c r="AF42" s="12"/>
-    </row>
-    <row r="43" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="43" spans="1:31" ht="15" customHeight="1">
       <c r="A43" s="3">
         <v>37</v>
       </c>
@@ -3566,8 +3906,12 @@
       <c r="R43" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S43" s="12"/>
-      <c r="T43" s="12"/>
+      <c r="S43" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T43" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U43" s="12"/>
       <c r="V43" s="12"/>
       <c r="W43" s="12"/>
@@ -3579,9 +3923,8 @@
       <c r="AC43" s="12"/>
       <c r="AD43" s="12"/>
       <c r="AE43" s="12"/>
-      <c r="AF43" s="12"/>
-    </row>
-    <row r="44" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="44" spans="1:31" ht="15" customHeight="1">
       <c r="A44" s="3">
         <v>38</v>
       </c>
@@ -3634,8 +3977,12 @@
       <c r="R44" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="S44" s="12"/>
-      <c r="T44" s="12"/>
+      <c r="S44" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T44" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U44" s="12"/>
       <c r="V44" s="12"/>
       <c r="W44" s="12"/>
@@ -3647,9 +3994,8 @@
       <c r="AC44" s="12"/>
       <c r="AD44" s="12"/>
       <c r="AE44" s="12"/>
-      <c r="AF44" s="12"/>
-    </row>
-    <row r="45" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="45" spans="1:31" ht="15" customHeight="1">
       <c r="A45" s="3">
         <v>39</v>
       </c>
@@ -3702,8 +4048,12 @@
       <c r="R45" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S45" s="12"/>
-      <c r="T45" s="12"/>
+      <c r="S45" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T45" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U45" s="12"/>
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
@@ -3715,9 +4065,8 @@
       <c r="AC45" s="12"/>
       <c r="AD45" s="12"/>
       <c r="AE45" s="12"/>
-      <c r="AF45" s="12"/>
-    </row>
-    <row r="46" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="46" spans="1:31" ht="15" customHeight="1">
       <c r="A46" s="3">
         <v>40</v>
       </c>
@@ -3770,8 +4119,12 @@
       <c r="R46" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S46" s="12"/>
-      <c r="T46" s="12"/>
+      <c r="S46" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T46" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U46" s="12"/>
       <c r="V46" s="12"/>
       <c r="W46" s="12"/>
@@ -3783,9 +4136,8 @@
       <c r="AC46" s="12"/>
       <c r="AD46" s="12"/>
       <c r="AE46" s="12"/>
-      <c r="AF46" s="12"/>
-    </row>
-    <row r="47" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="47" spans="1:31" ht="15" customHeight="1">
       <c r="A47" s="3">
         <v>41</v>
       </c>
@@ -3838,8 +4190,12 @@
       <c r="R47" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S47" s="12"/>
-      <c r="T47" s="12"/>
+      <c r="S47" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T47" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U47" s="12"/>
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>
@@ -3851,9 +4207,8 @@
       <c r="AC47" s="12"/>
       <c r="AD47" s="12"/>
       <c r="AE47" s="12"/>
-      <c r="AF47" s="12"/>
-    </row>
-    <row r="48" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="48" spans="1:31" ht="15" customHeight="1">
       <c r="A48" s="3">
         <v>42</v>
       </c>
@@ -3906,8 +4261,12 @@
       <c r="R48" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S48" s="12"/>
-      <c r="T48" s="12"/>
+      <c r="S48" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T48" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U48" s="12"/>
       <c r="V48" s="12"/>
       <c r="W48" s="12"/>
@@ -3919,9 +4278,8 @@
       <c r="AC48" s="12"/>
       <c r="AD48" s="12"/>
       <c r="AE48" s="12"/>
-      <c r="AF48" s="12"/>
-    </row>
-    <row r="49" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="49" spans="1:31" ht="15" customHeight="1">
       <c r="A49" s="3">
         <v>43</v>
       </c>
@@ -3974,8 +4332,12 @@
       <c r="R49" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S49" s="12"/>
-      <c r="T49" s="12"/>
+      <c r="S49" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T49" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U49" s="12"/>
       <c r="V49" s="12"/>
       <c r="W49" s="12"/>
@@ -3987,9 +4349,8 @@
       <c r="AC49" s="12"/>
       <c r="AD49" s="12"/>
       <c r="AE49" s="12"/>
-      <c r="AF49" s="12"/>
-    </row>
-    <row r="50" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="50" spans="1:31" ht="15" customHeight="1">
       <c r="A50" s="3">
         <v>44</v>
       </c>
@@ -4042,8 +4403,12 @@
       <c r="R50" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S50" s="12"/>
-      <c r="T50" s="12"/>
+      <c r="S50" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T50" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U50" s="12"/>
       <c r="V50" s="12"/>
       <c r="W50" s="12"/>
@@ -4055,9 +4420,8 @@
       <c r="AC50" s="12"/>
       <c r="AD50" s="12"/>
       <c r="AE50" s="12"/>
-      <c r="AF50" s="12"/>
-    </row>
-    <row r="51" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="51" spans="1:31" ht="15" customHeight="1">
       <c r="A51" s="3">
         <v>45</v>
       </c>
@@ -4110,8 +4474,12 @@
       <c r="R51" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S51" s="12"/>
-      <c r="T51" s="12"/>
+      <c r="S51" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T51" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U51" s="12"/>
       <c r="V51" s="12"/>
       <c r="W51" s="12"/>
@@ -4123,9 +4491,8 @@
       <c r="AC51" s="12"/>
       <c r="AD51" s="12"/>
       <c r="AE51" s="12"/>
-      <c r="AF51" s="12"/>
-    </row>
-    <row r="52" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="52" spans="1:31" ht="15" customHeight="1">
       <c r="A52" s="3">
         <v>46</v>
       </c>
@@ -4178,8 +4545,12 @@
       <c r="R52" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="S52" s="12"/>
-      <c r="T52" s="12"/>
+      <c r="S52" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T52" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U52" s="12"/>
       <c r="V52" s="12"/>
       <c r="W52" s="12"/>
@@ -4191,9 +4562,8 @@
       <c r="AC52" s="12"/>
       <c r="AD52" s="12"/>
       <c r="AE52" s="12"/>
-      <c r="AF52" s="12"/>
-    </row>
-    <row r="53" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="53" spans="1:31" ht="15" customHeight="1">
       <c r="A53" s="3">
         <v>47</v>
       </c>
@@ -4246,8 +4616,12 @@
       <c r="R53" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S53" s="12"/>
-      <c r="T53" s="12"/>
+      <c r="S53" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T53" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U53" s="12"/>
       <c r="V53" s="12"/>
       <c r="W53" s="12"/>
@@ -4259,9 +4633,8 @@
       <c r="AC53" s="12"/>
       <c r="AD53" s="12"/>
       <c r="AE53" s="12"/>
-      <c r="AF53" s="12"/>
-    </row>
-    <row r="54" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="54" spans="1:31" ht="15" customHeight="1">
       <c r="A54" s="3">
         <v>48</v>
       </c>
@@ -4314,8 +4687,12 @@
       <c r="R54" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="S54" s="12"/>
-      <c r="T54" s="12"/>
+      <c r="S54" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="T54" s="27" t="s">
+        <v>54</v>
+      </c>
       <c r="U54" s="12"/>
       <c r="V54" s="12"/>
       <c r="W54" s="12"/>
@@ -4327,13 +4704,12 @@
       <c r="AC54" s="12"/>
       <c r="AD54" s="12"/>
       <c r="AE54" s="12"/>
-      <c r="AF54" s="12"/>
-    </row>
-    <row r="55" spans="1:32">
-      <c r="A55" s="33" t="s">
+    </row>
+    <row r="55" spans="1:31">
+      <c r="A55" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="34"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="13"/>
       <c r="D55" s="12">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -4447,131 +4823,123 @@
         <f t="shared" ref="AE55" si="25">COUNTIF(AE7:AE54,"A")</f>
         <v>0</v>
       </c>
-      <c r="AF55" s="12">
-        <f t="shared" ref="AF55" si="26">COUNTIF(AF7:AF54,"A")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:32">
-      <c r="A56" s="27" t="s">
+    </row>
+    <row r="56" spans="1:31">
+      <c r="A56" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="28"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>(48-D55)</f>
         <v>48</v>
       </c>
       <c r="E56" s="24">
-        <f t="shared" ref="E56:AF56" si="27">(48-E55)</f>
+        <f t="shared" ref="E56:AE56" si="26">(48-E55)</f>
         <v>48</v>
       </c>
       <c r="F56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>47</v>
       </c>
       <c r="G56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>46</v>
       </c>
       <c r="H56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>37</v>
       </c>
       <c r="I56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>37</v>
       </c>
       <c r="J56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>47</v>
       </c>
       <c r="K56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>47</v>
       </c>
       <c r="L56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>42</v>
       </c>
       <c r="M56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>37</v>
       </c>
       <c r="N56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>45</v>
       </c>
       <c r="O56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>47</v>
       </c>
       <c r="P56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>47</v>
       </c>
       <c r="Q56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>46</v>
       </c>
       <c r="R56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>45</v>
       </c>
       <c r="S56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="T56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="U56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="V56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="W56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="X56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="Y56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="Z56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="AA56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="AB56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="AC56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="AD56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
       <c r="AE56" s="24">
-        <f t="shared" si="27"/>
-        <v>48</v>
-      </c>
-      <c r="AF56" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>48</v>
       </c>
     </row>
@@ -4589,6 +4957,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4596,8 +4965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF56"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -4610,61 +4979,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -4717,8 +5086,8 @@
       <c r="AF4" s="19"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="35"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -4769,8 +5138,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -7413,10 +7782,10 @@
       <c r="AF54" s="19"/>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="34"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="13"/>
       <c r="D55" s="19">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -7536,10 +7905,10 @@
       </c>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="27" t="s">
+      <c r="A56" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="28"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>(48-D55)</f>
@@ -7672,5 +8041,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last Update 26-09-2018 14:30:50.44
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -47,6 +47,297 @@
         </r>
       </text>
     </comment>
+    <comment ref="E6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Algorithm</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Good Qualities of Algorithm</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Building Blocks of Algorithm (Variables, Statements, Conditionals)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Building Blocks of Algorithm
+(Unconditional Control Flow, Functions)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Simple Algorithms
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Notations of Algorithms</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rajasekaran S
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Flow Chart</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Pseudo Code</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Algorithamic Problem Solving</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Simple Stratergies [Iteration]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+llustrative problems: find minimum
+in a list</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+insert a card in a list of sorted cards</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="Q6" authorId="0">
       <text>
         <r>
@@ -67,7 +358,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Factorial using Recurssion and Solving Tower of Honai Problem</t>
+guess an integer number in a range</t>
         </r>
       </text>
     </comment>
@@ -145,6 +436,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="U6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Unit Test 1</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -209,7 +524,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="62">
   <si>
     <t>S.NO</t>
   </si>
@@ -596,7 +911,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -638,6 +953,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1022,7 +1340,7 @@
   <dimension ref="A1:AE56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1036,61 +1354,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:31" ht="19.5">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:31" ht="18.75">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1147,7 +1465,9 @@
       <c r="T4" s="27">
         <v>9</v>
       </c>
-      <c r="U4" s="12"/>
+      <c r="U4" s="12">
+        <v>9</v>
+      </c>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
@@ -1160,8 +1480,8 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="1:31">
-      <c r="A5" s="36"/>
-      <c r="B5" s="38"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -1216,7 +1536,9 @@
       <c r="T5" s="27">
         <v>25</v>
       </c>
-      <c r="U5" s="12"/>
+      <c r="U5" s="12">
+        <v>26</v>
+      </c>
       <c r="V5" s="12"/>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
@@ -1229,8 +1551,8 @@
       <c r="AE5" s="12"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -1285,7 +1607,9 @@
       <c r="T6" s="27">
         <v>2</v>
       </c>
-      <c r="U6" s="12"/>
+      <c r="U6" s="12">
+        <v>5</v>
+      </c>
       <c r="V6" s="12"/>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
@@ -1356,7 +1680,9 @@
       <c r="T7" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U7" s="12"/>
+      <c r="U7" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
@@ -1427,7 +1753,9 @@
       <c r="T8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U8" s="12"/>
+      <c r="U8" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
@@ -1498,7 +1826,9 @@
       <c r="T9" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U9" s="12"/>
+      <c r="U9" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
@@ -1569,7 +1899,9 @@
       <c r="T10" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U10" s="12"/>
+      <c r="U10" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
@@ -1640,7 +1972,9 @@
       <c r="T11" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U11" s="12"/>
+      <c r="U11" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
@@ -1711,7 +2045,9 @@
       <c r="T12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U12" s="12"/>
+      <c r="U12" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
@@ -1782,7 +2118,9 @@
       <c r="T13" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U13" s="12"/>
+      <c r="U13" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
@@ -1853,7 +2191,9 @@
       <c r="T14" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U14" s="12"/>
+      <c r="U14" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
@@ -1924,7 +2264,9 @@
       <c r="T15" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U15" s="12"/>
+      <c r="U15" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
@@ -1995,7 +2337,9 @@
       <c r="T16" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U16" s="12"/>
+      <c r="U16" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
@@ -2066,7 +2410,9 @@
       <c r="T17" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U17" s="12"/>
+      <c r="U17" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
@@ -2137,7 +2483,9 @@
       <c r="T18" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U18" s="12"/>
+      <c r="U18" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
@@ -2208,7 +2556,9 @@
       <c r="T19" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U19" s="12"/>
+      <c r="U19" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
@@ -2279,7 +2629,9 @@
       <c r="T20" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U20" s="12"/>
+      <c r="U20" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
@@ -2350,7 +2702,9 @@
       <c r="T21" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U21" s="12"/>
+      <c r="U21" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V21" s="12"/>
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
@@ -2421,7 +2775,9 @@
       <c r="T22" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U22" s="12"/>
+      <c r="U22" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V22" s="12"/>
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
@@ -2492,7 +2848,9 @@
       <c r="T23" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U23" s="12"/>
+      <c r="U23" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V23" s="12"/>
       <c r="W23" s="12"/>
       <c r="X23" s="12"/>
@@ -2563,7 +2921,9 @@
       <c r="T24" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U24" s="12"/>
+      <c r="U24" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V24" s="12"/>
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
@@ -2634,7 +2994,9 @@
       <c r="T25" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U25" s="12"/>
+      <c r="U25" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V25" s="12"/>
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
@@ -2705,7 +3067,9 @@
       <c r="T26" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U26" s="12"/>
+      <c r="U26" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V26" s="12"/>
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
@@ -2776,7 +3140,9 @@
       <c r="T27" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U27" s="12"/>
+      <c r="U27" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V27" s="12"/>
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
@@ -2847,7 +3213,9 @@
       <c r="T28" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U28" s="12"/>
+      <c r="U28" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V28" s="12"/>
       <c r="W28" s="12"/>
       <c r="X28" s="12"/>
@@ -2918,7 +3286,9 @@
       <c r="T29" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U29" s="12"/>
+      <c r="U29" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V29" s="12"/>
       <c r="W29" s="12"/>
       <c r="X29" s="12"/>
@@ -2989,7 +3359,9 @@
       <c r="T30" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U30" s="12"/>
+      <c r="U30" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V30" s="12"/>
       <c r="W30" s="12"/>
       <c r="X30" s="12"/>
@@ -3060,7 +3432,9 @@
       <c r="T31" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U31" s="12"/>
+      <c r="U31" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V31" s="12"/>
       <c r="W31" s="12"/>
       <c r="X31" s="12"/>
@@ -3131,7 +3505,9 @@
       <c r="T32" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U32" s="12"/>
+      <c r="U32" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V32" s="12"/>
       <c r="W32" s="12"/>
       <c r="X32" s="12"/>
@@ -3202,7 +3578,9 @@
       <c r="T33" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U33" s="12"/>
+      <c r="U33" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V33" s="12"/>
       <c r="W33" s="12"/>
       <c r="X33" s="12"/>
@@ -3273,7 +3651,9 @@
       <c r="T34" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U34" s="12"/>
+      <c r="U34" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V34" s="12"/>
       <c r="W34" s="12"/>
       <c r="X34" s="12"/>
@@ -3344,7 +3724,9 @@
       <c r="T35" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U35" s="12"/>
+      <c r="U35" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V35" s="12"/>
       <c r="W35" s="12"/>
       <c r="X35" s="12"/>
@@ -3415,7 +3797,9 @@
       <c r="T36" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U36" s="12"/>
+      <c r="U36" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V36" s="12"/>
       <c r="W36" s="12"/>
       <c r="X36" s="12"/>
@@ -3486,7 +3870,9 @@
       <c r="T37" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U37" s="12"/>
+      <c r="U37" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V37" s="12"/>
       <c r="W37" s="12"/>
       <c r="X37" s="12"/>
@@ -3557,7 +3943,9 @@
       <c r="T38" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U38" s="12"/>
+      <c r="U38" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V38" s="12"/>
       <c r="W38" s="12"/>
       <c r="X38" s="12"/>
@@ -3628,7 +4016,9 @@
       <c r="T39" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U39" s="12"/>
+      <c r="U39" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
       <c r="X39" s="12"/>
@@ -3699,7 +4089,9 @@
       <c r="T40" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U40" s="12"/>
+      <c r="U40" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V40" s="12"/>
       <c r="W40" s="12"/>
       <c r="X40" s="12"/>
@@ -3770,7 +4162,9 @@
       <c r="T41" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U41" s="12"/>
+      <c r="U41" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V41" s="12"/>
       <c r="W41" s="12"/>
       <c r="X41" s="12"/>
@@ -3841,7 +4235,9 @@
       <c r="T42" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U42" s="12"/>
+      <c r="U42" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V42" s="12"/>
       <c r="W42" s="12"/>
       <c r="X42" s="12"/>
@@ -3912,7 +4308,9 @@
       <c r="T43" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U43" s="12"/>
+      <c r="U43" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V43" s="12"/>
       <c r="W43" s="12"/>
       <c r="X43" s="12"/>
@@ -3983,7 +4381,9 @@
       <c r="T44" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U44" s="12"/>
+      <c r="U44" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V44" s="12"/>
       <c r="W44" s="12"/>
       <c r="X44" s="12"/>
@@ -4054,7 +4454,9 @@
       <c r="T45" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U45" s="12"/>
+      <c r="U45" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V45" s="12"/>
       <c r="W45" s="12"/>
       <c r="X45" s="12"/>
@@ -4125,7 +4527,9 @@
       <c r="T46" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U46" s="12"/>
+      <c r="U46" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V46" s="12"/>
       <c r="W46" s="12"/>
       <c r="X46" s="12"/>
@@ -4196,7 +4600,9 @@
       <c r="T47" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U47" s="12"/>
+      <c r="U47" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V47" s="12"/>
       <c r="W47" s="12"/>
       <c r="X47" s="12"/>
@@ -4267,7 +4673,9 @@
       <c r="T48" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U48" s="12"/>
+      <c r="U48" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="V48" s="12"/>
       <c r="W48" s="12"/>
       <c r="X48" s="12"/>
@@ -4338,7 +4746,9 @@
       <c r="T49" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U49" s="12"/>
+      <c r="U49" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V49" s="12"/>
       <c r="W49" s="12"/>
       <c r="X49" s="12"/>
@@ -4409,7 +4819,9 @@
       <c r="T50" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U50" s="12"/>
+      <c r="U50" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V50" s="12"/>
       <c r="W50" s="12"/>
       <c r="X50" s="12"/>
@@ -4480,7 +4892,9 @@
       <c r="T51" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U51" s="12"/>
+      <c r="U51" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V51" s="12"/>
       <c r="W51" s="12"/>
       <c r="X51" s="12"/>
@@ -4551,7 +4965,9 @@
       <c r="T52" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U52" s="12"/>
+      <c r="U52" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V52" s="12"/>
       <c r="W52" s="12"/>
       <c r="X52" s="12"/>
@@ -4622,7 +5038,9 @@
       <c r="T53" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U53" s="12"/>
+      <c r="U53" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V53" s="12"/>
       <c r="W53" s="12"/>
       <c r="X53" s="12"/>
@@ -4693,7 +5111,9 @@
       <c r="T54" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="U54" s="12"/>
+      <c r="U54" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="V54" s="12"/>
       <c r="W54" s="12"/>
       <c r="X54" s="12"/>
@@ -4706,10 +5126,10 @@
       <c r="AE54" s="12"/>
     </row>
     <row r="55" spans="1:31">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="35"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="13"/>
       <c r="D55" s="12">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -4781,7 +5201,7 @@
       </c>
       <c r="U55" s="12">
         <f t="shared" ref="U55" si="15">COUNTIF(U7:U54,"A")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55" s="12">
         <f t="shared" ref="V55" si="16">COUNTIF(V7:V54,"A")</f>
@@ -4825,10 +5245,10 @@
       </c>
     </row>
     <row r="56" spans="1:31">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>(48-D55)</f>
@@ -4900,7 +5320,7 @@
       </c>
       <c r="U56" s="24">
         <f t="shared" si="26"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V56" s="24">
         <f t="shared" si="26"/>
@@ -4979,61 +5399,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
       <c r="D2" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -5086,8 +5506,8 @@
       <c r="AF4" s="19"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="36"/>
-      <c r="B5" s="38"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -5138,8 +5558,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="36"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -7782,10 +8202,10 @@
       <c r="AF54" s="19"/>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="35"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="13"/>
       <c r="D55" s="19">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -7905,10 +8325,10 @@
       </c>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>(48-D55)</f>

</xml_diff>

<commit_message>
Last Update 27-09-2018 18:28:11.45
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="16605" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="16605" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
     <sheet name="Lab Attendance" sheetId="4" r:id="rId2"/>
+    <sheet name="Lab Attendance (2)" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$Q$1:$Q$56</definedName>
@@ -524,7 +525,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="63">
   <si>
     <t>S.NO</t>
   </si>
@@ -711,6 +712,9 @@
   <si>
     <t>Absent</t>
   </si>
+  <si>
+    <t>U1</t>
+  </si>
 </sst>
 </file>
 
@@ -810,7 +814,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -907,11 +911,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -953,6 +966,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1043,11 +1062,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -1339,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1354,61 +1398,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:31" ht="19.5">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:31" ht="18.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="40" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1468,7 +1512,9 @@
       <c r="U4" s="12">
         <v>9</v>
       </c>
-      <c r="V4" s="12"/>
+      <c r="V4" s="12">
+        <v>9</v>
+      </c>
       <c r="W4" s="12"/>
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
@@ -1480,8 +1526,8 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="1:31">
-      <c r="A5" s="37"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -1539,7 +1585,9 @@
       <c r="U5" s="12">
         <v>26</v>
       </c>
-      <c r="V5" s="12"/>
+      <c r="V5" s="12">
+        <v>27</v>
+      </c>
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
@@ -1551,8 +1599,8 @@
       <c r="AE5" s="12"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -1610,7 +1658,9 @@
       <c r="U6" s="12">
         <v>5</v>
       </c>
-      <c r="V6" s="12"/>
+      <c r="V6" s="12">
+        <v>5</v>
+      </c>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
@@ -1683,7 +1733,9 @@
       <c r="U7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V7" s="12"/>
+      <c r="V7" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
@@ -1756,7 +1808,9 @@
       <c r="U8" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V8" s="12"/>
+      <c r="V8" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
@@ -1829,7 +1883,9 @@
       <c r="U9" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V9" s="12"/>
+      <c r="V9" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
@@ -1902,7 +1958,9 @@
       <c r="U10" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V10" s="12"/>
+      <c r="V10" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
@@ -1975,7 +2033,9 @@
       <c r="U11" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V11" s="12"/>
+      <c r="V11" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
@@ -2048,7 +2108,9 @@
       <c r="U12" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V12" s="12"/>
+      <c r="V12" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
@@ -2121,7 +2183,9 @@
       <c r="U13" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V13" s="12"/>
+      <c r="V13" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
@@ -2194,7 +2258,9 @@
       <c r="U14" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V14" s="12"/>
+      <c r="V14" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
@@ -2267,7 +2333,9 @@
       <c r="U15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V15" s="12"/>
+      <c r="V15" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
@@ -2340,7 +2408,9 @@
       <c r="U16" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V16" s="12"/>
+      <c r="V16" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
@@ -2413,7 +2483,9 @@
       <c r="U17" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V17" s="12"/>
+      <c r="V17" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
@@ -2486,7 +2558,9 @@
       <c r="U18" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V18" s="12"/>
+      <c r="V18" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
@@ -2559,7 +2633,9 @@
       <c r="U19" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V19" s="12"/>
+      <c r="V19" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
@@ -2632,7 +2708,9 @@
       <c r="U20" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V20" s="12"/>
+      <c r="V20" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
@@ -2705,7 +2783,9 @@
       <c r="U21" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V21" s="12"/>
+      <c r="V21" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
@@ -2778,7 +2858,9 @@
       <c r="U22" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V22" s="12"/>
+      <c r="V22" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
@@ -2851,7 +2933,9 @@
       <c r="U23" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V23" s="12"/>
+      <c r="V23" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W23" s="12"/>
       <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
@@ -2924,7 +3008,9 @@
       <c r="U24" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V24" s="12"/>
+      <c r="V24" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
@@ -2997,7 +3083,9 @@
       <c r="U25" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V25" s="12"/>
+      <c r="V25" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
@@ -3070,7 +3158,9 @@
       <c r="U26" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V26" s="12"/>
+      <c r="V26" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
@@ -3143,7 +3233,9 @@
       <c r="U27" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V27" s="12"/>
+      <c r="V27" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
       <c r="Y27" s="12"/>
@@ -3216,7 +3308,9 @@
       <c r="U28" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V28" s="12"/>
+      <c r="V28" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W28" s="12"/>
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
@@ -3289,7 +3383,9 @@
       <c r="U29" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V29" s="12"/>
+      <c r="V29" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W29" s="12"/>
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
@@ -3362,7 +3458,9 @@
       <c r="U30" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V30" s="12"/>
+      <c r="V30" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W30" s="12"/>
       <c r="X30" s="12"/>
       <c r="Y30" s="12"/>
@@ -3435,7 +3533,9 @@
       <c r="U31" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V31" s="12"/>
+      <c r="V31" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W31" s="12"/>
       <c r="X31" s="12"/>
       <c r="Y31" s="12"/>
@@ -3508,7 +3608,9 @@
       <c r="U32" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V32" s="12"/>
+      <c r="V32" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W32" s="12"/>
       <c r="X32" s="12"/>
       <c r="Y32" s="12"/>
@@ -3581,7 +3683,9 @@
       <c r="U33" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V33" s="12"/>
+      <c r="V33" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W33" s="12"/>
       <c r="X33" s="12"/>
       <c r="Y33" s="12"/>
@@ -3654,7 +3758,9 @@
       <c r="U34" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V34" s="12"/>
+      <c r="V34" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W34" s="12"/>
       <c r="X34" s="12"/>
       <c r="Y34" s="12"/>
@@ -3727,7 +3833,9 @@
       <c r="U35" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V35" s="12"/>
+      <c r="V35" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W35" s="12"/>
       <c r="X35" s="12"/>
       <c r="Y35" s="12"/>
@@ -3800,7 +3908,9 @@
       <c r="U36" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V36" s="12"/>
+      <c r="V36" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W36" s="12"/>
       <c r="X36" s="12"/>
       <c r="Y36" s="12"/>
@@ -3873,7 +3983,9 @@
       <c r="U37" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V37" s="12"/>
+      <c r="V37" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W37" s="12"/>
       <c r="X37" s="12"/>
       <c r="Y37" s="12"/>
@@ -3946,7 +4058,9 @@
       <c r="U38" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V38" s="12"/>
+      <c r="V38" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W38" s="12"/>
       <c r="X38" s="12"/>
       <c r="Y38" s="12"/>
@@ -4019,7 +4133,9 @@
       <c r="U39" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V39" s="12"/>
+      <c r="V39" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W39" s="12"/>
       <c r="X39" s="12"/>
       <c r="Y39" s="12"/>
@@ -4092,7 +4208,9 @@
       <c r="U40" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V40" s="12"/>
+      <c r="V40" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W40" s="12"/>
       <c r="X40" s="12"/>
       <c r="Y40" s="12"/>
@@ -4165,7 +4283,9 @@
       <c r="U41" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V41" s="12"/>
+      <c r="V41" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W41" s="12"/>
       <c r="X41" s="12"/>
       <c r="Y41" s="12"/>
@@ -4238,7 +4358,9 @@
       <c r="U42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V42" s="12"/>
+      <c r="V42" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W42" s="12"/>
       <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
@@ -4311,7 +4433,9 @@
       <c r="U43" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V43" s="12"/>
+      <c r="V43" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W43" s="12"/>
       <c r="X43" s="12"/>
       <c r="Y43" s="12"/>
@@ -4384,7 +4508,9 @@
       <c r="U44" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V44" s="12"/>
+      <c r="V44" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W44" s="12"/>
       <c r="X44" s="12"/>
       <c r="Y44" s="12"/>
@@ -4457,7 +4583,9 @@
       <c r="U45" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V45" s="12"/>
+      <c r="V45" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W45" s="12"/>
       <c r="X45" s="12"/>
       <c r="Y45" s="12"/>
@@ -4530,7 +4658,9 @@
       <c r="U46" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V46" s="12"/>
+      <c r="V46" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W46" s="12"/>
       <c r="X46" s="12"/>
       <c r="Y46" s="12"/>
@@ -4603,7 +4733,9 @@
       <c r="U47" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V47" s="12"/>
+      <c r="V47" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W47" s="12"/>
       <c r="X47" s="12"/>
       <c r="Y47" s="12"/>
@@ -4676,7 +4808,9 @@
       <c r="U48" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="V48" s="12"/>
+      <c r="V48" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="W48" s="12"/>
       <c r="X48" s="12"/>
       <c r="Y48" s="12"/>
@@ -4749,7 +4883,9 @@
       <c r="U49" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V49" s="12"/>
+      <c r="V49" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W49" s="12"/>
       <c r="X49" s="12"/>
       <c r="Y49" s="12"/>
@@ -4822,7 +4958,9 @@
       <c r="U50" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V50" s="12"/>
+      <c r="V50" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W50" s="12"/>
       <c r="X50" s="12"/>
       <c r="Y50" s="12"/>
@@ -4895,7 +5033,9 @@
       <c r="U51" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V51" s="12"/>
+      <c r="V51" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W51" s="12"/>
       <c r="X51" s="12"/>
       <c r="Y51" s="12"/>
@@ -4968,7 +5108,9 @@
       <c r="U52" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V52" s="12"/>
+      <c r="V52" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W52" s="12"/>
       <c r="X52" s="12"/>
       <c r="Y52" s="12"/>
@@ -5041,7 +5183,9 @@
       <c r="U53" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V53" s="12"/>
+      <c r="V53" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W53" s="12"/>
       <c r="X53" s="12"/>
       <c r="Y53" s="12"/>
@@ -5114,7 +5258,9 @@
       <c r="U54" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="V54" s="12"/>
+      <c r="V54" s="29" t="s">
+        <v>54</v>
+      </c>
       <c r="W54" s="12"/>
       <c r="X54" s="12"/>
       <c r="Y54" s="12"/>
@@ -5126,10 +5272,10 @@
       <c r="AE54" s="12"/>
     </row>
     <row r="55" spans="1:31">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="36"/>
+      <c r="B55" s="38"/>
       <c r="C55" s="13"/>
       <c r="D55" s="12">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -5205,7 +5351,7 @@
       </c>
       <c r="V55" s="12">
         <f t="shared" ref="V55" si="16">COUNTIF(V7:V54,"A")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W55" s="12">
         <f t="shared" ref="W55" si="17">COUNTIF(W7:W54,"A")</f>
@@ -5245,10 +5391,10 @@
       </c>
     </row>
     <row r="56" spans="1:31">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="30"/>
+      <c r="B56" s="32"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>(48-D55)</f>
@@ -5324,7 +5470,7 @@
       </c>
       <c r="V56" s="24">
         <f t="shared" si="26"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="W56" s="24">
         <f t="shared" si="26"/>
@@ -5399,61 +5545,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="40" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -5506,8 +5652,8 @@
       <c r="AF4" s="19"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="37"/>
-      <c r="B5" s="39"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -5558,8 +5704,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -8202,10 +8348,10 @@
       <c r="AF54" s="19"/>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="36"/>
+      <c r="B55" s="38"/>
       <c r="C55" s="13"/>
       <c r="D55" s="19">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -8325,10 +8471,10 @@
       </c>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="30"/>
+      <c r="B56" s="32"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>(48-D55)</f>
@@ -8463,4 +8609,757 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="2"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75">
+      <c r="A1" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+    </row>
+    <row r="2" spans="1:7" ht="19.5">
+      <c r="A2" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75">
+      <c r="A3" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="44"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="39"/>
+      <c r="B5" s="41"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="30">
+        <v>30</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="30">
+        <v>33</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="30">
+        <v>29</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
+      <c r="A10" s="3">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="30">
+        <v>26</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="30">
+        <v>29</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1">
+      <c r="A12" s="3">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="30">
+        <v>13</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1">
+      <c r="A13" s="3">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="30">
+        <v>33</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1">
+      <c r="A14" s="3">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="30">
+        <v>28</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1">
+      <c r="A15" s="3">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="30">
+        <v>31</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1">
+      <c r="A16" s="3">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="30">
+        <v>17</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="30">
+        <v>27</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="30">
+        <v>21</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1">
+      <c r="A19" s="3">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="30">
+        <v>33</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1">
+      <c r="A20" s="3">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="30">
+        <v>29</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1">
+      <c r="A21" s="3">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="30">
+        <v>16</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1">
+      <c r="A22" s="3">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1">
+      <c r="A23" s="3">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1">
+      <c r="A24" s="3">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1">
+      <c r="A25" s="3">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1">
+      <c r="A26" s="3">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1">
+      <c r="A27" s="3">
+        <v>21</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1">
+      <c r="A28" s="3">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1">
+      <c r="A29" s="3">
+        <v>23</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1">
+      <c r="A30" s="3">
+        <v>24</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1">
+      <c r="A31" s="3">
+        <v>25</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1">
+      <c r="A32" s="3">
+        <v>26</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1">
+      <c r="A33" s="3">
+        <v>27</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1">
+      <c r="A34" s="3">
+        <v>28</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="13"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1">
+      <c r="A35" s="3">
+        <v>29</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="13"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1">
+      <c r="A36" s="3">
+        <v>30</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="13"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1">
+      <c r="A37" s="3">
+        <v>31</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1">
+      <c r="A38" s="3">
+        <v>32</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1">
+      <c r="A39" s="3">
+        <v>33</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1">
+      <c r="A40" s="3">
+        <v>34</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1">
+      <c r="A41" s="3">
+        <v>35</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" ht="15" customHeight="1">
+      <c r="A42" s="3">
+        <v>36</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="1:7" ht="15" customHeight="1">
+      <c r="A43" s="3">
+        <v>37</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" ht="15" customHeight="1">
+      <c r="A44" s="3">
+        <v>38</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1">
+      <c r="A45" s="3">
+        <v>39</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="13"/>
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1">
+      <c r="A46" s="3">
+        <v>40</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" spans="1:7" ht="15" customHeight="1">
+      <c r="A47" s="3">
+        <v>41</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1">
+      <c r="A48" s="3">
+        <v>42</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" customHeight="1">
+      <c r="A49" s="3">
+        <v>43</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="13"/>
+    </row>
+    <row r="50" spans="1:7" ht="15" customHeight="1">
+      <c r="A50" s="3">
+        <v>44</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="13"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" customHeight="1">
+      <c r="A51" s="3">
+        <v>45</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="13"/>
+    </row>
+    <row r="52" spans="1:7" ht="15" customHeight="1">
+      <c r="A52" s="3">
+        <v>46</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="13"/>
+    </row>
+    <row r="53" spans="1:7" ht="15" customHeight="1">
+      <c r="A53" s="3">
+        <v>47</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="1:7" ht="15" customHeight="1">
+      <c r="A54" s="3">
+        <v>48</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="38"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C7:C54">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Last Update 28-09-2018  8:39:08.51
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="16605" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -1066,6 +1066,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1111,6 +1123,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1122,39 +1155,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1465,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+    <sheetView topLeftCell="C37" workbookViewId="0">
       <selection activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
@@ -1480,61 +1480,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="47" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1602,13 +1602,13 @@
       <c r="AC4" s="12"/>
       <c r="AD4" s="12"/>
       <c r="AE4" s="12"/>
-      <c r="AF4" s="60" t="s">
+      <c r="AF4" s="37" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="42"/>
-      <c r="B5" s="44"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -1674,11 +1674,11 @@
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
       <c r="AE5" s="12"/>
-      <c r="AF5" s="60"/>
+      <c r="AF5" s="37"/>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -1745,7 +1745,7 @@
       <c r="AD6" s="12"/>
       <c r="AE6" s="12"/>
       <c r="AF6" s="32">
-        <f>COUNTIF(D7:AE7,"A")</f>
+        <f t="shared" ref="AF6:AF37" si="0">COUNTIF(D7:AE7,"A")</f>
         <v>3</v>
       </c>
     </row>
@@ -1820,7 +1820,7 @@
       <c r="AD7" s="12"/>
       <c r="AE7" s="12"/>
       <c r="AF7" s="32">
-        <f>COUNTIF(D8:AE8,"A")</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
       <c r="AD8" s="12"/>
       <c r="AE8" s="12"/>
       <c r="AF8" s="32">
-        <f>COUNTIF(D9:AE9,"A")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       <c r="AD9" s="12"/>
       <c r="AE9" s="12"/>
       <c r="AF9" s="32">
-        <f>COUNTIF(D10:AE10,"A")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       <c r="AD10" s="12"/>
       <c r="AE10" s="12"/>
       <c r="AF10" s="32">
-        <f>COUNTIF(D11:AE11,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2120,7 +2120,7 @@
       <c r="AD11" s="12"/>
       <c r="AE11" s="12"/>
       <c r="AF11" s="32">
-        <f>COUNTIF(D12:AE12,"A")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       <c r="AD12" s="12"/>
       <c r="AE12" s="12"/>
       <c r="AF12" s="32">
-        <f>COUNTIF(D13:AE13,"A")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2270,7 +2270,7 @@
       <c r="AD13" s="12"/>
       <c r="AE13" s="12"/>
       <c r="AF13" s="32">
-        <f>COUNTIF(D14:AE14,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2345,7 +2345,7 @@
       <c r="AD14" s="12"/>
       <c r="AE14" s="12"/>
       <c r="AF14" s="32">
-        <f>COUNTIF(D15:AE15,"A")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2420,7 +2420,7 @@
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
       <c r="AF15" s="32">
-        <f>COUNTIF(D16:AE16,"A")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -2495,7 +2495,7 @@
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
       <c r="AF16" s="32">
-        <f>COUNTIF(D17:AE17,"A")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2570,7 +2570,7 @@
       <c r="AD17" s="12"/>
       <c r="AE17" s="12"/>
       <c r="AF17" s="32">
-        <f>COUNTIF(D18:AE18,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2645,7 +2645,7 @@
       <c r="AD18" s="12"/>
       <c r="AE18" s="12"/>
       <c r="AF18" s="32">
-        <f>COUNTIF(D19:AE19,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2720,7 +2720,7 @@
       <c r="AD19" s="12"/>
       <c r="AE19" s="12"/>
       <c r="AF19" s="32">
-        <f>COUNTIF(D20:AE20,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2795,7 +2795,7 @@
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
       <c r="AF20" s="32">
-        <f>COUNTIF(D21:AE21,"A")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -2870,7 +2870,7 @@
       <c r="AD21" s="12"/>
       <c r="AE21" s="12"/>
       <c r="AF21" s="32">
-        <f>COUNTIF(D22:AE22,"A")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -2945,7 +2945,7 @@
       <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="32">
-        <f>COUNTIF(D23:AE23,"A")</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -3020,7 +3020,7 @@
       <c r="AD23" s="12"/>
       <c r="AE23" s="12"/>
       <c r="AF23" s="32">
-        <f>COUNTIF(D24:AE24,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3095,7 +3095,7 @@
       <c r="AD24" s="12"/>
       <c r="AE24" s="12"/>
       <c r="AF24" s="32">
-        <f>COUNTIF(D25:AE25,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3170,7 +3170,7 @@
       <c r="AD25" s="12"/>
       <c r="AE25" s="12"/>
       <c r="AF25" s="32">
-        <f>COUNTIF(D26:AE26,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       <c r="AD26" s="12"/>
       <c r="AE26" s="12"/>
       <c r="AF26" s="32">
-        <f>COUNTIF(D27:AE27,"A")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3320,7 +3320,7 @@
       <c r="AD27" s="12"/>
       <c r="AE27" s="12"/>
       <c r="AF27" s="32">
-        <f>COUNTIF(D28:AE28,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3395,7 +3395,7 @@
       <c r="AD28" s="12"/>
       <c r="AE28" s="12"/>
       <c r="AF28" s="32">
-        <f>COUNTIF(D29:AE29,"A")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3470,7 +3470,7 @@
       <c r="AD29" s="12"/>
       <c r="AE29" s="12"/>
       <c r="AF29" s="32">
-        <f>COUNTIF(D30:AE30,"A")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3545,7 +3545,7 @@
       <c r="AD30" s="12"/>
       <c r="AE30" s="12"/>
       <c r="AF30" s="32">
-        <f>COUNTIF(D31:AE31,"A")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3620,7 +3620,7 @@
       <c r="AD31" s="12"/>
       <c r="AE31" s="12"/>
       <c r="AF31" s="32">
-        <f>COUNTIF(D32:AE32,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3695,7 +3695,7 @@
       <c r="AD32" s="12"/>
       <c r="AE32" s="12"/>
       <c r="AF32" s="32">
-        <f>COUNTIF(D33:AE33,"A")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -3770,7 +3770,7 @@
       <c r="AD33" s="12"/>
       <c r="AE33" s="12"/>
       <c r="AF33" s="32">
-        <f>COUNTIF(D34:AE34,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3845,7 +3845,7 @@
       <c r="AD34" s="12"/>
       <c r="AE34" s="12"/>
       <c r="AF34" s="32">
-        <f>COUNTIF(D35:AE35,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -3920,7 +3920,7 @@
       <c r="AD35" s="12"/>
       <c r="AE35" s="12"/>
       <c r="AF35" s="32">
-        <f>COUNTIF(D36:AE36,"A")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -3995,7 +3995,7 @@
       <c r="AD36" s="12"/>
       <c r="AE36" s="12"/>
       <c r="AF36" s="32">
-        <f>COUNTIF(D37:AE37,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4070,7 +4070,7 @@
       <c r="AD37" s="12"/>
       <c r="AE37" s="12"/>
       <c r="AF37" s="32">
-        <f>COUNTIF(D38:AE38,"A")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4145,7 +4145,7 @@
       <c r="AD38" s="12"/>
       <c r="AE38" s="12"/>
       <c r="AF38" s="32">
-        <f>COUNTIF(D39:AE39,"A")</f>
+        <f t="shared" ref="AF38:AF54" si="1">COUNTIF(D39:AE39,"A")</f>
         <v>1</v>
       </c>
     </row>
@@ -4220,7 +4220,7 @@
       <c r="AD39" s="12"/>
       <c r="AE39" s="12"/>
       <c r="AF39" s="32">
-        <f>COUNTIF(D40:AE40,"A")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4295,7 +4295,7 @@
       <c r="AD40" s="12"/>
       <c r="AE40" s="12"/>
       <c r="AF40" s="32">
-        <f>COUNTIF(D41:AE41,"A")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4370,7 +4370,7 @@
       <c r="AD41" s="12"/>
       <c r="AE41" s="12"/>
       <c r="AF41" s="32">
-        <f>COUNTIF(D42:AE42,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4445,7 +4445,7 @@
       <c r="AD42" s="12"/>
       <c r="AE42" s="12"/>
       <c r="AF42" s="32">
-        <f>COUNTIF(D43:AE43,"A")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4520,7 +4520,7 @@
       <c r="AD43" s="12"/>
       <c r="AE43" s="12"/>
       <c r="AF43" s="32">
-        <f>COUNTIF(D44:AE44,"A")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4595,7 +4595,7 @@
       <c r="AD44" s="12"/>
       <c r="AE44" s="12"/>
       <c r="AF44" s="32">
-        <f>COUNTIF(D45:AE45,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4670,7 +4670,7 @@
       <c r="AD45" s="12"/>
       <c r="AE45" s="12"/>
       <c r="AF45" s="32">
-        <f>COUNTIF(D46:AE46,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4745,7 +4745,7 @@
       <c r="AD46" s="12"/>
       <c r="AE46" s="12"/>
       <c r="AF46" s="32">
-        <f>COUNTIF(D47:AE47,"A")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4820,7 +4820,7 @@
       <c r="AD47" s="12"/>
       <c r="AE47" s="12"/>
       <c r="AF47" s="32">
-        <f>COUNTIF(D48:AE48,"A")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4895,7 +4895,7 @@
       <c r="AD48" s="12"/>
       <c r="AE48" s="12"/>
       <c r="AF48" s="32">
-        <f>COUNTIF(D49:AE49,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4970,7 +4970,7 @@
       <c r="AD49" s="12"/>
       <c r="AE49" s="12"/>
       <c r="AF49" s="32">
-        <f>COUNTIF(D50:AE50,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5045,7 +5045,7 @@
       <c r="AD50" s="12"/>
       <c r="AE50" s="12"/>
       <c r="AF50" s="32">
-        <f>COUNTIF(D51:AE51,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5120,7 +5120,7 @@
       <c r="AD51" s="12"/>
       <c r="AE51" s="12"/>
       <c r="AF51" s="32">
-        <f>COUNTIF(D52:AE52,"A")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5195,7 +5195,7 @@
       <c r="AD52" s="12"/>
       <c r="AE52" s="12"/>
       <c r="AF52" s="32">
-        <f>COUNTIF(D53:AE53,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5270,7 +5270,7 @@
       <c r="AD53" s="12"/>
       <c r="AE53" s="12"/>
       <c r="AF53" s="32">
-        <f>COUNTIF(D54:AE54,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -5345,245 +5345,245 @@
       <c r="AD54" s="12"/>
       <c r="AE54" s="12"/>
       <c r="AF54" s="32">
-        <f>COUNTIF(D55:AE55,"A")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:32">
-      <c r="A55" s="40" t="s">
+      <c r="A55" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="41"/>
+      <c r="B55" s="45"/>
       <c r="C55" s="13"/>
       <c r="D55" s="12">
         <f>COUNTIF(D7:D54,"A")</f>
         <v>0</v>
       </c>
       <c r="E55" s="12">
-        <f t="shared" ref="E55:F55" si="0">COUNTIF(E7:E54,"A")</f>
+        <f t="shared" ref="E55:F55" si="2">COUNTIF(E7:E54,"A")</f>
         <v>0</v>
       </c>
       <c r="F55" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G55" s="12">
-        <f t="shared" ref="G55" si="1">COUNTIF(G7:G54,"A")</f>
+        <f t="shared" ref="G55" si="3">COUNTIF(G7:G54,"A")</f>
         <v>2</v>
       </c>
       <c r="H55" s="12">
-        <f t="shared" ref="H55" si="2">COUNTIF(H7:H54,"A")</f>
+        <f t="shared" ref="H55" si="4">COUNTIF(H7:H54,"A")</f>
         <v>11</v>
       </c>
       <c r="I55" s="12">
-        <f t="shared" ref="I55" si="3">COUNTIF(I7:I54,"A")</f>
+        <f t="shared" ref="I55" si="5">COUNTIF(I7:I54,"A")</f>
         <v>11</v>
       </c>
       <c r="J55" s="12">
-        <f t="shared" ref="J55" si="4">COUNTIF(J7:J54,"A")</f>
+        <f t="shared" ref="J55" si="6">COUNTIF(J7:J54,"A")</f>
         <v>1</v>
       </c>
       <c r="K55" s="12">
-        <f t="shared" ref="K55" si="5">COUNTIF(K7:K54,"A")</f>
+        <f t="shared" ref="K55" si="7">COUNTIF(K7:K54,"A")</f>
         <v>1</v>
       </c>
       <c r="L55" s="12">
-        <f t="shared" ref="L55" si="6">COUNTIF(L7:L54,"A")</f>
+        <f t="shared" ref="L55" si="8">COUNTIF(L7:L54,"A")</f>
         <v>6</v>
       </c>
       <c r="M55" s="12">
-        <f t="shared" ref="M55" si="7">COUNTIF(M7:M54,"A")</f>
+        <f t="shared" ref="M55" si="9">COUNTIF(M7:M54,"A")</f>
         <v>11</v>
       </c>
       <c r="N55" s="12">
-        <f t="shared" ref="N55" si="8">COUNTIF(N7:N54,"A")</f>
+        <f t="shared" ref="N55" si="10">COUNTIF(N7:N54,"A")</f>
         <v>3</v>
       </c>
       <c r="O55" s="12">
-        <f t="shared" ref="O55" si="9">COUNTIF(O7:O54,"A")</f>
+        <f t="shared" ref="O55" si="11">COUNTIF(O7:O54,"A")</f>
         <v>1</v>
       </c>
       <c r="P55" s="12">
-        <f t="shared" ref="P55" si="10">COUNTIF(P7:P54,"A")</f>
+        <f t="shared" ref="P55" si="12">COUNTIF(P7:P54,"A")</f>
         <v>1</v>
       </c>
       <c r="Q55" s="12">
-        <f t="shared" ref="Q55" si="11">COUNTIF(Q7:Q54,"A")</f>
+        <f t="shared" ref="Q55" si="13">COUNTIF(Q7:Q54,"A")</f>
         <v>2</v>
       </c>
       <c r="R55" s="12">
-        <f t="shared" ref="R55:V55" si="12">COUNTIF(R7:R54,"A")</f>
+        <f t="shared" ref="R55:V55" si="14">COUNTIF(R7:R54,"A")</f>
         <v>3</v>
       </c>
       <c r="S55" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T55" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="U55" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="V55" s="32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="W55" s="12">
-        <f t="shared" ref="W55" si="13">COUNTIF(W7:W54,"A")</f>
+        <f t="shared" ref="W55" si="15">COUNTIF(W7:W54,"A")</f>
         <v>0</v>
       </c>
       <c r="X55" s="12">
-        <f t="shared" ref="X55" si="14">COUNTIF(X7:X54,"A")</f>
+        <f t="shared" ref="X55" si="16">COUNTIF(X7:X54,"A")</f>
         <v>0</v>
       </c>
       <c r="Y55" s="12">
-        <f t="shared" ref="Y55" si="15">COUNTIF(Y7:Y54,"A")</f>
+        <f t="shared" ref="Y55" si="17">COUNTIF(Y7:Y54,"A")</f>
         <v>0</v>
       </c>
       <c r="Z55" s="12">
-        <f t="shared" ref="Z55" si="16">COUNTIF(Z7:Z54,"A")</f>
+        <f t="shared" ref="Z55" si="18">COUNTIF(Z7:Z54,"A")</f>
         <v>0</v>
       </c>
       <c r="AA55" s="12">
-        <f t="shared" ref="AA55" si="17">COUNTIF(AA7:AA54,"A")</f>
+        <f t="shared" ref="AA55" si="19">COUNTIF(AA7:AA54,"A")</f>
         <v>0</v>
       </c>
       <c r="AB55" s="12">
-        <f t="shared" ref="AB55" si="18">COUNTIF(AB7:AB54,"A")</f>
+        <f t="shared" ref="AB55" si="20">COUNTIF(AB7:AB54,"A")</f>
         <v>0</v>
       </c>
       <c r="AC55" s="12">
-        <f t="shared" ref="AC55" si="19">COUNTIF(AC7:AC54,"A")</f>
+        <f t="shared" ref="AC55" si="21">COUNTIF(AC7:AC54,"A")</f>
         <v>0</v>
       </c>
       <c r="AD55" s="12">
-        <f t="shared" ref="AD55" si="20">COUNTIF(AD7:AD54,"A")</f>
+        <f t="shared" ref="AD55" si="22">COUNTIF(AD7:AD54,"A")</f>
         <v>0</v>
       </c>
       <c r="AE55" s="12">
-        <f t="shared" ref="AE55" si="21">COUNTIF(AE7:AE54,"A")</f>
+        <f t="shared" ref="AE55" si="23">COUNTIF(AE7:AE54,"A")</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="35"/>
+      <c r="B56" s="39"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>(48-D55)</f>
         <v>48</v>
       </c>
       <c r="E56" s="24">
-        <f t="shared" ref="E56:AE56" si="22">(48-E55)</f>
+        <f t="shared" ref="E56:AE56" si="24">(48-E55)</f>
         <v>48</v>
       </c>
       <c r="F56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="G56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>46</v>
       </c>
       <c r="H56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>37</v>
       </c>
       <c r="I56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>37</v>
       </c>
       <c r="J56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="K56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="L56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>42</v>
       </c>
       <c r="M56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>37</v>
       </c>
       <c r="N56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>45</v>
       </c>
       <c r="O56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="P56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="Q56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>46</v>
       </c>
       <c r="R56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>45</v>
       </c>
       <c r="S56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="T56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>47</v>
       </c>
       <c r="U56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="V56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="W56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="X56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="Y56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="Z56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="AA56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="AB56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="AC56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="AD56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
       <c r="AE56" s="24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>48</v>
       </c>
     </row>
@@ -5634,82 +5634,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="39"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
     </row>
     <row r="4" spans="1:32" ht="18.75">
       <c r="A4" s="33"/>
-      <c r="B4" s="52"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="33"/>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="57" t="s">
         <v>65</v>
       </c>
       <c r="I4" s="58"/>
       <c r="J4" s="58"/>
       <c r="K4" s="58"/>
-      <c r="L4" s="59" t="s">
+      <c r="L4" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="59"/>
+      <c r="M4" s="52"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="47" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -5766,8 +5766,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="42"/>
-      <c r="B6" s="44"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -5822,8 +5822,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1">
-      <c r="A7" s="42"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -8662,10 +8662,10 @@
       <c r="AF55" s="19"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="40" t="s">
+      <c r="A56" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="41"/>
+      <c r="B56" s="45"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -8785,10 +8785,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="35"/>
+      <c r="B57" s="39"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>(48-D56)</f>
@@ -8932,8 +8932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -8946,56 +8946,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:7" ht="19.5">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
     </row>
     <row r="3" spans="1:7" ht="18.75">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="36" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="42"/>
-      <c r="B5" s="44"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="48"/>
       <c r="C5" s="32" t="s">
         <v>62</v>
       </c>
@@ -9005,9 +9005,9 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
-      <c r="A6" s="42"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="61">
+      <c r="A6" s="46"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="35">
         <v>50</v>
       </c>
       <c r="D6" s="32"/>
@@ -9247,7 +9247,9 @@
       <c r="B22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="30"/>
+      <c r="C22" s="30">
+        <v>17</v>
+      </c>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
@@ -9734,10 +9736,10 @@
       <c r="G54" s="13"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="40" t="s">
+      <c r="A55" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="41"/>
+      <c r="B55" s="45"/>
       <c r="C55" s="32">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -9748,13 +9750,13 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="34" t="s">
+      <c r="A56" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="35"/>
+      <c r="B56" s="39"/>
       <c r="C56" s="32">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D56" s="32"/>
       <c r="E56" s="32"/>
@@ -9762,10 +9764,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="35"/>
+      <c r="B57" s="39"/>
       <c r="C57" s="32">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -9776,11 +9778,11 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="34" t="s">
+      <c r="A58" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="62">
+      <c r="B58" s="39"/>
+      <c r="C58" s="36">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>
       </c>

</xml_diff>

<commit_message>
Last Update 04-10-2018 11:23:41.48
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -412,6 +412,102 @@
         </r>
       </text>
     </comment>
+    <comment ref="T6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Unit Test Preparation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Introduction to Python Language and SetUp</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Values and Datatypes</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Tuples and Operators [Arithmetic, Relational]</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -422,6 +518,102 @@
     <author>Rajasekaran S</author>
   </authors>
   <commentList>
+    <comment ref="D4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Rajasekaran S:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Finding GCD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Squre root of Given number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Unit Test 1 Preparation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Exp of Number</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D6" authorId="0">
       <text>
         <r>
@@ -526,7 +718,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="72">
   <si>
     <t>S.NO</t>
   </si>
@@ -739,6 +931,9 @@
   </si>
   <si>
     <t>Pass Persentage</t>
+  </si>
+  <si>
+    <t>Lab 3</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1270,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1463,10 +1658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF56"/>
+  <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView topLeftCell="C37" workbookViewId="0">
-      <selection activeCell="AH26" sqref="AH26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1475,11 +1670,10 @@
     <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
     <col min="4" max="31" width="4.140625" style="2" customWidth="1"/>
-    <col min="32" max="32" width="19.42578125" style="2" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
+    <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="18.75">
+    <row r="1" spans="1:31" ht="18.75">
       <c r="A1" s="41" t="s">
         <v>53</v>
       </c>
@@ -1492,7 +1686,7 @@
       <c r="H1" s="42"/>
       <c r="I1" s="43"/>
     </row>
-    <row r="2" spans="1:32" ht="19.5">
+    <row r="2" spans="1:31" ht="19.5">
       <c r="A2" s="50" t="s">
         <v>51</v>
       </c>
@@ -1511,7 +1705,7 @@
       <c r="H2" s="40"/>
       <c r="I2" s="40"/>
     </row>
-    <row r="3" spans="1:32" ht="18.75">
+    <row r="3" spans="1:31" ht="18.75">
       <c r="A3" s="51" t="s">
         <v>52</v>
       </c>
@@ -1530,7 +1724,7 @@
       <c r="H3" s="40"/>
       <c r="I3" s="40"/>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:31">
       <c r="A4" s="46" t="s">
         <v>0</v>
       </c>
@@ -1591,9 +1785,15 @@
       <c r="T4" s="12">
         <v>9</v>
       </c>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="12"/>
+      <c r="U4" s="37">
+        <v>9</v>
+      </c>
+      <c r="V4" s="32">
+        <v>10</v>
+      </c>
+      <c r="W4" s="37">
+        <v>10</v>
+      </c>
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
@@ -1602,11 +1802,8 @@
       <c r="AC4" s="12"/>
       <c r="AD4" s="12"/>
       <c r="AE4" s="12"/>
-      <c r="AF4" s="37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32">
+    </row>
+    <row r="5" spans="1:31">
       <c r="A5" s="46"/>
       <c r="B5" s="48"/>
       <c r="C5" s="9" t="s">
@@ -1663,9 +1860,15 @@
       <c r="T5" s="12">
         <v>27</v>
       </c>
-      <c r="U5" s="32"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="12"/>
+      <c r="U5" s="37">
+        <v>28</v>
+      </c>
+      <c r="V5" s="32">
+        <v>1</v>
+      </c>
+      <c r="W5" s="37">
+        <v>3</v>
+      </c>
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
@@ -1674,9 +1877,8 @@
       <c r="AC5" s="12"/>
       <c r="AD5" s="12"/>
       <c r="AE5" s="12"/>
-      <c r="AF5" s="37"/>
-    </row>
-    <row r="6" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="6" spans="1:31" ht="15" customHeight="1">
       <c r="A6" s="46"/>
       <c r="B6" s="49"/>
       <c r="C6" s="10" t="s">
@@ -1733,9 +1935,15 @@
       <c r="T6" s="12">
         <v>5</v>
       </c>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="12"/>
+      <c r="U6" s="37">
+        <v>4</v>
+      </c>
+      <c r="V6" s="32">
+        <v>4</v>
+      </c>
+      <c r="W6" s="37">
+        <v>7</v>
+      </c>
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
@@ -1744,12 +1952,8 @@
       <c r="AC6" s="12"/>
       <c r="AD6" s="12"/>
       <c r="AE6" s="12"/>
-      <c r="AF6" s="32">
-        <f t="shared" ref="AF6:AF37" si="0">COUNTIF(D7:AE7,"A")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="7" spans="1:31" ht="15" customHeight="1">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -1808,9 +2012,15 @@
       <c r="T7" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="12"/>
+      <c r="U7" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W7" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
@@ -1819,12 +2029,8 @@
       <c r="AC7" s="12"/>
       <c r="AD7" s="12"/>
       <c r="AE7" s="12"/>
-      <c r="AF7" s="32">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="8" spans="1:31" ht="15" customHeight="1">
       <c r="A8" s="3">
         <v>2</v>
       </c>
@@ -1883,9 +2089,15 @@
       <c r="T8" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U8" s="32"/>
-      <c r="V8" s="32"/>
-      <c r="W8" s="12"/>
+      <c r="U8" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W8" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
@@ -1894,12 +2106,8 @@
       <c r="AC8" s="12"/>
       <c r="AD8" s="12"/>
       <c r="AE8" s="12"/>
-      <c r="AF8" s="32">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="9" spans="1:31" ht="15" customHeight="1">
       <c r="A9" s="3">
         <v>3</v>
       </c>
@@ -1958,9 +2166,15 @@
       <c r="T9" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="12"/>
+      <c r="U9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="V9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W9" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
@@ -1969,12 +2183,8 @@
       <c r="AC9" s="12"/>
       <c r="AD9" s="12"/>
       <c r="AE9" s="12"/>
-      <c r="AF9" s="32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="10" spans="1:31" ht="15" customHeight="1">
       <c r="A10" s="3">
         <v>4</v>
       </c>
@@ -2033,9 +2243,15 @@
       <c r="T10" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U10" s="32"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="12"/>
+      <c r="U10" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V10" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W10" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
@@ -2044,12 +2260,8 @@
       <c r="AC10" s="12"/>
       <c r="AD10" s="12"/>
       <c r="AE10" s="12"/>
-      <c r="AF10" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="11" spans="1:31" ht="15" customHeight="1">
       <c r="A11" s="3">
         <v>5</v>
       </c>
@@ -2108,9 +2320,15 @@
       <c r="T11" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U11" s="32"/>
-      <c r="V11" s="32"/>
-      <c r="W11" s="12"/>
+      <c r="U11" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V11" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W11" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
@@ -2119,12 +2337,8 @@
       <c r="AC11" s="12"/>
       <c r="AD11" s="12"/>
       <c r="AE11" s="12"/>
-      <c r="AF11" s="32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="12" spans="1:31" ht="15" customHeight="1">
       <c r="A12" s="3">
         <v>6</v>
       </c>
@@ -2183,9 +2397,15 @@
       <c r="T12" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U12" s="32"/>
-      <c r="V12" s="32"/>
-      <c r="W12" s="12"/>
+      <c r="U12" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V12" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W12" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
@@ -2194,12 +2414,8 @@
       <c r="AC12" s="12"/>
       <c r="AD12" s="12"/>
       <c r="AE12" s="12"/>
-      <c r="AF12" s="32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="13" spans="1:31" ht="15" customHeight="1">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -2258,9 +2474,15 @@
       <c r="T13" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="12"/>
+      <c r="U13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W13" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
@@ -2269,12 +2491,8 @@
       <c r="AC13" s="12"/>
       <c r="AD13" s="12"/>
       <c r="AE13" s="12"/>
-      <c r="AF13" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="14" spans="1:31" ht="15" customHeight="1">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -2333,9 +2551,15 @@
       <c r="T14" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="12"/>
+      <c r="U14" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V14" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W14" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
@@ -2344,12 +2568,8 @@
       <c r="AC14" s="12"/>
       <c r="AD14" s="12"/>
       <c r="AE14" s="12"/>
-      <c r="AF14" s="32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="15" spans="1:31" ht="15" customHeight="1">
       <c r="A15" s="3">
         <v>9</v>
       </c>
@@ -2408,9 +2628,15 @@
       <c r="T15" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U15" s="32"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="12"/>
+      <c r="U15" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V15" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W15" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
@@ -2419,12 +2645,8 @@
       <c r="AC15" s="12"/>
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
-      <c r="AF15" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="16" spans="1:31" ht="15" customHeight="1">
       <c r="A16" s="3">
         <v>10</v>
       </c>
@@ -2483,9 +2705,15 @@
       <c r="T16" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U16" s="32"/>
-      <c r="V16" s="32"/>
-      <c r="W16" s="12"/>
+      <c r="U16" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V16" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W16" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
@@ -2494,12 +2722,8 @@
       <c r="AC16" s="12"/>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
-      <c r="AF16" s="32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="17" spans="1:31" ht="15" customHeight="1">
       <c r="A17" s="3">
         <v>11</v>
       </c>
@@ -2558,9 +2782,15 @@
       <c r="T17" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U17" s="32"/>
-      <c r="V17" s="32"/>
-      <c r="W17" s="12"/>
+      <c r="U17" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W17" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
@@ -2569,12 +2799,8 @@
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
       <c r="AE17" s="12"/>
-      <c r="AF17" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="18" spans="1:31" ht="15" customHeight="1">
       <c r="A18" s="3">
         <v>12</v>
       </c>
@@ -2633,9 +2859,15 @@
       <c r="T18" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U18" s="32"/>
-      <c r="V18" s="32"/>
-      <c r="W18" s="12"/>
+      <c r="U18" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V18" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W18" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
@@ -2644,12 +2876,8 @@
       <c r="AC18" s="12"/>
       <c r="AD18" s="12"/>
       <c r="AE18" s="12"/>
-      <c r="AF18" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="19" spans="1:31" ht="15" customHeight="1">
       <c r="A19" s="3">
         <v>13</v>
       </c>
@@ -2708,9 +2936,15 @@
       <c r="T19" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U19" s="32"/>
-      <c r="V19" s="32"/>
-      <c r="W19" s="12"/>
+      <c r="U19" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="V19" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W19" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
@@ -2719,12 +2953,8 @@
       <c r="AC19" s="12"/>
       <c r="AD19" s="12"/>
       <c r="AE19" s="12"/>
-      <c r="AF19" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="20" spans="1:31" ht="15" customHeight="1">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -2783,9 +3013,15 @@
       <c r="T20" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U20" s="32"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="12"/>
+      <c r="U20" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V20" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W20" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
@@ -2794,12 +3030,8 @@
       <c r="AC20" s="12"/>
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
-      <c r="AF20" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="21" spans="1:31" ht="15" customHeight="1">
       <c r="A21" s="3">
         <v>15</v>
       </c>
@@ -2858,9 +3090,15 @@
       <c r="T21" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U21" s="32"/>
-      <c r="V21" s="32"/>
-      <c r="W21" s="12"/>
+      <c r="U21" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V21" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W21" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
@@ -2869,12 +3107,8 @@
       <c r="AC21" s="12"/>
       <c r="AD21" s="12"/>
       <c r="AE21" s="12"/>
-      <c r="AF21" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="22" spans="1:31" ht="15" customHeight="1">
       <c r="A22" s="3">
         <v>16</v>
       </c>
@@ -2933,9 +3167,15 @@
       <c r="T22" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U22" s="32"/>
-      <c r="V22" s="32"/>
-      <c r="W22" s="12"/>
+      <c r="U22" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V22" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W22" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
@@ -2944,12 +3184,8 @@
       <c r="AC22" s="12"/>
       <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
-      <c r="AF22" s="32">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="23" spans="1:31" ht="15" customHeight="1">
       <c r="A23" s="3">
         <v>17</v>
       </c>
@@ -3008,9 +3244,15 @@
       <c r="T23" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U23" s="32"/>
-      <c r="V23" s="32"/>
-      <c r="W23" s="12"/>
+      <c r="U23" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W23" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="X23" s="12"/>
       <c r="Y23" s="12"/>
       <c r="Z23" s="12"/>
@@ -3019,12 +3261,8 @@
       <c r="AC23" s="12"/>
       <c r="AD23" s="12"/>
       <c r="AE23" s="12"/>
-      <c r="AF23" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="24" spans="1:31" ht="15" customHeight="1">
       <c r="A24" s="3">
         <v>18</v>
       </c>
@@ -3083,9 +3321,15 @@
       <c r="T24" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U24" s="32"/>
-      <c r="V24" s="32"/>
-      <c r="W24" s="12"/>
+      <c r="U24" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V24" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W24" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X24" s="12"/>
       <c r="Y24" s="12"/>
       <c r="Z24" s="12"/>
@@ -3094,12 +3338,8 @@
       <c r="AC24" s="12"/>
       <c r="AD24" s="12"/>
       <c r="AE24" s="12"/>
-      <c r="AF24" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="25" spans="1:31" ht="15" customHeight="1">
       <c r="A25" s="3">
         <v>19</v>
       </c>
@@ -3158,9 +3398,15 @@
       <c r="T25" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U25" s="32"/>
-      <c r="V25" s="32"/>
-      <c r="W25" s="12"/>
+      <c r="U25" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W25" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
@@ -3169,12 +3415,8 @@
       <c r="AC25" s="12"/>
       <c r="AD25" s="12"/>
       <c r="AE25" s="12"/>
-      <c r="AF25" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="26" spans="1:31" ht="15" customHeight="1">
       <c r="A26" s="3">
         <v>20</v>
       </c>
@@ -3233,9 +3475,15 @@
       <c r="T26" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U26" s="32"/>
-      <c r="V26" s="32"/>
-      <c r="W26" s="12"/>
+      <c r="U26" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V26" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W26" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
@@ -3244,12 +3492,8 @@
       <c r="AC26" s="12"/>
       <c r="AD26" s="12"/>
       <c r="AE26" s="12"/>
-      <c r="AF26" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="27" spans="1:31" ht="15" customHeight="1">
       <c r="A27" s="3">
         <v>21</v>
       </c>
@@ -3308,9 +3552,15 @@
       <c r="T27" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U27" s="32"/>
-      <c r="V27" s="32"/>
-      <c r="W27" s="12"/>
+      <c r="U27" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V27" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W27" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X27" s="12"/>
       <c r="Y27" s="12"/>
       <c r="Z27" s="12"/>
@@ -3319,12 +3569,8 @@
       <c r="AC27" s="12"/>
       <c r="AD27" s="12"/>
       <c r="AE27" s="12"/>
-      <c r="AF27" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="28" spans="1:31" ht="15" customHeight="1">
       <c r="A28" s="3">
         <v>22</v>
       </c>
@@ -3383,9 +3629,15 @@
       <c r="T28" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="12"/>
+      <c r="U28" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V28" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W28" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
       <c r="Z28" s="12"/>
@@ -3394,12 +3646,8 @@
       <c r="AC28" s="12"/>
       <c r="AD28" s="12"/>
       <c r="AE28" s="12"/>
-      <c r="AF28" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="29" spans="1:31" ht="15" customHeight="1">
       <c r="A29" s="3">
         <v>23</v>
       </c>
@@ -3458,9 +3706,15 @@
       <c r="T29" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U29" s="32"/>
-      <c r="V29" s="32"/>
-      <c r="W29" s="12"/>
+      <c r="U29" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V29" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W29" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
       <c r="Z29" s="12"/>
@@ -3469,12 +3723,8 @@
       <c r="AC29" s="12"/>
       <c r="AD29" s="12"/>
       <c r="AE29" s="12"/>
-      <c r="AF29" s="32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="30" spans="1:31" ht="15" customHeight="1">
       <c r="A30" s="3">
         <v>24</v>
       </c>
@@ -3533,9 +3783,15 @@
       <c r="T30" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U30" s="32"/>
-      <c r="V30" s="32"/>
-      <c r="W30" s="12"/>
+      <c r="U30" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="V30" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W30" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X30" s="12"/>
       <c r="Y30" s="12"/>
       <c r="Z30" s="12"/>
@@ -3544,12 +3800,8 @@
       <c r="AC30" s="12"/>
       <c r="AD30" s="12"/>
       <c r="AE30" s="12"/>
-      <c r="AF30" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="31" spans="1:31" ht="15" customHeight="1">
       <c r="A31" s="3">
         <v>25</v>
       </c>
@@ -3608,9 +3860,15 @@
       <c r="T31" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
-      <c r="W31" s="12"/>
+      <c r="U31" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V31" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W31" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X31" s="12"/>
       <c r="Y31" s="12"/>
       <c r="Z31" s="12"/>
@@ -3619,12 +3877,8 @@
       <c r="AC31" s="12"/>
       <c r="AD31" s="12"/>
       <c r="AE31" s="12"/>
-      <c r="AF31" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="32" spans="1:31" ht="15" customHeight="1">
       <c r="A32" s="3">
         <v>26</v>
       </c>
@@ -3683,9 +3937,15 @@
       <c r="T32" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U32" s="32"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="12"/>
+      <c r="U32" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V32" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W32" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X32" s="12"/>
       <c r="Y32" s="12"/>
       <c r="Z32" s="12"/>
@@ -3694,12 +3954,8 @@
       <c r="AC32" s="12"/>
       <c r="AD32" s="12"/>
       <c r="AE32" s="12"/>
-      <c r="AF32" s="32">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="33" spans="1:31" ht="15" customHeight="1">
       <c r="A33" s="3">
         <v>27</v>
       </c>
@@ -3758,9 +4014,15 @@
       <c r="T33" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U33" s="32"/>
-      <c r="V33" s="32"/>
-      <c r="W33" s="12"/>
+      <c r="U33" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="V33" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W33" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X33" s="12"/>
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
@@ -3769,12 +4031,8 @@
       <c r="AC33" s="12"/>
       <c r="AD33" s="12"/>
       <c r="AE33" s="12"/>
-      <c r="AF33" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="34" spans="1:31" ht="15" customHeight="1">
       <c r="A34" s="3">
         <v>28</v>
       </c>
@@ -3833,9 +4091,15 @@
       <c r="T34" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
-      <c r="W34" s="12"/>
+      <c r="U34" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V34" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W34" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X34" s="12"/>
       <c r="Y34" s="12"/>
       <c r="Z34" s="12"/>
@@ -3844,12 +4108,8 @@
       <c r="AC34" s="12"/>
       <c r="AD34" s="12"/>
       <c r="AE34" s="12"/>
-      <c r="AF34" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="35" spans="1:31" ht="15" customHeight="1">
       <c r="A35" s="3">
         <v>29</v>
       </c>
@@ -3908,9 +4168,15 @@
       <c r="T35" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U35" s="32"/>
-      <c r="V35" s="32"/>
-      <c r="W35" s="12"/>
+      <c r="U35" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V35" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W35" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X35" s="12"/>
       <c r="Y35" s="12"/>
       <c r="Z35" s="12"/>
@@ -3919,12 +4185,8 @@
       <c r="AC35" s="12"/>
       <c r="AD35" s="12"/>
       <c r="AE35" s="12"/>
-      <c r="AF35" s="32">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="36" spans="1:31" ht="15" customHeight="1">
       <c r="A36" s="3">
         <v>30</v>
       </c>
@@ -3983,9 +4245,15 @@
       <c r="T36" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
-      <c r="W36" s="12"/>
+      <c r="U36" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V36" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W36" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X36" s="12"/>
       <c r="Y36" s="12"/>
       <c r="Z36" s="12"/>
@@ -3994,12 +4262,8 @@
       <c r="AC36" s="12"/>
       <c r="AD36" s="12"/>
       <c r="AE36" s="12"/>
-      <c r="AF36" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="37" spans="1:31" ht="15" customHeight="1">
       <c r="A37" s="3">
         <v>31</v>
       </c>
@@ -4058,9 +4322,15 @@
       <c r="T37" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U37" s="32"/>
-      <c r="V37" s="32"/>
-      <c r="W37" s="12"/>
+      <c r="U37" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V37" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W37" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X37" s="12"/>
       <c r="Y37" s="12"/>
       <c r="Z37" s="12"/>
@@ -4069,12 +4339,8 @@
       <c r="AC37" s="12"/>
       <c r="AD37" s="12"/>
       <c r="AE37" s="12"/>
-      <c r="AF37" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="38" spans="1:31" ht="15" customHeight="1">
       <c r="A38" s="3">
         <v>32</v>
       </c>
@@ -4133,9 +4399,15 @@
       <c r="T38" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U38" s="32"/>
-      <c r="V38" s="32"/>
-      <c r="W38" s="12"/>
+      <c r="U38" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V38" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W38" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X38" s="12"/>
       <c r="Y38" s="12"/>
       <c r="Z38" s="12"/>
@@ -4144,12 +4416,8 @@
       <c r="AC38" s="12"/>
       <c r="AD38" s="12"/>
       <c r="AE38" s="12"/>
-      <c r="AF38" s="32">
-        <f t="shared" ref="AF38:AF54" si="1">COUNTIF(D39:AE39,"A")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="39" spans="1:31" ht="15" customHeight="1">
       <c r="A39" s="3">
         <v>33</v>
       </c>
@@ -4208,9 +4476,15 @@
       <c r="T39" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U39" s="32"/>
-      <c r="V39" s="32"/>
-      <c r="W39" s="12"/>
+      <c r="U39" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V39" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W39" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X39" s="12"/>
       <c r="Y39" s="12"/>
       <c r="Z39" s="12"/>
@@ -4219,12 +4493,8 @@
       <c r="AC39" s="12"/>
       <c r="AD39" s="12"/>
       <c r="AE39" s="12"/>
-      <c r="AF39" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="40" spans="1:31" ht="15" customHeight="1">
       <c r="A40" s="3">
         <v>34</v>
       </c>
@@ -4283,9 +4553,15 @@
       <c r="T40" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U40" s="32"/>
-      <c r="V40" s="32"/>
-      <c r="W40" s="12"/>
+      <c r="U40" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V40" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W40" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X40" s="12"/>
       <c r="Y40" s="12"/>
       <c r="Z40" s="12"/>
@@ -4294,12 +4570,8 @@
       <c r="AC40" s="12"/>
       <c r="AD40" s="12"/>
       <c r="AE40" s="12"/>
-      <c r="AF40" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="41" spans="1:31" ht="15" customHeight="1">
       <c r="A41" s="3">
         <v>35</v>
       </c>
@@ -4358,9 +4630,15 @@
       <c r="T41" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U41" s="32"/>
-      <c r="V41" s="32"/>
-      <c r="W41" s="12"/>
+      <c r="U41" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V41" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W41" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X41" s="12"/>
       <c r="Y41" s="12"/>
       <c r="Z41" s="12"/>
@@ -4369,12 +4647,8 @@
       <c r="AC41" s="12"/>
       <c r="AD41" s="12"/>
       <c r="AE41" s="12"/>
-      <c r="AF41" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="42" spans="1:31" ht="15" customHeight="1">
       <c r="A42" s="3">
         <v>36</v>
       </c>
@@ -4433,9 +4707,15 @@
       <c r="T42" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U42" s="32"/>
-      <c r="V42" s="32"/>
-      <c r="W42" s="12"/>
+      <c r="U42" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V42" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W42" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
       <c r="Z42" s="12"/>
@@ -4444,12 +4724,8 @@
       <c r="AC42" s="12"/>
       <c r="AD42" s="12"/>
       <c r="AE42" s="12"/>
-      <c r="AF42" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="43" spans="1:31" ht="15" customHeight="1">
       <c r="A43" s="3">
         <v>37</v>
       </c>
@@ -4508,9 +4784,15 @@
       <c r="T43" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U43" s="32"/>
-      <c r="V43" s="32"/>
-      <c r="W43" s="12"/>
+      <c r="U43" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V43" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W43" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X43" s="12"/>
       <c r="Y43" s="12"/>
       <c r="Z43" s="12"/>
@@ -4519,12 +4801,8 @@
       <c r="AC43" s="12"/>
       <c r="AD43" s="12"/>
       <c r="AE43" s="12"/>
-      <c r="AF43" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="44" spans="1:31" ht="15" customHeight="1">
       <c r="A44" s="3">
         <v>38</v>
       </c>
@@ -4583,9 +4861,15 @@
       <c r="T44" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U44" s="32"/>
-      <c r="V44" s="32"/>
-      <c r="W44" s="12"/>
+      <c r="U44" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V44" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W44" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X44" s="12"/>
       <c r="Y44" s="12"/>
       <c r="Z44" s="12"/>
@@ -4594,12 +4878,8 @@
       <c r="AC44" s="12"/>
       <c r="AD44" s="12"/>
       <c r="AE44" s="12"/>
-      <c r="AF44" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="45" spans="1:31" ht="15" customHeight="1">
       <c r="A45" s="3">
         <v>39</v>
       </c>
@@ -4658,9 +4938,15 @@
       <c r="T45" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U45" s="32"/>
-      <c r="V45" s="32"/>
-      <c r="W45" s="12"/>
+      <c r="U45" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V45" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W45" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X45" s="12"/>
       <c r="Y45" s="12"/>
       <c r="Z45" s="12"/>
@@ -4669,12 +4955,8 @@
       <c r="AC45" s="12"/>
       <c r="AD45" s="12"/>
       <c r="AE45" s="12"/>
-      <c r="AF45" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="46" spans="1:31" ht="15" customHeight="1">
       <c r="A46" s="3">
         <v>40</v>
       </c>
@@ -4733,9 +5015,15 @@
       <c r="T46" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U46" s="32"/>
-      <c r="V46" s="32"/>
-      <c r="W46" s="12"/>
+      <c r="U46" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V46" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W46" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X46" s="12"/>
       <c r="Y46" s="12"/>
       <c r="Z46" s="12"/>
@@ -4744,12 +5032,8 @@
       <c r="AC46" s="12"/>
       <c r="AD46" s="12"/>
       <c r="AE46" s="12"/>
-      <c r="AF46" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="47" spans="1:31" ht="15" customHeight="1">
       <c r="A47" s="3">
         <v>41</v>
       </c>
@@ -4808,9 +5092,15 @@
       <c r="T47" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U47" s="32"/>
-      <c r="V47" s="32"/>
-      <c r="W47" s="12"/>
+      <c r="U47" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V47" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W47" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X47" s="12"/>
       <c r="Y47" s="12"/>
       <c r="Z47" s="12"/>
@@ -4819,12 +5109,8 @@
       <c r="AC47" s="12"/>
       <c r="AD47" s="12"/>
       <c r="AE47" s="12"/>
-      <c r="AF47" s="32">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="48" spans="1:31" ht="15" customHeight="1">
       <c r="A48" s="3">
         <v>42</v>
       </c>
@@ -4883,9 +5169,15 @@
       <c r="T48" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="U48" s="32"/>
-      <c r="V48" s="32"/>
-      <c r="W48" s="12"/>
+      <c r="U48" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="V48" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W48" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X48" s="12"/>
       <c r="Y48" s="12"/>
       <c r="Z48" s="12"/>
@@ -4894,12 +5186,8 @@
       <c r="AC48" s="12"/>
       <c r="AD48" s="12"/>
       <c r="AE48" s="12"/>
-      <c r="AF48" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="49" spans="1:31" ht="15" customHeight="1">
       <c r="A49" s="3">
         <v>43</v>
       </c>
@@ -4958,9 +5246,15 @@
       <c r="T49" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U49" s="32"/>
-      <c r="V49" s="32"/>
-      <c r="W49" s="12"/>
+      <c r="U49" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V49" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W49" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X49" s="12"/>
       <c r="Y49" s="12"/>
       <c r="Z49" s="12"/>
@@ -4969,12 +5263,8 @@
       <c r="AC49" s="12"/>
       <c r="AD49" s="12"/>
       <c r="AE49" s="12"/>
-      <c r="AF49" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="50" spans="1:31" ht="15" customHeight="1">
       <c r="A50" s="3">
         <v>44</v>
       </c>
@@ -5033,9 +5323,15 @@
       <c r="T50" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U50" s="32"/>
-      <c r="V50" s="32"/>
-      <c r="W50" s="12"/>
+      <c r="U50" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V50" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W50" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="X50" s="12"/>
       <c r="Y50" s="12"/>
       <c r="Z50" s="12"/>
@@ -5044,12 +5340,8 @@
       <c r="AC50" s="12"/>
       <c r="AD50" s="12"/>
       <c r="AE50" s="12"/>
-      <c r="AF50" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="51" spans="1:31" ht="15" customHeight="1">
       <c r="A51" s="3">
         <v>45</v>
       </c>
@@ -5108,9 +5400,15 @@
       <c r="T51" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U51" s="32"/>
-      <c r="V51" s="32"/>
-      <c r="W51" s="12"/>
+      <c r="U51" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V51" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W51" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X51" s="12"/>
       <c r="Y51" s="12"/>
       <c r="Z51" s="12"/>
@@ -5119,12 +5417,8 @@
       <c r="AC51" s="12"/>
       <c r="AD51" s="12"/>
       <c r="AE51" s="12"/>
-      <c r="AF51" s="32">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="52" spans="1:31" ht="15" customHeight="1">
       <c r="A52" s="3">
         <v>46</v>
       </c>
@@ -5183,9 +5477,15 @@
       <c r="T52" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U52" s="32"/>
-      <c r="V52" s="32"/>
-      <c r="W52" s="12"/>
+      <c r="U52" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V52" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W52" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X52" s="12"/>
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
@@ -5194,12 +5494,8 @@
       <c r="AC52" s="12"/>
       <c r="AD52" s="12"/>
       <c r="AE52" s="12"/>
-      <c r="AF52" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="53" spans="1:31" ht="15" customHeight="1">
       <c r="A53" s="3">
         <v>47</v>
       </c>
@@ -5258,9 +5554,15 @@
       <c r="T53" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U53" s="32"/>
-      <c r="V53" s="32"/>
-      <c r="W53" s="12"/>
+      <c r="U53" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V53" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W53" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X53" s="12"/>
       <c r="Y53" s="12"/>
       <c r="Z53" s="12"/>
@@ -5269,12 +5571,8 @@
       <c r="AC53" s="12"/>
       <c r="AD53" s="12"/>
       <c r="AE53" s="12"/>
-      <c r="AF53" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:32" ht="15" customHeight="1">
+    </row>
+    <row r="54" spans="1:31" ht="15" customHeight="1">
       <c r="A54" s="3">
         <v>48</v>
       </c>
@@ -5333,9 +5631,15 @@
       <c r="T54" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="U54" s="32"/>
-      <c r="V54" s="32"/>
-      <c r="W54" s="12"/>
+      <c r="U54" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="V54" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="W54" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="X54" s="12"/>
       <c r="Y54" s="12"/>
       <c r="Z54" s="12"/>
@@ -5344,12 +5648,8 @@
       <c r="AC54" s="12"/>
       <c r="AD54" s="12"/>
       <c r="AE54" s="12"/>
-      <c r="AF54" s="32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:32">
+    </row>
+    <row r="55" spans="1:31">
       <c r="A55" s="44" t="s">
         <v>57</v>
       </c>
@@ -5360,115 +5660,115 @@
         <v>0</v>
       </c>
       <c r="E55" s="12">
-        <f t="shared" ref="E55:F55" si="2">COUNTIF(E7:E54,"A")</f>
+        <f t="shared" ref="E55:F55" si="0">COUNTIF(E7:E54,"A")</f>
         <v>0</v>
       </c>
       <c r="F55" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G55" s="12">
-        <f t="shared" ref="G55" si="3">COUNTIF(G7:G54,"A")</f>
+        <f t="shared" ref="G55" si="1">COUNTIF(G7:G54,"A")</f>
         <v>2</v>
       </c>
       <c r="H55" s="12">
-        <f t="shared" ref="H55" si="4">COUNTIF(H7:H54,"A")</f>
+        <f t="shared" ref="H55" si="2">COUNTIF(H7:H54,"A")</f>
         <v>11</v>
       </c>
       <c r="I55" s="12">
-        <f t="shared" ref="I55" si="5">COUNTIF(I7:I54,"A")</f>
+        <f t="shared" ref="I55" si="3">COUNTIF(I7:I54,"A")</f>
         <v>11</v>
       </c>
       <c r="J55" s="12">
-        <f t="shared" ref="J55" si="6">COUNTIF(J7:J54,"A")</f>
+        <f t="shared" ref="J55" si="4">COUNTIF(J7:J54,"A")</f>
         <v>1</v>
       </c>
       <c r="K55" s="12">
-        <f t="shared" ref="K55" si="7">COUNTIF(K7:K54,"A")</f>
+        <f t="shared" ref="K55" si="5">COUNTIF(K7:K54,"A")</f>
         <v>1</v>
       </c>
       <c r="L55" s="12">
-        <f t="shared" ref="L55" si="8">COUNTIF(L7:L54,"A")</f>
+        <f t="shared" ref="L55" si="6">COUNTIF(L7:L54,"A")</f>
         <v>6</v>
       </c>
       <c r="M55" s="12">
-        <f t="shared" ref="M55" si="9">COUNTIF(M7:M54,"A")</f>
+        <f t="shared" ref="M55" si="7">COUNTIF(M7:M54,"A")</f>
         <v>11</v>
       </c>
       <c r="N55" s="12">
-        <f t="shared" ref="N55" si="10">COUNTIF(N7:N54,"A")</f>
+        <f t="shared" ref="N55" si="8">COUNTIF(N7:N54,"A")</f>
         <v>3</v>
       </c>
       <c r="O55" s="12">
-        <f t="shared" ref="O55" si="11">COUNTIF(O7:O54,"A")</f>
+        <f t="shared" ref="O55" si="9">COUNTIF(O7:O54,"A")</f>
         <v>1</v>
       </c>
       <c r="P55" s="12">
-        <f t="shared" ref="P55" si="12">COUNTIF(P7:P54,"A")</f>
+        <f t="shared" ref="P55" si="10">COUNTIF(P7:P54,"A")</f>
         <v>1</v>
       </c>
       <c r="Q55" s="12">
-        <f t="shared" ref="Q55" si="13">COUNTIF(Q7:Q54,"A")</f>
+        <f t="shared" ref="Q55" si="11">COUNTIF(Q7:Q54,"A")</f>
         <v>2</v>
       </c>
       <c r="R55" s="12">
-        <f t="shared" ref="R55:V55" si="14">COUNTIF(R7:R54,"A")</f>
+        <f t="shared" ref="R55:V55" si="12">COUNTIF(R7:R54,"A")</f>
         <v>3</v>
       </c>
       <c r="S55" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="T55" s="32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="U55" s="32">
-        <f t="shared" si="14"/>
+      <c r="U55" s="37">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="V55" s="32">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="W55" s="12">
+        <f t="shared" ref="W55" si="13">COUNTIF(W7:W54,"A")</f>
+        <v>4</v>
+      </c>
+      <c r="X55" s="12">
+        <f t="shared" ref="X55" si="14">COUNTIF(X7:X54,"A")</f>
         <v>0</v>
       </c>
-      <c r="V55" s="32">
-        <f t="shared" si="14"/>
+      <c r="Y55" s="12">
+        <f t="shared" ref="Y55" si="15">COUNTIF(Y7:Y54,"A")</f>
         <v>0</v>
       </c>
-      <c r="W55" s="12">
-        <f t="shared" ref="W55" si="15">COUNTIF(W7:W54,"A")</f>
+      <c r="Z55" s="12">
+        <f t="shared" ref="Z55" si="16">COUNTIF(Z7:Z54,"A")</f>
         <v>0</v>
       </c>
-      <c r="X55" s="12">
-        <f t="shared" ref="X55" si="16">COUNTIF(X7:X54,"A")</f>
+      <c r="AA55" s="12">
+        <f t="shared" ref="AA55" si="17">COUNTIF(AA7:AA54,"A")</f>
         <v>0</v>
       </c>
-      <c r="Y55" s="12">
-        <f t="shared" ref="Y55" si="17">COUNTIF(Y7:Y54,"A")</f>
+      <c r="AB55" s="12">
+        <f t="shared" ref="AB55" si="18">COUNTIF(AB7:AB54,"A")</f>
         <v>0</v>
       </c>
-      <c r="Z55" s="12">
-        <f t="shared" ref="Z55" si="18">COUNTIF(Z7:Z54,"A")</f>
+      <c r="AC55" s="12">
+        <f t="shared" ref="AC55" si="19">COUNTIF(AC7:AC54,"A")</f>
         <v>0</v>
       </c>
-      <c r="AA55" s="12">
-        <f t="shared" ref="AA55" si="19">COUNTIF(AA7:AA54,"A")</f>
+      <c r="AD55" s="12">
+        <f t="shared" ref="AD55" si="20">COUNTIF(AD7:AD54,"A")</f>
         <v>0</v>
       </c>
-      <c r="AB55" s="12">
-        <f t="shared" ref="AB55" si="20">COUNTIF(AB7:AB54,"A")</f>
+      <c r="AE55" s="12">
+        <f t="shared" ref="AE55" si="21">COUNTIF(AE7:AE54,"A")</f>
         <v>0</v>
       </c>
-      <c r="AC55" s="12">
-        <f t="shared" ref="AC55" si="21">COUNTIF(AC7:AC54,"A")</f>
-        <v>0</v>
-      </c>
-      <c r="AD55" s="12">
-        <f t="shared" ref="AD55" si="22">COUNTIF(AD7:AD54,"A")</f>
-        <v>0</v>
-      </c>
-      <c r="AE55" s="12">
-        <f t="shared" ref="AE55" si="23">COUNTIF(AE7:AE54,"A")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:32">
+    </row>
+    <row r="56" spans="1:31">
       <c r="A56" s="38" t="s">
         <v>58</v>
       </c>
@@ -5479,117 +5779,116 @@
         <v>48</v>
       </c>
       <c r="E56" s="24">
-        <f t="shared" ref="E56:AE56" si="24">(48-E55)</f>
+        <f t="shared" ref="E56:AE56" si="22">(48-E55)</f>
         <v>48</v>
       </c>
       <c r="F56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
       <c r="G56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>46</v>
       </c>
       <c r="H56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>37</v>
       </c>
       <c r="I56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>37</v>
       </c>
       <c r="J56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
       <c r="K56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
       <c r="L56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>42</v>
       </c>
       <c r="M56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>37</v>
       </c>
       <c r="N56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>45</v>
       </c>
       <c r="O56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
       <c r="P56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
       <c r="Q56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>46</v>
       </c>
       <c r="R56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>45</v>
       </c>
       <c r="S56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
       <c r="T56" s="24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
-      <c r="U56" s="24">
-        <f t="shared" si="24"/>
+      <c r="U56" s="37">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="V56" s="24">
+        <f t="shared" si="22"/>
+        <v>40</v>
+      </c>
+      <c r="W56" s="24">
+        <f t="shared" si="22"/>
+        <v>44</v>
+      </c>
+      <c r="X56" s="24">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="V56" s="24">
-        <f t="shared" si="24"/>
+      <c r="Y56" s="24">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="W56" s="24">
-        <f t="shared" si="24"/>
+      <c r="Z56" s="24">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="X56" s="24">
-        <f t="shared" si="24"/>
+      <c r="AA56" s="24">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="Y56" s="24">
-        <f t="shared" si="24"/>
+      <c r="AB56" s="24">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="Z56" s="24">
-        <f t="shared" si="24"/>
+      <c r="AC56" s="24">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="AA56" s="24">
-        <f t="shared" si="24"/>
+      <c r="AD56" s="24">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="AB56" s="24">
-        <f t="shared" si="24"/>
+      <c r="AE56" s="24">
+        <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="AC56" s="24">
-        <f t="shared" si="24"/>
-        <v>48</v>
-      </c>
-      <c r="AD56" s="24">
-        <f t="shared" si="24"/>
-        <v>48</v>
-      </c>
-      <c r="AE56" s="24">
-        <f t="shared" si="24"/>
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="AF4:AF5"/>
+  <mergeCells count="9">
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F3:I3"/>
@@ -5600,15 +5899,6 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
   </mergeCells>
-  <conditionalFormatting sqref="AF1:AF1048576">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -5620,7 +5910,7 @@
   <dimension ref="A1:AF57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AG5" sqref="AG5"/>
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -5704,6 +5994,12 @@
         <v>62</v>
       </c>
       <c r="M4" s="52"/>
+      <c r="N4" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58"/>
+      <c r="Q4" s="58"/>
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="46" t="s">
@@ -5745,10 +6041,18 @@
       <c r="M5" s="27">
         <v>9</v>
       </c>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
+      <c r="N5" s="19">
+        <v>10</v>
+      </c>
+      <c r="O5" s="37">
+        <v>10</v>
+      </c>
+      <c r="P5" s="37">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="37">
+        <v>10</v>
+      </c>
       <c r="R5" s="19"/>
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
@@ -5801,10 +6105,18 @@
       <c r="M6" s="27">
         <v>25</v>
       </c>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
+      <c r="N6" s="19">
+        <v>3</v>
+      </c>
+      <c r="O6" s="37">
+        <v>3</v>
+      </c>
+      <c r="P6" s="37">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="37">
+        <v>3</v>
+      </c>
       <c r="R6" s="19"/>
       <c r="S6" s="19"/>
       <c r="T6" s="19"/>
@@ -5857,10 +6169,18 @@
       <c r="M7" s="27">
         <v>2</v>
       </c>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
+      <c r="N7" s="19">
+        <v>1</v>
+      </c>
+      <c r="O7" s="37">
+        <v>2</v>
+      </c>
+      <c r="P7" s="37">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="37">
+        <v>4</v>
+      </c>
       <c r="R7" s="19"/>
       <c r="S7" s="19"/>
       <c r="T7" s="19"/>
@@ -5915,10 +6235,18 @@
       <c r="M8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
+      <c r="N8" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O8" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R8" s="19"/>
       <c r="S8" s="19"/>
       <c r="T8" s="19"/>
@@ -5973,10 +6301,18 @@
       <c r="M9" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
+      <c r="N9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R9" s="19"/>
       <c r="S9" s="19"/>
       <c r="T9" s="19"/>
@@ -6031,10 +6367,18 @@
       <c r="M10" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
+      <c r="N10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="R10" s="19"/>
       <c r="S10" s="19"/>
       <c r="T10" s="19"/>
@@ -6089,10 +6433,18 @@
       <c r="M11" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
+      <c r="N11" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P11" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R11" s="19"/>
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
@@ -6147,10 +6499,18 @@
       <c r="M12" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
+      <c r="N12" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O12" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q12" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R12" s="19"/>
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
@@ -6205,10 +6565,18 @@
       <c r="M13" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
+      <c r="N13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q13" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R13" s="19"/>
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
@@ -6263,10 +6631,18 @@
       <c r="M14" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
+      <c r="N14" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q14" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R14" s="19"/>
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
@@ -6321,10 +6697,18 @@
       <c r="M15" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
+      <c r="N15" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q15" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R15" s="19"/>
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>
@@ -6379,10 +6763,18 @@
       <c r="M16" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
+      <c r="N16" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O16" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P16" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q16" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R16" s="19"/>
       <c r="S16" s="19"/>
       <c r="T16" s="19"/>
@@ -6437,10 +6829,18 @@
       <c r="M17" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
+      <c r="N17" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O17" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P17" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q17" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R17" s="19"/>
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
@@ -6495,10 +6895,18 @@
       <c r="M18" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
+      <c r="N18" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O18" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P18" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q18" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R18" s="19"/>
       <c r="S18" s="19"/>
       <c r="T18" s="19"/>
@@ -6553,10 +6961,18 @@
       <c r="M19" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
+      <c r="N19" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O19" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P19" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q19" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R19" s="19"/>
       <c r="S19" s="19"/>
       <c r="T19" s="19"/>
@@ -6611,10 +7027,18 @@
       <c r="M20" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
+      <c r="N20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q20" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="R20" s="19"/>
       <c r="S20" s="19"/>
       <c r="T20" s="19"/>
@@ -6669,10 +7093,18 @@
       <c r="M21" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
+      <c r="N21" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O21" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P21" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q21" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R21" s="19"/>
       <c r="S21" s="19"/>
       <c r="T21" s="19"/>
@@ -6727,10 +7159,18 @@
       <c r="M22" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
+      <c r="N22" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O22" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P22" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q22" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R22" s="19"/>
       <c r="S22" s="19"/>
       <c r="T22" s="19"/>
@@ -6785,10 +7225,18 @@
       <c r="M23" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
+      <c r="N23" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O23" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P23" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q23" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R23" s="19"/>
       <c r="S23" s="19"/>
       <c r="T23" s="19"/>
@@ -6843,10 +7291,18 @@
       <c r="M24" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
+      <c r="N24" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O24" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="R24" s="19"/>
       <c r="S24" s="19"/>
       <c r="T24" s="19"/>
@@ -6901,10 +7357,18 @@
       <c r="M25" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N25" s="19"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
+      <c r="N25" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O25" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P25" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q25" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R25" s="19"/>
       <c r="S25" s="19"/>
       <c r="T25" s="19"/>
@@ -6959,10 +7423,18 @@
       <c r="M26" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N26" s="19"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
+      <c r="N26" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O26" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P26" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q26" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R26" s="19"/>
       <c r="S26" s="19"/>
       <c r="T26" s="19"/>
@@ -7017,10 +7489,18 @@
       <c r="M27" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
+      <c r="N27" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O27" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P27" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q27" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R27" s="19"/>
       <c r="S27" s="19"/>
       <c r="T27" s="19"/>
@@ -7075,10 +7555,18 @@
       <c r="M28" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
+      <c r="N28" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O28" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P28" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q28" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R28" s="19"/>
       <c r="S28" s="19"/>
       <c r="T28" s="19"/>
@@ -7133,10 +7621,18 @@
       <c r="M29" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="19"/>
+      <c r="N29" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O29" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P29" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q29" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R29" s="19"/>
       <c r="S29" s="19"/>
       <c r="T29" s="19"/>
@@ -7191,10 +7687,18 @@
       <c r="M30" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
+      <c r="N30" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O30" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P30" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q30" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R30" s="19"/>
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
@@ -7249,10 +7753,18 @@
       <c r="M31" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
+      <c r="N31" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O31" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P31" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q31" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R31" s="19"/>
       <c r="S31" s="19"/>
       <c r="T31" s="19"/>
@@ -7307,10 +7819,18 @@
       <c r="M32" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
+      <c r="N32" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O32" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P32" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q32" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R32" s="19"/>
       <c r="S32" s="19"/>
       <c r="T32" s="19"/>
@@ -7365,10 +7885,18 @@
       <c r="M33" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
+      <c r="N33" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O33" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P33" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q33" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R33" s="19"/>
       <c r="S33" s="19"/>
       <c r="T33" s="19"/>
@@ -7423,10 +7951,18 @@
       <c r="M34" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
+      <c r="N34" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O34" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P34" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q34" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R34" s="19"/>
       <c r="S34" s="19"/>
       <c r="T34" s="19"/>
@@ -7481,10 +8017,18 @@
       <c r="M35" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
+      <c r="N35" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O35" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P35" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q35" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R35" s="19"/>
       <c r="S35" s="19"/>
       <c r="T35" s="19"/>
@@ -7539,10 +8083,18 @@
       <c r="M36" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
+      <c r="N36" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O36" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P36" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q36" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R36" s="19"/>
       <c r="S36" s="19"/>
       <c r="T36" s="19"/>
@@ -7597,10 +8149,18 @@
       <c r="M37" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
+      <c r="N37" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O37" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P37" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q37" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R37" s="19"/>
       <c r="S37" s="19"/>
       <c r="T37" s="19"/>
@@ -7655,10 +8215,18 @@
       <c r="M38" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
+      <c r="N38" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O38" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P38" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q38" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R38" s="19"/>
       <c r="S38" s="19"/>
       <c r="T38" s="19"/>
@@ -7713,10 +8281,18 @@
       <c r="M39" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
+      <c r="N39" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O39" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P39" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q39" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R39" s="19"/>
       <c r="S39" s="19"/>
       <c r="T39" s="19"/>
@@ -7771,10 +8347,18 @@
       <c r="M40" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="19"/>
+      <c r="N40" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O40" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P40" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q40" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R40" s="19"/>
       <c r="S40" s="19"/>
       <c r="T40" s="19"/>
@@ -7829,10 +8413,18 @@
       <c r="M41" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="19"/>
+      <c r="N41" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O41" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P41" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q41" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R41" s="19"/>
       <c r="S41" s="19"/>
       <c r="T41" s="19"/>
@@ -7887,10 +8479,18 @@
       <c r="M42" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
+      <c r="N42" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O42" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P42" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q42" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R42" s="19"/>
       <c r="S42" s="19"/>
       <c r="T42" s="19"/>
@@ -7945,10 +8545,18 @@
       <c r="M43" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="19"/>
+      <c r="N43" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O43" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P43" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q43" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R43" s="19"/>
       <c r="S43" s="19"/>
       <c r="T43" s="19"/>
@@ -8003,10 +8611,18 @@
       <c r="M44" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="19"/>
+      <c r="N44" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O44" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P44" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q44" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R44" s="19"/>
       <c r="S44" s="19"/>
       <c r="T44" s="19"/>
@@ -8061,10 +8677,18 @@
       <c r="M45" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
+      <c r="N45" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O45" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P45" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q45" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R45" s="19"/>
       <c r="S45" s="19"/>
       <c r="T45" s="19"/>
@@ -8119,10 +8743,18 @@
       <c r="M46" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
+      <c r="N46" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O46" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P46" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q46" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R46" s="19"/>
       <c r="S46" s="19"/>
       <c r="T46" s="19"/>
@@ -8177,10 +8809,18 @@
       <c r="M47" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N47" s="19"/>
-      <c r="O47" s="19"/>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="19"/>
+      <c r="N47" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O47" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P47" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q47" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R47" s="19"/>
       <c r="S47" s="19"/>
       <c r="T47" s="19"/>
@@ -8235,10 +8875,18 @@
       <c r="M48" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N48" s="19"/>
-      <c r="O48" s="19"/>
-      <c r="P48" s="19"/>
-      <c r="Q48" s="19"/>
+      <c r="N48" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O48" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P48" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q48" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R48" s="19"/>
       <c r="S48" s="19"/>
       <c r="T48" s="19"/>
@@ -8293,10 +8941,18 @@
       <c r="M49" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N49" s="19"/>
-      <c r="O49" s="19"/>
-      <c r="P49" s="19"/>
-      <c r="Q49" s="19"/>
+      <c r="N49" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O49" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P49" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q49" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R49" s="19"/>
       <c r="S49" s="19"/>
       <c r="T49" s="19"/>
@@ -8351,10 +9007,18 @@
       <c r="M50" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="19"/>
+      <c r="N50" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O50" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P50" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q50" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R50" s="19"/>
       <c r="S50" s="19"/>
       <c r="T50" s="19"/>
@@ -8409,10 +9073,18 @@
       <c r="M51" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="19"/>
-      <c r="Q51" s="19"/>
+      <c r="N51" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O51" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="P51" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q51" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="R51" s="19"/>
       <c r="S51" s="19"/>
       <c r="T51" s="19"/>
@@ -8467,10 +9139,18 @@
       <c r="M52" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N52" s="19"/>
-      <c r="O52" s="19"/>
-      <c r="P52" s="19"/>
-      <c r="Q52" s="19"/>
+      <c r="N52" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O52" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P52" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q52" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R52" s="19"/>
       <c r="S52" s="19"/>
       <c r="T52" s="19"/>
@@ -8525,10 +9205,18 @@
       <c r="M53" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
-      <c r="P53" s="19"/>
-      <c r="Q53" s="19"/>
+      <c r="N53" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O53" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P53" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q53" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R53" s="19"/>
       <c r="S53" s="19"/>
       <c r="T53" s="19"/>
@@ -8583,10 +9271,18 @@
       <c r="M54" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N54" s="19"/>
-      <c r="O54" s="19"/>
-      <c r="P54" s="19"/>
-      <c r="Q54" s="19"/>
+      <c r="N54" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O54" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P54" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q54" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R54" s="19"/>
       <c r="S54" s="19"/>
       <c r="T54" s="19"/>
@@ -8641,10 +9337,18 @@
       <c r="M55" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="N55" s="19"/>
-      <c r="O55" s="19"/>
-      <c r="P55" s="19"/>
-      <c r="Q55" s="19"/>
+      <c r="N55" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="O55" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P55" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q55" s="37" t="s">
+        <v>54</v>
+      </c>
       <c r="R55" s="19"/>
       <c r="S55" s="19"/>
       <c r="T55" s="19"/>
@@ -8709,19 +9413,19 @@
       </c>
       <c r="N56" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O56" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P56" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q56" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R56" s="19">
         <f t="shared" si="0"/>
@@ -8832,19 +9536,19 @@
       </c>
       <c r="N57" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="O57" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P57" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="Q57" s="24">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="R57" s="24">
         <f t="shared" si="1"/>
@@ -8908,7 +9612,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A57:B57"/>
@@ -8932,8 +9637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Last Update 04-10-2018 14:23:23.24
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Test Marks" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$M$1:$M$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$X$1:$X$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Test Marks'!$C$1:$C$56</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -508,6 +508,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="X6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Operators [Logical, Bitwise, Membership, Identity], Operator Precedence</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -718,7 +742,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1824" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="72">
   <si>
     <t>S.NO</t>
   </si>
@@ -1159,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1273,6 +1297,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1318,6 +1345,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1331,12 +1364,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1660,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1674,61 +1701,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:31" ht="19.5">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:31" ht="18.75">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="48" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1794,7 +1821,9 @@
       <c r="W4" s="37">
         <v>10</v>
       </c>
-      <c r="X4" s="12"/>
+      <c r="X4" s="12">
+        <v>10</v>
+      </c>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
       <c r="AA4" s="12"/>
@@ -1804,8 +1833,8 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="1:31">
-      <c r="A5" s="46"/>
-      <c r="B5" s="48"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -1869,7 +1898,9 @@
       <c r="W5" s="37">
         <v>3</v>
       </c>
-      <c r="X5" s="12"/>
+      <c r="X5" s="12">
+        <v>4</v>
+      </c>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
       <c r="AA5" s="12"/>
@@ -1879,8 +1910,8 @@
       <c r="AE5" s="12"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -1944,7 +1975,9 @@
       <c r="W6" s="37">
         <v>7</v>
       </c>
-      <c r="X6" s="12"/>
+      <c r="X6" s="12">
+        <v>5</v>
+      </c>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
       <c r="AA6" s="12"/>
@@ -2021,7 +2054,9 @@
       <c r="W7" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X7" s="12"/>
+      <c r="X7" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
       <c r="AA7" s="12"/>
@@ -2098,7 +2133,9 @@
       <c r="W8" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X8" s="12"/>
+      <c r="X8" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="12"/>
@@ -2175,7 +2212,9 @@
       <c r="W9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="X9" s="12"/>
+      <c r="X9" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
       <c r="AA9" s="12"/>
@@ -2252,7 +2291,9 @@
       <c r="W10" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X10" s="12"/>
+      <c r="X10" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
       <c r="AA10" s="12"/>
@@ -2329,7 +2370,9 @@
       <c r="W11" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X11" s="12"/>
+      <c r="X11" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12"/>
@@ -2406,7 +2449,9 @@
       <c r="W12" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X12" s="12"/>
+      <c r="X12" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
@@ -2483,7 +2528,9 @@
       <c r="W13" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X13" s="12"/>
+      <c r="X13" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
       <c r="AA13" s="12"/>
@@ -2560,7 +2607,9 @@
       <c r="W14" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X14" s="12"/>
+      <c r="X14" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
       <c r="AA14" s="12"/>
@@ -2637,7 +2686,9 @@
       <c r="W15" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X15" s="12"/>
+      <c r="X15" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
@@ -2714,7 +2765,9 @@
       <c r="W16" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X16" s="12"/>
+      <c r="X16" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
@@ -2791,7 +2844,9 @@
       <c r="W17" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X17" s="12"/>
+      <c r="X17" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
@@ -2868,7 +2923,9 @@
       <c r="W18" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X18" s="12"/>
+      <c r="X18" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
@@ -2945,7 +3002,9 @@
       <c r="W19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="X19" s="12"/>
+      <c r="X19" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
       <c r="AA19" s="12"/>
@@ -3022,7 +3081,9 @@
       <c r="W20" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X20" s="12"/>
+      <c r="X20" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
@@ -3099,7 +3160,9 @@
       <c r="W21" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X21" s="12"/>
+      <c r="X21" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
@@ -3176,7 +3239,9 @@
       <c r="W22" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X22" s="12"/>
+      <c r="X22" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
       <c r="AA22" s="12"/>
@@ -3253,7 +3318,9 @@
       <c r="W23" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="X23" s="12"/>
+      <c r="X23" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y23" s="12"/>
       <c r="Z23" s="12"/>
       <c r="AA23" s="12"/>
@@ -3330,7 +3397,9 @@
       <c r="W24" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X24" s="12"/>
+      <c r="X24" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y24" s="12"/>
       <c r="Z24" s="12"/>
       <c r="AA24" s="12"/>
@@ -3407,7 +3476,9 @@
       <c r="W25" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X25" s="12"/>
+      <c r="X25" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
       <c r="AA25" s="12"/>
@@ -3484,7 +3555,9 @@
       <c r="W26" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X26" s="12"/>
+      <c r="X26" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
       <c r="AA26" s="12"/>
@@ -3561,7 +3634,9 @@
       <c r="W27" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X27" s="12"/>
+      <c r="X27" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y27" s="12"/>
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
@@ -3638,7 +3713,9 @@
       <c r="W28" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X28" s="12"/>
+      <c r="X28" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y28" s="12"/>
       <c r="Z28" s="12"/>
       <c r="AA28" s="12"/>
@@ -3715,7 +3792,9 @@
       <c r="W29" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X29" s="12"/>
+      <c r="X29" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="Y29" s="12"/>
       <c r="Z29" s="12"/>
       <c r="AA29" s="12"/>
@@ -3792,7 +3871,9 @@
       <c r="W30" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X30" s="12"/>
+      <c r="X30" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y30" s="12"/>
       <c r="Z30" s="12"/>
       <c r="AA30" s="12"/>
@@ -3869,7 +3950,9 @@
       <c r="W31" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X31" s="12"/>
+      <c r="X31" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="Y31" s="12"/>
       <c r="Z31" s="12"/>
       <c r="AA31" s="12"/>
@@ -3946,7 +4029,9 @@
       <c r="W32" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X32" s="12"/>
+      <c r="X32" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y32" s="12"/>
       <c r="Z32" s="12"/>
       <c r="AA32" s="12"/>
@@ -4023,7 +4108,9 @@
       <c r="W33" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X33" s="12"/>
+      <c r="X33" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
       <c r="AA33" s="12"/>
@@ -4100,7 +4187,9 @@
       <c r="W34" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X34" s="12"/>
+      <c r="X34" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y34" s="12"/>
       <c r="Z34" s="12"/>
       <c r="AA34" s="12"/>
@@ -4177,7 +4266,9 @@
       <c r="W35" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X35" s="12"/>
+      <c r="X35" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y35" s="12"/>
       <c r="Z35" s="12"/>
       <c r="AA35" s="12"/>
@@ -4254,7 +4345,9 @@
       <c r="W36" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X36" s="12"/>
+      <c r="X36" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="Y36" s="12"/>
       <c r="Z36" s="12"/>
       <c r="AA36" s="12"/>
@@ -4331,7 +4424,9 @@
       <c r="W37" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X37" s="12"/>
+      <c r="X37" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y37" s="12"/>
       <c r="Z37" s="12"/>
       <c r="AA37" s="12"/>
@@ -4408,7 +4503,9 @@
       <c r="W38" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X38" s="12"/>
+      <c r="X38" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y38" s="12"/>
       <c r="Z38" s="12"/>
       <c r="AA38" s="12"/>
@@ -4485,7 +4582,9 @@
       <c r="W39" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X39" s="12"/>
+      <c r="X39" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y39" s="12"/>
       <c r="Z39" s="12"/>
       <c r="AA39" s="12"/>
@@ -4562,7 +4661,9 @@
       <c r="W40" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X40" s="12"/>
+      <c r="X40" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y40" s="12"/>
       <c r="Z40" s="12"/>
       <c r="AA40" s="12"/>
@@ -4639,7 +4740,9 @@
       <c r="W41" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X41" s="12"/>
+      <c r="X41" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y41" s="12"/>
       <c r="Z41" s="12"/>
       <c r="AA41" s="12"/>
@@ -4716,7 +4819,9 @@
       <c r="W42" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X42" s="12"/>
+      <c r="X42" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y42" s="12"/>
       <c r="Z42" s="12"/>
       <c r="AA42" s="12"/>
@@ -4793,7 +4898,9 @@
       <c r="W43" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X43" s="12"/>
+      <c r="X43" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y43" s="12"/>
       <c r="Z43" s="12"/>
       <c r="AA43" s="12"/>
@@ -4870,7 +4977,9 @@
       <c r="W44" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X44" s="12"/>
+      <c r="X44" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y44" s="12"/>
       <c r="Z44" s="12"/>
       <c r="AA44" s="12"/>
@@ -4947,7 +5056,9 @@
       <c r="W45" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X45" s="12"/>
+      <c r="X45" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y45" s="12"/>
       <c r="Z45" s="12"/>
       <c r="AA45" s="12"/>
@@ -5024,7 +5135,9 @@
       <c r="W46" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X46" s="12"/>
+      <c r="X46" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y46" s="12"/>
       <c r="Z46" s="12"/>
       <c r="AA46" s="12"/>
@@ -5101,7 +5214,9 @@
       <c r="W47" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X47" s="12"/>
+      <c r="X47" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y47" s="12"/>
       <c r="Z47" s="12"/>
       <c r="AA47" s="12"/>
@@ -5178,7 +5293,9 @@
       <c r="W48" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X48" s="12"/>
+      <c r="X48" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y48" s="12"/>
       <c r="Z48" s="12"/>
       <c r="AA48" s="12"/>
@@ -5255,7 +5372,9 @@
       <c r="W49" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X49" s="12"/>
+      <c r="X49" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y49" s="12"/>
       <c r="Z49" s="12"/>
       <c r="AA49" s="12"/>
@@ -5332,7 +5451,9 @@
       <c r="W50" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="X50" s="12"/>
+      <c r="X50" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y50" s="12"/>
       <c r="Z50" s="12"/>
       <c r="AA50" s="12"/>
@@ -5409,7 +5530,9 @@
       <c r="W51" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X51" s="12"/>
+      <c r="X51" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y51" s="12"/>
       <c r="Z51" s="12"/>
       <c r="AA51" s="12"/>
@@ -5486,7 +5609,9 @@
       <c r="W52" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X52" s="12"/>
+      <c r="X52" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
       <c r="AA52" s="12"/>
@@ -5563,7 +5688,9 @@
       <c r="W53" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X53" s="12"/>
+      <c r="X53" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y53" s="12"/>
       <c r="Z53" s="12"/>
       <c r="AA53" s="12"/>
@@ -5640,7 +5767,9 @@
       <c r="W54" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="X54" s="12"/>
+      <c r="X54" s="38" t="s">
+        <v>54</v>
+      </c>
       <c r="Y54" s="12"/>
       <c r="Z54" s="12"/>
       <c r="AA54" s="12"/>
@@ -5650,10 +5779,10 @@
       <c r="AE54" s="12"/>
     </row>
     <row r="55" spans="1:31">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="45"/>
+      <c r="B55" s="46"/>
       <c r="C55" s="13"/>
       <c r="D55" s="12">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -5737,7 +5866,7 @@
       </c>
       <c r="X55" s="12">
         <f t="shared" ref="X55" si="14">COUNTIF(X7:X54,"A")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y55" s="12">
         <f t="shared" ref="Y55" si="15">COUNTIF(Y7:Y54,"A")</f>
@@ -5769,10 +5898,10 @@
       </c>
     </row>
     <row r="56" spans="1:31">
-      <c r="A56" s="38" t="s">
+      <c r="A56" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="39"/>
+      <c r="B56" s="40"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>(48-D55)</f>
@@ -5856,7 +5985,7 @@
       </c>
       <c r="X56" s="24">
         <f t="shared" si="22"/>
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="Y56" s="24">
         <f t="shared" si="22"/>
@@ -5924,88 +6053,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
       <c r="D2" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
     </row>
     <row r="4" spans="1:32" ht="18.75">
       <c r="A4" s="33"/>
       <c r="B4" s="34"/>
       <c r="C4" s="33"/>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="57" t="s">
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="52" t="s">
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="57" t="s">
+      <c r="M4" s="55"/>
+      <c r="N4" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="48" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -6070,8 +6199,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="46"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -6134,8 +6263,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1">
-      <c r="A7" s="46"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -9366,10 +9495,10 @@
       <c r="AF55" s="19"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="44" t="s">
+      <c r="A56" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="45"/>
+      <c r="B56" s="46"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -9489,10 +9618,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="38" t="s">
+      <c r="A57" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="39"/>
+      <c r="B57" s="40"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>(48-D56)</f>
@@ -9651,56 +9780,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:7" ht="19.5">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
     </row>
     <row r="3" spans="1:7" ht="18.75">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="46"/>
-      <c r="B5" s="48"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="32" t="s">
         <v>62</v>
       </c>
@@ -9710,8 +9839,8 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
-      <c r="A6" s="46"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="35">
         <v>50</v>
       </c>
@@ -10441,10 +10570,10 @@
       <c r="G54" s="13"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="45"/>
+      <c r="B55" s="46"/>
       <c r="C55" s="32">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -10455,10 +10584,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="38" t="s">
+      <c r="A56" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="39"/>
+      <c r="B56" s="40"/>
       <c r="C56" s="32">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -10469,10 +10598,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="38" t="s">
+      <c r="A57" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="39"/>
+      <c r="B57" s="40"/>
       <c r="C57" s="32">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -10483,10 +10612,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="38" t="s">
+      <c r="A58" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="39"/>
+      <c r="B58" s="40"/>
       <c r="C58" s="36">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>

</xml_diff>

<commit_message>
Last Update 05-10-2018 15:45:09.80
</commit_message>
<xml_diff>
--- a/Acadamic Log Book.xlsx
+++ b/Acadamic Log Book.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Test Marks" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$X$1:$X$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$Y$1:$Y$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Test Marks'!$C$1:$C$56</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
@@ -532,6 +532,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="Y6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Comments, Built In Functions</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rajasekaran S:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+User defined functions</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -742,7 +790,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="72">
   <si>
     <t>S.NO</t>
   </si>
@@ -1183,7 +1231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1292,6 +1340,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1687,8 +1741,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="AF7" sqref="AF7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1701,61 +1758,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:31" ht="19.5">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:31" ht="18.75">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
     </row>
     <row r="4" spans="1:31">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="50" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1824,8 +1881,12 @@
       <c r="X4" s="12">
         <v>10</v>
       </c>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
+      <c r="Y4" s="12">
+        <v>10</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>10</v>
+      </c>
       <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
@@ -1833,8 +1894,8 @@
       <c r="AE4" s="12"/>
     </row>
     <row r="5" spans="1:31">
-      <c r="A5" s="47"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="9" t="s">
         <v>48</v>
       </c>
@@ -1901,8 +1962,12 @@
       <c r="X5" s="12">
         <v>4</v>
       </c>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
+      <c r="Y5" s="12">
+        <v>5</v>
+      </c>
+      <c r="Z5" s="12">
+        <v>5</v>
+      </c>
       <c r="AA5" s="12"/>
       <c r="AB5" s="12"/>
       <c r="AC5" s="12"/>
@@ -1910,8 +1975,8 @@
       <c r="AE5" s="12"/>
     </row>
     <row r="6" spans="1:31" ht="15" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="10" t="s">
         <v>49</v>
       </c>
@@ -1978,8 +2043,12 @@
       <c r="X6" s="12">
         <v>5</v>
       </c>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
+      <c r="Y6" s="12">
+        <v>5</v>
+      </c>
+      <c r="Z6" s="12">
+        <v>7</v>
+      </c>
       <c r="AA6" s="12"/>
       <c r="AB6" s="12"/>
       <c r="AC6" s="12"/>
@@ -2057,8 +2126,12 @@
       <c r="X7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
+      <c r="Y7" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z7" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
       <c r="AC7" s="12"/>
@@ -2136,8 +2209,12 @@
       <c r="X8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
+      <c r="Y8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z8" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AA8" s="12"/>
       <c r="AB8" s="12"/>
       <c r="AC8" s="12"/>
@@ -2215,8 +2292,12 @@
       <c r="X9" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="12"/>
+      <c r="Y9" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z9" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA9" s="12"/>
       <c r="AB9" s="12"/>
       <c r="AC9" s="12"/>
@@ -2294,8 +2375,12 @@
       <c r="X10" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y10" s="12"/>
-      <c r="Z10" s="12"/>
+      <c r="Y10" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z10" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA10" s="12"/>
       <c r="AB10" s="12"/>
       <c r="AC10" s="12"/>
@@ -2373,8 +2458,12 @@
       <c r="X11" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="12"/>
+      <c r="Y11" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z11" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
@@ -2452,8 +2541,12 @@
       <c r="X12" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y12" s="12"/>
-      <c r="Z12" s="12"/>
+      <c r="Y12" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z12" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
       <c r="AC12" s="12"/>
@@ -2531,8 +2624,12 @@
       <c r="X13" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
+      <c r="Y13" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z13" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA13" s="12"/>
       <c r="AB13" s="12"/>
       <c r="AC13" s="12"/>
@@ -2610,8 +2707,12 @@
       <c r="X14" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y14" s="12"/>
-      <c r="Z14" s="12"/>
+      <c r="Y14" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z14" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA14" s="12"/>
       <c r="AB14" s="12"/>
       <c r="AC14" s="12"/>
@@ -2689,8 +2790,12 @@
       <c r="X15" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y15" s="12"/>
-      <c r="Z15" s="12"/>
+      <c r="Y15" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z15" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
       <c r="AC15" s="12"/>
@@ -2768,8 +2873,12 @@
       <c r="X16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
+      <c r="Y16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z16" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
@@ -2847,8 +2956,12 @@
       <c r="X17" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
+      <c r="Y17" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z17" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
@@ -2926,8 +3039,12 @@
       <c r="X18" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y18" s="12"/>
-      <c r="Z18" s="12"/>
+      <c r="Y18" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z18" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
       <c r="AC18" s="12"/>
@@ -3005,8 +3122,12 @@
       <c r="X19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
+      <c r="Y19" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z19" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA19" s="12"/>
       <c r="AB19" s="12"/>
       <c r="AC19" s="12"/>
@@ -3084,8 +3205,12 @@
       <c r="X20" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y20" s="12"/>
-      <c r="Z20" s="12"/>
+      <c r="Y20" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z20" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA20" s="12"/>
       <c r="AB20" s="12"/>
       <c r="AC20" s="12"/>
@@ -3163,8 +3288,12 @@
       <c r="X21" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="12"/>
+      <c r="Y21" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z21" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA21" s="12"/>
       <c r="AB21" s="12"/>
       <c r="AC21" s="12"/>
@@ -3242,8 +3371,12 @@
       <c r="X22" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
+      <c r="Y22" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z22" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
@@ -3321,8 +3454,12 @@
       <c r="X23" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
+      <c r="Y23" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z23" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA23" s="12"/>
       <c r="AB23" s="12"/>
       <c r="AC23" s="12"/>
@@ -3400,8 +3537,12 @@
       <c r="X24" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y24" s="12"/>
-      <c r="Z24" s="12"/>
+      <c r="Y24" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z24" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA24" s="12"/>
       <c r="AB24" s="12"/>
       <c r="AC24" s="12"/>
@@ -3479,8 +3620,12 @@
       <c r="X25" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y25" s="12"/>
-      <c r="Z25" s="12"/>
+      <c r="Y25" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z25" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA25" s="12"/>
       <c r="AB25" s="12"/>
       <c r="AC25" s="12"/>
@@ -3558,8 +3703,12 @@
       <c r="X26" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y26" s="12"/>
-      <c r="Z26" s="12"/>
+      <c r="Y26" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z26" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
       <c r="AC26" s="12"/>
@@ -3637,8 +3786,12 @@
       <c r="X27" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y27" s="12"/>
-      <c r="Z27" s="12"/>
+      <c r="Y27" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z27" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA27" s="12"/>
       <c r="AB27" s="12"/>
       <c r="AC27" s="12"/>
@@ -3716,8 +3869,12 @@
       <c r="X28" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y28" s="12"/>
-      <c r="Z28" s="12"/>
+      <c r="Y28" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z28" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA28" s="12"/>
       <c r="AB28" s="12"/>
       <c r="AC28" s="12"/>
@@ -3795,8 +3952,12 @@
       <c r="X29" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Y29" s="12"/>
-      <c r="Z29" s="12"/>
+      <c r="Y29" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z29" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA29" s="12"/>
       <c r="AB29" s="12"/>
       <c r="AC29" s="12"/>
@@ -3874,8 +4035,12 @@
       <c r="X30" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y30" s="12"/>
-      <c r="Z30" s="12"/>
+      <c r="Y30" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z30" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA30" s="12"/>
       <c r="AB30" s="12"/>
       <c r="AC30" s="12"/>
@@ -3953,8 +4118,12 @@
       <c r="X31" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Y31" s="12"/>
-      <c r="Z31" s="12"/>
+      <c r="Y31" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z31" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA31" s="12"/>
       <c r="AB31" s="12"/>
       <c r="AC31" s="12"/>
@@ -4032,8 +4201,12 @@
       <c r="X32" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y32" s="12"/>
-      <c r="Z32" s="12"/>
+      <c r="Y32" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z32" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA32" s="12"/>
       <c r="AB32" s="12"/>
       <c r="AC32" s="12"/>
@@ -4111,8 +4284,12 @@
       <c r="X33" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y33" s="12"/>
-      <c r="Z33" s="12"/>
+      <c r="Y33" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z33" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA33" s="12"/>
       <c r="AB33" s="12"/>
       <c r="AC33" s="12"/>
@@ -4190,8 +4367,12 @@
       <c r="X34" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y34" s="12"/>
-      <c r="Z34" s="12"/>
+      <c r="Y34" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z34" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA34" s="12"/>
       <c r="AB34" s="12"/>
       <c r="AC34" s="12"/>
@@ -4269,8 +4450,12 @@
       <c r="X35" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y35" s="12"/>
-      <c r="Z35" s="12"/>
+      <c r="Y35" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z35" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA35" s="12"/>
       <c r="AB35" s="12"/>
       <c r="AC35" s="12"/>
@@ -4348,8 +4533,12 @@
       <c r="X36" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="Y36" s="12"/>
-      <c r="Z36" s="12"/>
+      <c r="Y36" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z36" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA36" s="12"/>
       <c r="AB36" s="12"/>
       <c r="AC36" s="12"/>
@@ -4427,8 +4616,12 @@
       <c r="X37" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y37" s="12"/>
-      <c r="Z37" s="12"/>
+      <c r="Y37" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z37" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA37" s="12"/>
       <c r="AB37" s="12"/>
       <c r="AC37" s="12"/>
@@ -4506,8 +4699,12 @@
       <c r="X38" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y38" s="12"/>
-      <c r="Z38" s="12"/>
+      <c r="Y38" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z38" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA38" s="12"/>
       <c r="AB38" s="12"/>
       <c r="AC38" s="12"/>
@@ -4585,8 +4782,12 @@
       <c r="X39" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y39" s="12"/>
-      <c r="Z39" s="12"/>
+      <c r="Y39" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z39" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA39" s="12"/>
       <c r="AB39" s="12"/>
       <c r="AC39" s="12"/>
@@ -4664,8 +4865,12 @@
       <c r="X40" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y40" s="12"/>
-      <c r="Z40" s="12"/>
+      <c r="Y40" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z40" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA40" s="12"/>
       <c r="AB40" s="12"/>
       <c r="AC40" s="12"/>
@@ -4743,8 +4948,12 @@
       <c r="X41" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y41" s="12"/>
-      <c r="Z41" s="12"/>
+      <c r="Y41" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z41" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA41" s="12"/>
       <c r="AB41" s="12"/>
       <c r="AC41" s="12"/>
@@ -4822,8 +5031,12 @@
       <c r="X42" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y42" s="12"/>
-      <c r="Z42" s="12"/>
+      <c r="Y42" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z42" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA42" s="12"/>
       <c r="AB42" s="12"/>
       <c r="AC42" s="12"/>
@@ -4901,8 +5114,12 @@
       <c r="X43" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y43" s="12"/>
-      <c r="Z43" s="12"/>
+      <c r="Y43" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z43" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA43" s="12"/>
       <c r="AB43" s="12"/>
       <c r="AC43" s="12"/>
@@ -4980,8 +5197,12 @@
       <c r="X44" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y44" s="12"/>
-      <c r="Z44" s="12"/>
+      <c r="Y44" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z44" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA44" s="12"/>
       <c r="AB44" s="12"/>
       <c r="AC44" s="12"/>
@@ -5059,8 +5280,12 @@
       <c r="X45" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y45" s="12"/>
-      <c r="Z45" s="12"/>
+      <c r="Y45" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z45" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA45" s="12"/>
       <c r="AB45" s="12"/>
       <c r="AC45" s="12"/>
@@ -5138,8 +5363,12 @@
       <c r="X46" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y46" s="12"/>
-      <c r="Z46" s="12"/>
+      <c r="Y46" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z46" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA46" s="12"/>
       <c r="AB46" s="12"/>
       <c r="AC46" s="12"/>
@@ -5217,8 +5446,12 @@
       <c r="X47" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y47" s="12"/>
-      <c r="Z47" s="12"/>
+      <c r="Y47" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z47" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA47" s="12"/>
       <c r="AB47" s="12"/>
       <c r="AC47" s="12"/>
@@ -5296,8 +5529,12 @@
       <c r="X48" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y48" s="12"/>
-      <c r="Z48" s="12"/>
+      <c r="Y48" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z48" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA48" s="12"/>
       <c r="AB48" s="12"/>
       <c r="AC48" s="12"/>
@@ -5375,8 +5612,12 @@
       <c r="X49" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y49" s="12"/>
-      <c r="Z49" s="12"/>
+      <c r="Y49" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z49" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AA49" s="12"/>
       <c r="AB49" s="12"/>
       <c r="AC49" s="12"/>
@@ -5454,8 +5695,12 @@
       <c r="X50" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y50" s="12"/>
-      <c r="Z50" s="12"/>
+      <c r="Y50" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z50" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA50" s="12"/>
       <c r="AB50" s="12"/>
       <c r="AC50" s="12"/>
@@ -5533,8 +5778,12 @@
       <c r="X51" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y51" s="12"/>
-      <c r="Z51" s="12"/>
+      <c r="Y51" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z51" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA51" s="12"/>
       <c r="AB51" s="12"/>
       <c r="AC51" s="12"/>
@@ -5612,8 +5861,12 @@
       <c r="X52" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y52" s="12"/>
-      <c r="Z52" s="12"/>
+      <c r="Y52" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z52" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA52" s="12"/>
       <c r="AB52" s="12"/>
       <c r="AC52" s="12"/>
@@ -5691,8 +5944,12 @@
       <c r="X53" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y53" s="12"/>
-      <c r="Z53" s="12"/>
+      <c r="Y53" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z53" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA53" s="12"/>
       <c r="AB53" s="12"/>
       <c r="AC53" s="12"/>
@@ -5770,8 +6027,12 @@
       <c r="X54" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="Y54" s="12"/>
-      <c r="Z54" s="12"/>
+      <c r="Y54" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z54" s="40" t="s">
+        <v>54</v>
+      </c>
       <c r="AA54" s="12"/>
       <c r="AB54" s="12"/>
       <c r="AC54" s="12"/>
@@ -5779,10 +6040,10 @@
       <c r="AE54" s="12"/>
     </row>
     <row r="55" spans="1:31">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B55" s="46"/>
+      <c r="B55" s="48"/>
       <c r="C55" s="13"/>
       <c r="D55" s="12">
         <f>COUNTIF(D7:D54,"A")</f>
@@ -5870,11 +6131,11 @@
       </c>
       <c r="Y55" s="12">
         <f t="shared" ref="Y55" si="15">COUNTIF(Y7:Y54,"A")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z55" s="12">
         <f t="shared" ref="Z55" si="16">COUNTIF(Z7:Z54,"A")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA55" s="12">
         <f t="shared" ref="AA55" si="17">COUNTIF(AA7:AA54,"A")</f>
@@ -5898,10 +6159,10 @@
       </c>
     </row>
     <row r="56" spans="1:31">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="40"/>
+      <c r="B56" s="42"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f>(48-D55)</f>
@@ -5989,11 +6250,11 @@
       </c>
       <c r="Y56" s="24">
         <f t="shared" si="22"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="Z56" s="24">
         <f t="shared" si="22"/>
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AA56" s="24">
         <f t="shared" si="22"/>
@@ -6053,88 +6314,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:32" ht="19.5">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
       <c r="D2" s="19" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:32" ht="18.75">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:32" ht="18.75">
       <c r="A4" s="33"/>
       <c r="B4" s="34"/>
       <c r="C4" s="33"/>
-      <c r="D4" s="57" t="s">
+      <c r="D4" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="53" t="s">
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="55" t="s">
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="55"/>
-      <c r="N4" s="53" t="s">
+      <c r="M4" s="57"/>
+      <c r="N4" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56"/>
+      <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="1:32">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="50" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -6199,8 +6460,8 @@
       <c r="AF5" s="19"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="47"/>
-      <c r="B6" s="49"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="51"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -6263,8 +6524,8 @@
       <c r="AF6" s="19"/>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1">
-      <c r="A7" s="47"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -9495,10 +9756,10 @@
       <c r="AF55" s="19"/>
     </row>
     <row r="56" spans="1:32">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="46"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="13"/>
       <c r="D56" s="19">
         <f>COUNTIF(D8:D55,"A")</f>
@@ -9618,10 +9879,10 @@
       </c>
     </row>
     <row r="57" spans="1:32">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="40"/>
+      <c r="B57" s="42"/>
       <c r="C57" s="13"/>
       <c r="D57" s="19">
         <f>(48-D56)</f>
@@ -9780,56 +10041,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="19.5">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
     </row>
     <row r="3" spans="1:7" ht="18.75">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="47"/>
-      <c r="B5" s="49"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="32" t="s">
         <v>62</v>
       </c>
@@ -9839,8 +10100,8 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1">
-      <c r="A6" s="47"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="35">
         <v>50</v>
       </c>
@@ -10570,10 +10831,10 @@
       <c r="G54" s="13"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="46"/>
+      <c r="B55" s="48"/>
       <c r="C55" s="32">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>32</v>
@@ -10584,10 +10845,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="39" t="s">
+      <c r="A56" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="40"/>
+      <c r="B56" s="42"/>
       <c r="C56" s="32">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>15</v>
@@ -10598,10 +10859,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="39" t="s">
+      <c r="A57" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="40"/>
+      <c r="B57" s="42"/>
       <c r="C57" s="32">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>1</v>
@@ -10612,10 +10873,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="39" t="s">
+      <c r="A58" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="B58" s="40"/>
+      <c r="B58" s="42"/>
       <c r="C58" s="36">
         <f>(C55/48)*100</f>
         <v>66.666666666666657</v>

</xml_diff>